<commit_message>
Updated with completion of requirements chapter draft.
</commit_message>
<xml_diff>
--- a/project_management/E2E-Deliverables-Completion-Timeline.xlsx
+++ b/project_management/E2E-Deliverables-Completion-Timeline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="35260" windowHeight="22260" tabRatio="500"/>
+    <workbookView xWindow="39660" yWindow="460" windowWidth="35260" windowHeight="22260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Current Plan 2015-16" sheetId="3" r:id="rId1"/>
@@ -1679,24 +1679,6 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1827,6 +1809,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2505,7 +2505,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2594,40 +2594,40 @@
       <c r="A3" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="195" t="s">
+      <c r="C3" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="181" t="s">
+      <c r="D3" s="225" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="180" t="s">
+      <c r="E3" s="225"/>
+      <c r="F3" s="225"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="224" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="181"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="180" t="s">
+      <c r="I3" s="225"/>
+      <c r="J3" s="225"/>
+      <c r="K3" s="225"/>
+      <c r="L3" s="226"/>
+      <c r="M3" s="224" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="181"/>
-      <c r="O3" s="181"/>
-      <c r="P3" s="182"/>
-      <c r="Q3" s="180" t="s">
+      <c r="N3" s="225"/>
+      <c r="O3" s="225"/>
+      <c r="P3" s="226"/>
+      <c r="Q3" s="224" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="181"/>
-      <c r="S3" s="181"/>
-      <c r="T3" s="182"/>
-      <c r="U3" s="180" t="s">
+      <c r="R3" s="225"/>
+      <c r="S3" s="225"/>
+      <c r="T3" s="226"/>
+      <c r="U3" s="224" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="181"/>
-      <c r="W3" s="181"/>
-      <c r="X3" s="182"/>
+      <c r="V3" s="225"/>
+      <c r="W3" s="225"/>
+      <c r="X3" s="226"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51"/>
@@ -2779,27 +2779,27 @@
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="81"/>
-      <c r="D6" s="207"/>
-      <c r="E6" s="207"/>
-      <c r="F6" s="207"/>
-      <c r="G6" s="225"/>
-      <c r="H6" s="208"/>
-      <c r="I6" s="207"/>
-      <c r="J6" s="215"/>
-      <c r="K6" s="209"/>
-      <c r="L6" s="209"/>
-      <c r="M6" s="208"/>
-      <c r="N6" s="207"/>
-      <c r="O6" s="215"/>
-      <c r="P6" s="209"/>
-      <c r="Q6" s="208"/>
-      <c r="R6" s="207"/>
-      <c r="S6" s="215"/>
-      <c r="T6" s="209"/>
-      <c r="U6" s="208"/>
-      <c r="V6" s="207"/>
-      <c r="W6" s="215"/>
-      <c r="X6" s="209"/>
+      <c r="D6" s="201"/>
+      <c r="E6" s="201"/>
+      <c r="F6" s="201"/>
+      <c r="G6" s="219"/>
+      <c r="H6" s="202"/>
+      <c r="I6" s="201"/>
+      <c r="J6" s="209"/>
+      <c r="K6" s="203"/>
+      <c r="L6" s="203"/>
+      <c r="M6" s="202"/>
+      <c r="N6" s="201"/>
+      <c r="O6" s="209"/>
+      <c r="P6" s="203"/>
+      <c r="Q6" s="202"/>
+      <c r="R6" s="201"/>
+      <c r="S6" s="209"/>
+      <c r="T6" s="203"/>
+      <c r="U6" s="202"/>
+      <c r="V6" s="201"/>
+      <c r="W6" s="209"/>
+      <c r="X6" s="203"/>
     </row>
     <row r="7" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
@@ -2807,55 +2807,55 @@
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="82"/>
-      <c r="D7" s="216"/>
-      <c r="E7" s="216"/>
-      <c r="F7" s="216"/>
-      <c r="G7" s="226"/>
-      <c r="H7" s="204"/>
-      <c r="I7" s="196"/>
-      <c r="J7" s="196"/>
-      <c r="K7" s="217"/>
-      <c r="L7" s="217"/>
-      <c r="M7" s="204"/>
-      <c r="N7" s="196"/>
-      <c r="O7" s="196"/>
-      <c r="P7" s="217"/>
-      <c r="Q7" s="204"/>
-      <c r="R7" s="196"/>
-      <c r="S7" s="196"/>
-      <c r="T7" s="217"/>
-      <c r="U7" s="204"/>
-      <c r="V7" s="196"/>
-      <c r="W7" s="196"/>
-      <c r="X7" s="217"/>
+      <c r="D7" s="210"/>
+      <c r="E7" s="210"/>
+      <c r="F7" s="210"/>
+      <c r="G7" s="220"/>
+      <c r="H7" s="198"/>
+      <c r="I7" s="190"/>
+      <c r="J7" s="190"/>
+      <c r="K7" s="211"/>
+      <c r="L7" s="211"/>
+      <c r="M7" s="198"/>
+      <c r="N7" s="190"/>
+      <c r="O7" s="190"/>
+      <c r="P7" s="211"/>
+      <c r="Q7" s="198"/>
+      <c r="R7" s="190"/>
+      <c r="S7" s="190"/>
+      <c r="T7" s="211"/>
+      <c r="U7" s="198"/>
+      <c r="V7" s="190"/>
+      <c r="W7" s="190"/>
+      <c r="X7" s="211"/>
     </row>
     <row r="8" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="39"/>
       <c r="B8" s="46"/>
       <c r="C8" s="87"/>
-      <c r="D8" s="219"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="229">
+      <c r="D8" s="213"/>
+      <c r="E8" s="213"/>
+      <c r="F8" s="223">
         <v>1</v>
       </c>
-      <c r="G8" s="227"/>
-      <c r="H8" s="198"/>
-      <c r="I8" s="218"/>
-      <c r="J8" s="219"/>
-      <c r="K8" s="220"/>
-      <c r="L8" s="220"/>
-      <c r="M8" s="198"/>
-      <c r="N8" s="218"/>
-      <c r="O8" s="219"/>
-      <c r="P8" s="220"/>
-      <c r="Q8" s="198"/>
-      <c r="R8" s="218"/>
-      <c r="S8" s="219"/>
-      <c r="T8" s="220"/>
-      <c r="U8" s="198"/>
-      <c r="V8" s="218"/>
-      <c r="W8" s="219"/>
-      <c r="X8" s="220"/>
+      <c r="G8" s="221"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="212"/>
+      <c r="J8" s="213"/>
+      <c r="K8" s="214"/>
+      <c r="L8" s="214"/>
+      <c r="M8" s="192"/>
+      <c r="N8" s="212"/>
+      <c r="O8" s="213"/>
+      <c r="P8" s="214"/>
+      <c r="Q8" s="192"/>
+      <c r="R8" s="212"/>
+      <c r="S8" s="213"/>
+      <c r="T8" s="214"/>
+      <c r="U8" s="192"/>
+      <c r="V8" s="212"/>
+      <c r="W8" s="213"/>
+      <c r="X8" s="214"/>
     </row>
     <row r="9" spans="1:28" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
@@ -2863,27 +2863,27 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="81"/>
-      <c r="D9" s="207"/>
-      <c r="E9" s="207"/>
-      <c r="F9" s="207"/>
-      <c r="G9" s="225"/>
-      <c r="H9" s="208"/>
-      <c r="I9" s="207"/>
-      <c r="J9" s="215"/>
-      <c r="K9" s="209"/>
-      <c r="L9" s="209"/>
-      <c r="M9" s="208"/>
-      <c r="N9" s="207"/>
-      <c r="O9" s="215"/>
-      <c r="P9" s="209"/>
-      <c r="Q9" s="208"/>
-      <c r="R9" s="207"/>
-      <c r="S9" s="215"/>
-      <c r="T9" s="209"/>
-      <c r="U9" s="208"/>
-      <c r="V9" s="207"/>
-      <c r="W9" s="215"/>
-      <c r="X9" s="209"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="219"/>
+      <c r="H9" s="202"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="209"/>
+      <c r="K9" s="203"/>
+      <c r="L9" s="203"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="201"/>
+      <c r="O9" s="209"/>
+      <c r="P9" s="203"/>
+      <c r="Q9" s="202"/>
+      <c r="R9" s="201"/>
+      <c r="S9" s="209"/>
+      <c r="T9" s="203"/>
+      <c r="U9" s="202"/>
+      <c r="V9" s="201"/>
+      <c r="W9" s="209"/>
+      <c r="X9" s="203"/>
     </row>
     <row r="10" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
@@ -2891,177 +2891,179 @@
       </c>
       <c r="B10" s="178"/>
       <c r="C10" s="82"/>
-      <c r="D10" s="223"/>
-      <c r="E10" s="222"/>
-      <c r="F10" s="222"/>
-      <c r="G10" s="228"/>
-      <c r="H10" s="221"/>
-      <c r="I10" s="222"/>
-      <c r="J10" s="223"/>
-      <c r="K10" s="217"/>
-      <c r="L10" s="217"/>
-      <c r="M10" s="224"/>
-      <c r="N10" s="223"/>
-      <c r="O10" s="223"/>
-      <c r="P10" s="217"/>
-      <c r="Q10" s="224"/>
-      <c r="R10" s="223"/>
-      <c r="S10" s="223"/>
-      <c r="T10" s="217"/>
-      <c r="U10" s="224"/>
-      <c r="V10" s="223"/>
-      <c r="W10" s="223"/>
-      <c r="X10" s="217"/>
+      <c r="D10" s="217"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="222"/>
+      <c r="H10" s="215"/>
+      <c r="I10" s="216"/>
+      <c r="J10" s="217"/>
+      <c r="K10" s="211"/>
+      <c r="L10" s="211"/>
+      <c r="M10" s="218"/>
+      <c r="N10" s="217"/>
+      <c r="O10" s="217"/>
+      <c r="P10" s="211"/>
+      <c r="Q10" s="218"/>
+      <c r="R10" s="217"/>
+      <c r="S10" s="217"/>
+      <c r="T10" s="211"/>
+      <c r="U10" s="218"/>
+      <c r="V10" s="217"/>
+      <c r="W10" s="217"/>
+      <c r="X10" s="211"/>
     </row>
     <row r="11" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="39"/>
       <c r="B11" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="186" t="s">
+      <c r="C11" s="180" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="196"/>
-      <c r="E11" s="196"/>
-      <c r="F11" s="196"/>
-      <c r="G11" s="197">
+      <c r="D11" s="190"/>
+      <c r="E11" s="190"/>
+      <c r="F11" s="190"/>
+      <c r="G11" s="191">
         <v>0.3</v>
       </c>
-      <c r="H11" s="198"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="196"/>
-      <c r="K11" s="200"/>
-      <c r="L11" s="200"/>
-      <c r="M11" s="198"/>
-      <c r="N11" s="199"/>
-      <c r="O11" s="196"/>
-      <c r="P11" s="200"/>
-      <c r="Q11" s="198"/>
-      <c r="R11" s="199"/>
-      <c r="S11" s="196"/>
-      <c r="T11" s="200"/>
-      <c r="U11" s="198"/>
-      <c r="V11" s="199"/>
-      <c r="W11" s="196"/>
-      <c r="X11" s="200"/>
+      <c r="H11" s="192"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="190"/>
+      <c r="K11" s="194"/>
+      <c r="L11" s="194"/>
+      <c r="M11" s="192"/>
+      <c r="N11" s="193"/>
+      <c r="O11" s="190"/>
+      <c r="P11" s="194"/>
+      <c r="Q11" s="192"/>
+      <c r="R11" s="193"/>
+      <c r="S11" s="190"/>
+      <c r="T11" s="194"/>
+      <c r="U11" s="192"/>
+      <c r="V11" s="193"/>
+      <c r="W11" s="190"/>
+      <c r="X11" s="194"/>
     </row>
     <row r="12" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="39"/>
       <c r="B12" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="186" t="s">
+      <c r="C12" s="180" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="196"/>
-      <c r="E12" s="196"/>
-      <c r="F12" s="196"/>
-      <c r="G12" s="197">
+      <c r="D12" s="190"/>
+      <c r="E12" s="190"/>
+      <c r="F12" s="190"/>
+      <c r="G12" s="191">
         <v>0.25</v>
       </c>
-      <c r="H12" s="196"/>
-      <c r="I12" s="199"/>
-      <c r="J12" s="196"/>
-      <c r="K12" s="196"/>
-      <c r="L12" s="196"/>
-      <c r="M12" s="196"/>
-      <c r="N12" s="199"/>
-      <c r="O12" s="196"/>
-      <c r="P12" s="196"/>
-      <c r="Q12" s="196"/>
-      <c r="R12" s="199"/>
-      <c r="S12" s="196"/>
-      <c r="T12" s="196"/>
-      <c r="U12" s="196"/>
-      <c r="V12" s="199"/>
-      <c r="W12" s="196"/>
-      <c r="X12" s="196"/>
+      <c r="H12" s="190"/>
+      <c r="I12" s="193"/>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
+      <c r="M12" s="190"/>
+      <c r="N12" s="193"/>
+      <c r="O12" s="190"/>
+      <c r="P12" s="190"/>
+      <c r="Q12" s="190"/>
+      <c r="R12" s="193"/>
+      <c r="S12" s="190"/>
+      <c r="T12" s="190"/>
+      <c r="U12" s="190"/>
+      <c r="V12" s="193"/>
+      <c r="W12" s="190"/>
+      <c r="X12" s="190"/>
     </row>
     <row r="13" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="39"/>
       <c r="B13" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="186" t="s">
+      <c r="C13" s="180" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="196"/>
-      <c r="E13" s="196"/>
-      <c r="F13" s="196"/>
-      <c r="G13" s="197">
+      <c r="D13" s="190"/>
+      <c r="E13" s="190"/>
+      <c r="F13" s="190"/>
+      <c r="G13" s="191">
         <v>0.6</v>
       </c>
-      <c r="H13" s="196"/>
-      <c r="I13" s="199"/>
-      <c r="J13" s="196"/>
-      <c r="K13" s="196"/>
-      <c r="L13" s="196"/>
-      <c r="M13" s="196"/>
-      <c r="N13" s="199"/>
-      <c r="O13" s="196"/>
-      <c r="P13" s="196"/>
-      <c r="Q13" s="196"/>
-      <c r="R13" s="199"/>
-      <c r="S13" s="196"/>
-      <c r="T13" s="196"/>
-      <c r="U13" s="196"/>
-      <c r="V13" s="199"/>
-      <c r="W13" s="196"/>
-      <c r="X13" s="196"/>
+      <c r="H13" s="191">
+        <v>1</v>
+      </c>
+      <c r="I13" s="193"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
+      <c r="M13" s="190"/>
+      <c r="N13" s="193"/>
+      <c r="O13" s="190"/>
+      <c r="P13" s="190"/>
+      <c r="Q13" s="190"/>
+      <c r="R13" s="193"/>
+      <c r="S13" s="190"/>
+      <c r="T13" s="190"/>
+      <c r="U13" s="190"/>
+      <c r="V13" s="193"/>
+      <c r="W13" s="190"/>
+      <c r="X13" s="190"/>
     </row>
     <row r="14" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="39"/>
       <c r="B14" s="46"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="196"/>
-      <c r="E14" s="196"/>
-      <c r="F14" s="196"/>
-      <c r="G14" s="196"/>
-      <c r="H14" s="196"/>
-      <c r="I14" s="199"/>
-      <c r="J14" s="196"/>
-      <c r="K14" s="196"/>
-      <c r="L14" s="196"/>
-      <c r="M14" s="196"/>
-      <c r="N14" s="199"/>
-      <c r="O14" s="196"/>
-      <c r="P14" s="196"/>
-      <c r="Q14" s="196"/>
-      <c r="R14" s="199"/>
-      <c r="S14" s="196"/>
-      <c r="T14" s="196"/>
-      <c r="U14" s="196"/>
-      <c r="V14" s="199"/>
-      <c r="W14" s="196"/>
-      <c r="X14" s="196"/>
+      <c r="C14" s="180"/>
+      <c r="D14" s="190"/>
+      <c r="E14" s="190"/>
+      <c r="F14" s="190"/>
+      <c r="G14" s="190"/>
+      <c r="H14" s="190"/>
+      <c r="I14" s="193"/>
+      <c r="J14" s="190"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="N14" s="193"/>
+      <c r="O14" s="190"/>
+      <c r="P14" s="190"/>
+      <c r="Q14" s="190"/>
+      <c r="R14" s="193"/>
+      <c r="S14" s="190"/>
+      <c r="T14" s="190"/>
+      <c r="U14" s="190"/>
+      <c r="V14" s="193"/>
+      <c r="W14" s="190"/>
+      <c r="X14" s="190"/>
     </row>
     <row r="15" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="169" t="s">
         <v>80</v>
       </c>
       <c r="B15" s="170"/>
-      <c r="C15" s="187"/>
-      <c r="D15" s="201"/>
-      <c r="E15" s="201"/>
-      <c r="F15" s="201"/>
-      <c r="G15" s="201"/>
-      <c r="H15" s="201"/>
-      <c r="I15" s="201"/>
-      <c r="J15" s="201"/>
-      <c r="K15" s="201"/>
-      <c r="L15" s="201"/>
-      <c r="M15" s="201"/>
-      <c r="N15" s="201"/>
-      <c r="O15" s="201"/>
-      <c r="P15" s="201"/>
-      <c r="Q15" s="201"/>
-      <c r="R15" s="201"/>
-      <c r="S15" s="201"/>
-      <c r="T15" s="201"/>
-      <c r="U15" s="201"/>
-      <c r="V15" s="201"/>
-      <c r="W15" s="201"/>
-      <c r="X15" s="201"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="195"/>
+      <c r="E15" s="195"/>
+      <c r="F15" s="195"/>
+      <c r="G15" s="195"/>
+      <c r="H15" s="195"/>
+      <c r="I15" s="195"/>
+      <c r="J15" s="195"/>
+      <c r="K15" s="195"/>
+      <c r="L15" s="195"/>
+      <c r="M15" s="195"/>
+      <c r="N15" s="195"/>
+      <c r="O15" s="195"/>
+      <c r="P15" s="195"/>
+      <c r="Q15" s="195"/>
+      <c r="R15" s="195"/>
+      <c r="S15" s="195"/>
+      <c r="T15" s="195"/>
+      <c r="U15" s="195"/>
+      <c r="V15" s="195"/>
+      <c r="W15" s="195"/>
+      <c r="X15" s="195"/>
       <c r="Y15" s="171"/>
       <c r="Z15" s="171"/>
       <c r="AA15" s="171"/>
@@ -3072,365 +3074,365 @@
         <v>53</v>
       </c>
       <c r="B16" s="178"/>
-      <c r="C16" s="186"/>
-      <c r="D16" s="196"/>
-      <c r="E16" s="196"/>
-      <c r="F16" s="196"/>
-      <c r="G16" s="202"/>
-      <c r="H16" s="202"/>
-      <c r="I16" s="202"/>
-      <c r="J16" s="202"/>
-      <c r="K16" s="202"/>
-      <c r="L16" s="196"/>
-      <c r="M16" s="196"/>
-      <c r="N16" s="196"/>
-      <c r="O16" s="196"/>
-      <c r="P16" s="196"/>
-      <c r="Q16" s="196"/>
-      <c r="R16" s="196"/>
-      <c r="S16" s="196"/>
-      <c r="T16" s="196"/>
-      <c r="U16" s="196"/>
-      <c r="V16" s="196"/>
-      <c r="W16" s="196"/>
-      <c r="X16" s="196"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="190"/>
+      <c r="E16" s="190"/>
+      <c r="F16" s="190"/>
+      <c r="G16" s="196"/>
+      <c r="H16" s="196"/>
+      <c r="I16" s="196"/>
+      <c r="J16" s="196"/>
+      <c r="K16" s="196"/>
+      <c r="L16" s="190"/>
+      <c r="M16" s="190"/>
+      <c r="N16" s="190"/>
+      <c r="O16" s="190"/>
+      <c r="P16" s="190"/>
+      <c r="Q16" s="190"/>
+      <c r="R16" s="190"/>
+      <c r="S16" s="190"/>
+      <c r="T16" s="190"/>
+      <c r="U16" s="190"/>
+      <c r="V16" s="190"/>
+      <c r="W16" s="190"/>
+      <c r="X16" s="190"/>
     </row>
     <row r="17" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="39"/>
       <c r="B17" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="186" t="s">
+      <c r="C17" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="196"/>
-      <c r="E17" s="196"/>
-      <c r="F17" s="196"/>
-      <c r="G17" s="197">
+      <c r="D17" s="190"/>
+      <c r="E17" s="190"/>
+      <c r="F17" s="190"/>
+      <c r="G17" s="191">
         <v>0.15</v>
       </c>
-      <c r="H17" s="196"/>
-      <c r="I17" s="199"/>
-      <c r="J17" s="196"/>
-      <c r="K17" s="196"/>
-      <c r="L17" s="196"/>
-      <c r="M17" s="196"/>
-      <c r="N17" s="199"/>
-      <c r="O17" s="196"/>
-      <c r="P17" s="196"/>
-      <c r="Q17" s="196"/>
-      <c r="R17" s="199"/>
-      <c r="S17" s="196"/>
-      <c r="T17" s="196"/>
-      <c r="U17" s="196"/>
-      <c r="V17" s="199"/>
-      <c r="W17" s="196"/>
-      <c r="X17" s="196"/>
+      <c r="H17" s="190"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="190"/>
+      <c r="K17" s="190"/>
+      <c r="L17" s="190"/>
+      <c r="M17" s="190"/>
+      <c r="N17" s="193"/>
+      <c r="O17" s="190"/>
+      <c r="P17" s="190"/>
+      <c r="Q17" s="190"/>
+      <c r="R17" s="193"/>
+      <c r="S17" s="190"/>
+      <c r="T17" s="190"/>
+      <c r="U17" s="190"/>
+      <c r="V17" s="193"/>
+      <c r="W17" s="190"/>
+      <c r="X17" s="190"/>
     </row>
     <row r="18" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="39"/>
       <c r="B18" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="186" t="s">
+      <c r="C18" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="196"/>
-      <c r="E18" s="196"/>
-      <c r="F18" s="196"/>
-      <c r="G18" s="197">
+      <c r="D18" s="190"/>
+      <c r="E18" s="190"/>
+      <c r="F18" s="190"/>
+      <c r="G18" s="191">
         <v>0.15</v>
       </c>
-      <c r="H18" s="196"/>
-      <c r="I18" s="199"/>
-      <c r="J18" s="196"/>
-      <c r="K18" s="196"/>
-      <c r="L18" s="196"/>
-      <c r="M18" s="196"/>
-      <c r="N18" s="199"/>
-      <c r="O18" s="196"/>
-      <c r="P18" s="196"/>
-      <c r="Q18" s="196"/>
-      <c r="R18" s="199"/>
-      <c r="S18" s="196"/>
-      <c r="T18" s="196"/>
-      <c r="U18" s="196"/>
-      <c r="V18" s="199"/>
-      <c r="W18" s="196"/>
-      <c r="X18" s="196"/>
+      <c r="H18" s="190"/>
+      <c r="I18" s="193"/>
+      <c r="J18" s="190"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="190"/>
+      <c r="M18" s="190"/>
+      <c r="N18" s="193"/>
+      <c r="O18" s="190"/>
+      <c r="P18" s="190"/>
+      <c r="Q18" s="190"/>
+      <c r="R18" s="193"/>
+      <c r="S18" s="190"/>
+      <c r="T18" s="190"/>
+      <c r="U18" s="190"/>
+      <c r="V18" s="193"/>
+      <c r="W18" s="190"/>
+      <c r="X18" s="190"/>
     </row>
     <row r="19" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="188" t="s">
+      <c r="C19" s="182" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="203"/>
-      <c r="E19" s="203"/>
-      <c r="F19" s="203"/>
-      <c r="G19" s="199">
+      <c r="D19" s="197"/>
+      <c r="E19" s="197"/>
+      <c r="F19" s="197"/>
+      <c r="G19" s="193">
         <v>0.15</v>
       </c>
-      <c r="H19" s="203"/>
-      <c r="I19" s="199"/>
-      <c r="J19" s="199"/>
-      <c r="K19" s="203"/>
-      <c r="L19" s="203"/>
-      <c r="M19" s="203"/>
-      <c r="N19" s="199"/>
-      <c r="O19" s="199"/>
-      <c r="P19" s="203"/>
-      <c r="Q19" s="203"/>
-      <c r="R19" s="199"/>
-      <c r="S19" s="199"/>
-      <c r="T19" s="203"/>
-      <c r="U19" s="203"/>
-      <c r="V19" s="199"/>
-      <c r="W19" s="199"/>
-      <c r="X19" s="203"/>
+      <c r="H19" s="197"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
+      <c r="K19" s="197"/>
+      <c r="L19" s="197"/>
+      <c r="M19" s="197"/>
+      <c r="N19" s="193"/>
+      <c r="O19" s="193"/>
+      <c r="P19" s="197"/>
+      <c r="Q19" s="197"/>
+      <c r="R19" s="193"/>
+      <c r="S19" s="193"/>
+      <c r="T19" s="197"/>
+      <c r="U19" s="197"/>
+      <c r="V19" s="193"/>
+      <c r="W19" s="193"/>
+      <c r="X19" s="197"/>
     </row>
     <row r="20" spans="1:27" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="188" t="s">
+      <c r="C20" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="203"/>
-      <c r="E20" s="203"/>
-      <c r="F20" s="203"/>
-      <c r="G20" s="205">
+      <c r="D20" s="197"/>
+      <c r="E20" s="197"/>
+      <c r="F20" s="197"/>
+      <c r="G20" s="199">
         <v>0.2</v>
       </c>
-      <c r="H20" s="203"/>
-      <c r="I20" s="199"/>
-      <c r="J20" s="203"/>
-      <c r="K20" s="203"/>
-      <c r="L20" s="203"/>
-      <c r="M20" s="203"/>
-      <c r="N20" s="199"/>
-      <c r="O20" s="203"/>
-      <c r="P20" s="203"/>
-      <c r="Q20" s="203"/>
-      <c r="R20" s="199"/>
-      <c r="S20" s="203"/>
-      <c r="T20" s="203"/>
-      <c r="U20" s="203"/>
-      <c r="V20" s="199"/>
-      <c r="W20" s="203"/>
-      <c r="X20" s="203"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="197"/>
+      <c r="K20" s="197"/>
+      <c r="L20" s="197"/>
+      <c r="M20" s="197"/>
+      <c r="N20" s="193"/>
+      <c r="O20" s="197"/>
+      <c r="P20" s="197"/>
+      <c r="Q20" s="197"/>
+      <c r="R20" s="193"/>
+      <c r="S20" s="197"/>
+      <c r="T20" s="197"/>
+      <c r="U20" s="197"/>
+      <c r="V20" s="193"/>
+      <c r="W20" s="197"/>
+      <c r="X20" s="197"/>
     </row>
     <row r="21" spans="1:27" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="172"/>
-      <c r="C21" s="188"/>
-      <c r="D21" s="203"/>
-      <c r="E21" s="203"/>
-      <c r="F21" s="203"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="203"/>
-      <c r="I21" s="199"/>
-      <c r="J21" s="203"/>
-      <c r="K21" s="203"/>
-      <c r="L21" s="203"/>
-      <c r="M21" s="203"/>
-      <c r="N21" s="199"/>
-      <c r="O21" s="203"/>
-      <c r="P21" s="203"/>
-      <c r="Q21" s="203"/>
-      <c r="R21" s="199"/>
-      <c r="S21" s="203"/>
-      <c r="T21" s="203"/>
-      <c r="U21" s="203"/>
-      <c r="V21" s="199"/>
-      <c r="W21" s="203"/>
-      <c r="X21" s="203"/>
+      <c r="C21" s="182"/>
+      <c r="D21" s="197"/>
+      <c r="E21" s="197"/>
+      <c r="F21" s="197"/>
+      <c r="G21" s="200"/>
+      <c r="H21" s="197"/>
+      <c r="I21" s="193"/>
+      <c r="J21" s="197"/>
+      <c r="K21" s="197"/>
+      <c r="L21" s="197"/>
+      <c r="M21" s="197"/>
+      <c r="N21" s="193"/>
+      <c r="O21" s="197"/>
+      <c r="P21" s="197"/>
+      <c r="Q21" s="197"/>
+      <c r="R21" s="193"/>
+      <c r="S21" s="197"/>
+      <c r="T21" s="197"/>
+      <c r="U21" s="197"/>
+      <c r="V21" s="193"/>
+      <c r="W21" s="197"/>
+      <c r="X21" s="197"/>
     </row>
     <row r="22" spans="1:27" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="18"/>
-      <c r="C22" s="189"/>
-      <c r="D22" s="207"/>
-      <c r="E22" s="207"/>
-      <c r="F22" s="207"/>
-      <c r="G22" s="207"/>
-      <c r="H22" s="207"/>
-      <c r="I22" s="207"/>
-      <c r="J22" s="207"/>
-      <c r="K22" s="207"/>
-      <c r="L22" s="207"/>
-      <c r="M22" s="207"/>
-      <c r="N22" s="207"/>
-      <c r="O22" s="207"/>
-      <c r="P22" s="207"/>
-      <c r="Q22" s="207"/>
-      <c r="R22" s="207"/>
-      <c r="S22" s="207"/>
-      <c r="T22" s="207"/>
-      <c r="U22" s="207"/>
-      <c r="V22" s="207"/>
-      <c r="W22" s="207"/>
-      <c r="X22" s="207"/>
+      <c r="C22" s="183"/>
+      <c r="D22" s="201"/>
+      <c r="E22" s="201"/>
+      <c r="F22" s="201"/>
+      <c r="G22" s="201"/>
+      <c r="H22" s="201"/>
+      <c r="I22" s="201"/>
+      <c r="J22" s="201"/>
+      <c r="K22" s="201"/>
+      <c r="L22" s="201"/>
+      <c r="M22" s="201"/>
+      <c r="N22" s="201"/>
+      <c r="O22" s="201"/>
+      <c r="P22" s="201"/>
+      <c r="Q22" s="201"/>
+      <c r="R22" s="201"/>
+      <c r="S22" s="201"/>
+      <c r="T22" s="201"/>
+      <c r="U22" s="201"/>
+      <c r="V22" s="201"/>
+      <c r="W22" s="201"/>
+      <c r="X22" s="201"/>
     </row>
     <row r="23" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="57" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="40"/>
-      <c r="C23" s="190"/>
-      <c r="D23" s="196"/>
-      <c r="E23" s="196"/>
-      <c r="F23" s="196"/>
-      <c r="G23" s="196"/>
-      <c r="H23" s="203"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="202"/>
-      <c r="K23" s="202"/>
-      <c r="L23" s="202"/>
-      <c r="M23" s="202"/>
-      <c r="N23" s="202"/>
-      <c r="O23" s="210"/>
-      <c r="P23" s="210"/>
-      <c r="Q23" s="210"/>
-      <c r="R23" s="196"/>
-      <c r="S23" s="196"/>
-      <c r="T23" s="196"/>
-      <c r="U23" s="210"/>
-      <c r="V23" s="196"/>
-      <c r="W23" s="196"/>
-      <c r="X23" s="196"/>
+      <c r="C23" s="184"/>
+      <c r="D23" s="190"/>
+      <c r="E23" s="190"/>
+      <c r="F23" s="190"/>
+      <c r="G23" s="190"/>
+      <c r="H23" s="197"/>
+      <c r="I23" s="190"/>
+      <c r="J23" s="196"/>
+      <c r="K23" s="196"/>
+      <c r="L23" s="196"/>
+      <c r="M23" s="196"/>
+      <c r="N23" s="196"/>
+      <c r="O23" s="204"/>
+      <c r="P23" s="204"/>
+      <c r="Q23" s="204"/>
+      <c r="R23" s="190"/>
+      <c r="S23" s="190"/>
+      <c r="T23" s="190"/>
+      <c r="U23" s="204"/>
+      <c r="V23" s="190"/>
+      <c r="W23" s="190"/>
+      <c r="X23" s="190"/>
     </row>
     <row r="24" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="173"/>
       <c r="B24" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="186" t="s">
+      <c r="C24" s="180" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="196"/>
-      <c r="E24" s="196"/>
-      <c r="F24" s="196"/>
-      <c r="G24" s="197">
+      <c r="D24" s="190"/>
+      <c r="E24" s="190"/>
+      <c r="F24" s="190"/>
+      <c r="G24" s="191">
         <v>0</v>
       </c>
-      <c r="H24" s="203"/>
-      <c r="I24" s="196"/>
-      <c r="J24" s="196"/>
-      <c r="K24" s="196"/>
-      <c r="L24" s="196"/>
-      <c r="M24" s="196"/>
-      <c r="N24" s="196"/>
-      <c r="O24" s="210"/>
-      <c r="P24" s="210"/>
-      <c r="Q24" s="210"/>
-      <c r="R24" s="196"/>
-      <c r="S24" s="196"/>
-      <c r="T24" s="196"/>
-      <c r="U24" s="210"/>
-      <c r="V24" s="196"/>
-      <c r="W24" s="196"/>
-      <c r="X24" s="196"/>
+      <c r="H24" s="197"/>
+      <c r="I24" s="190"/>
+      <c r="J24" s="190"/>
+      <c r="K24" s="190"/>
+      <c r="L24" s="190"/>
+      <c r="M24" s="190"/>
+      <c r="N24" s="190"/>
+      <c r="O24" s="204"/>
+      <c r="P24" s="204"/>
+      <c r="Q24" s="204"/>
+      <c r="R24" s="190"/>
+      <c r="S24" s="190"/>
+      <c r="T24" s="190"/>
+      <c r="U24" s="204"/>
+      <c r="V24" s="190"/>
+      <c r="W24" s="190"/>
+      <c r="X24" s="190"/>
     </row>
     <row r="25" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="39"/>
       <c r="B25" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="186" t="s">
+      <c r="C25" s="180" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="196"/>
-      <c r="E25" s="196"/>
-      <c r="F25" s="196"/>
-      <c r="G25" s="197">
+      <c r="D25" s="190"/>
+      <c r="E25" s="190"/>
+      <c r="F25" s="190"/>
+      <c r="G25" s="191">
         <v>0.25</v>
       </c>
-      <c r="H25" s="196"/>
-      <c r="I25" s="199"/>
-      <c r="J25" s="196"/>
-      <c r="K25" s="196"/>
-      <c r="L25" s="196"/>
-      <c r="M25" s="196"/>
-      <c r="N25" s="199"/>
-      <c r="O25" s="196"/>
-      <c r="P25" s="196"/>
-      <c r="Q25" s="196"/>
-      <c r="R25" s="199"/>
-      <c r="S25" s="196"/>
-      <c r="T25" s="196"/>
-      <c r="U25" s="196"/>
-      <c r="V25" s="199"/>
-      <c r="W25" s="196"/>
-      <c r="X25" s="196"/>
+      <c r="H25" s="190"/>
+      <c r="I25" s="193"/>
+      <c r="J25" s="190"/>
+      <c r="K25" s="190"/>
+      <c r="L25" s="190"/>
+      <c r="M25" s="190"/>
+      <c r="N25" s="193"/>
+      <c r="O25" s="190"/>
+      <c r="P25" s="190"/>
+      <c r="Q25" s="190"/>
+      <c r="R25" s="193"/>
+      <c r="S25" s="190"/>
+      <c r="T25" s="190"/>
+      <c r="U25" s="190"/>
+      <c r="V25" s="193"/>
+      <c r="W25" s="190"/>
+      <c r="X25" s="190"/>
     </row>
     <row r="26" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="39"/>
       <c r="B26" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="186" t="s">
+      <c r="C26" s="180" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="196"/>
-      <c r="E26" s="196"/>
-      <c r="F26" s="196"/>
-      <c r="G26" s="197">
+      <c r="D26" s="190"/>
+      <c r="E26" s="190"/>
+      <c r="F26" s="190"/>
+      <c r="G26" s="191">
         <v>0.25</v>
       </c>
-      <c r="H26" s="196"/>
-      <c r="I26" s="199"/>
-      <c r="J26" s="196"/>
-      <c r="K26" s="196"/>
-      <c r="L26" s="196"/>
-      <c r="M26" s="196"/>
-      <c r="N26" s="199"/>
-      <c r="O26" s="196"/>
-      <c r="P26" s="196"/>
-      <c r="Q26" s="196"/>
-      <c r="R26" s="199"/>
-      <c r="S26" s="196"/>
-      <c r="T26" s="196"/>
-      <c r="U26" s="196"/>
-      <c r="V26" s="199"/>
-      <c r="W26" s="196"/>
-      <c r="X26" s="196"/>
+      <c r="H26" s="190"/>
+      <c r="I26" s="193"/>
+      <c r="J26" s="190"/>
+      <c r="K26" s="190"/>
+      <c r="L26" s="190"/>
+      <c r="M26" s="190"/>
+      <c r="N26" s="193"/>
+      <c r="O26" s="190"/>
+      <c r="P26" s="190"/>
+      <c r="Q26" s="190"/>
+      <c r="R26" s="193"/>
+      <c r="S26" s="190"/>
+      <c r="T26" s="190"/>
+      <c r="U26" s="190"/>
+      <c r="V26" s="193"/>
+      <c r="W26" s="190"/>
+      <c r="X26" s="190"/>
     </row>
     <row r="27" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="174"/>
       <c r="B27" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="191" t="s">
+      <c r="C27" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="203"/>
-      <c r="E27" s="203"/>
-      <c r="F27" s="203"/>
-      <c r="G27" s="199">
+      <c r="D27" s="197"/>
+      <c r="E27" s="197"/>
+      <c r="F27" s="197"/>
+      <c r="G27" s="193">
         <v>0</v>
       </c>
-      <c r="H27" s="199"/>
-      <c r="I27" s="203"/>
-      <c r="J27" s="203"/>
-      <c r="K27" s="203"/>
-      <c r="L27" s="203"/>
-      <c r="M27" s="199"/>
-      <c r="N27" s="203"/>
-      <c r="O27" s="203"/>
-      <c r="P27" s="203"/>
-      <c r="Q27" s="199"/>
-      <c r="R27" s="203"/>
-      <c r="S27" s="203"/>
-      <c r="T27" s="203"/>
-      <c r="U27" s="199"/>
-      <c r="V27" s="203"/>
-      <c r="W27" s="203"/>
-      <c r="X27" s="213"/>
+      <c r="H27" s="193"/>
+      <c r="I27" s="197"/>
+      <c r="J27" s="197"/>
+      <c r="K27" s="197"/>
+      <c r="L27" s="197"/>
+      <c r="M27" s="193"/>
+      <c r="N27" s="197"/>
+      <c r="O27" s="197"/>
+      <c r="P27" s="197"/>
+      <c r="Q27" s="193"/>
+      <c r="R27" s="197"/>
+      <c r="S27" s="197"/>
+      <c r="T27" s="197"/>
+      <c r="U27" s="193"/>
+      <c r="V27" s="197"/>
+      <c r="W27" s="197"/>
+      <c r="X27" s="207"/>
       <c r="Y27" s="176"/>
       <c r="Z27" s="176"/>
       <c r="AA27" s="176"/>
@@ -3440,897 +3442,897 @@
       <c r="B28" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="186" t="s">
+      <c r="C28" s="180" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="196"/>
-      <c r="E28" s="196"/>
-      <c r="F28" s="196"/>
-      <c r="G28" s="196" t="s">
+      <c r="D28" s="190"/>
+      <c r="E28" s="190"/>
+      <c r="F28" s="190"/>
+      <c r="G28" s="190" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="196"/>
-      <c r="I28" s="199"/>
-      <c r="J28" s="196"/>
-      <c r="K28" s="196"/>
-      <c r="L28" s="196"/>
-      <c r="M28" s="196"/>
-      <c r="N28" s="199"/>
-      <c r="O28" s="196"/>
-      <c r="P28" s="196"/>
-      <c r="Q28" s="196"/>
-      <c r="R28" s="199"/>
-      <c r="S28" s="196"/>
-      <c r="T28" s="196"/>
-      <c r="U28" s="196"/>
-      <c r="V28" s="199"/>
-      <c r="W28" s="196"/>
-      <c r="X28" s="196"/>
+      <c r="H28" s="190"/>
+      <c r="I28" s="193"/>
+      <c r="J28" s="190"/>
+      <c r="K28" s="190"/>
+      <c r="L28" s="190"/>
+      <c r="M28" s="190"/>
+      <c r="N28" s="193"/>
+      <c r="O28" s="190"/>
+      <c r="P28" s="190"/>
+      <c r="Q28" s="190"/>
+      <c r="R28" s="193"/>
+      <c r="S28" s="190"/>
+      <c r="T28" s="190"/>
+      <c r="U28" s="190"/>
+      <c r="V28" s="193"/>
+      <c r="W28" s="190"/>
+      <c r="X28" s="190"/>
     </row>
     <row r="29" spans="1:27" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="188"/>
-      <c r="D29" s="203"/>
-      <c r="E29" s="203"/>
-      <c r="F29" s="203"/>
-      <c r="G29" s="206"/>
-      <c r="H29" s="203"/>
-      <c r="I29" s="199"/>
-      <c r="J29" s="203"/>
-      <c r="K29" s="203"/>
-      <c r="L29" s="203"/>
-      <c r="M29" s="203"/>
-      <c r="N29" s="199"/>
-      <c r="O29" s="203"/>
-      <c r="P29" s="203"/>
-      <c r="Q29" s="203"/>
-      <c r="R29" s="199"/>
-      <c r="S29" s="203"/>
-      <c r="T29" s="203"/>
-      <c r="U29" s="203"/>
-      <c r="V29" s="199"/>
-      <c r="W29" s="203"/>
-      <c r="X29" s="203"/>
+      <c r="C29" s="182"/>
+      <c r="D29" s="197"/>
+      <c r="E29" s="197"/>
+      <c r="F29" s="197"/>
+      <c r="G29" s="200"/>
+      <c r="H29" s="197"/>
+      <c r="I29" s="193"/>
+      <c r="J29" s="197"/>
+      <c r="K29" s="197"/>
+      <c r="L29" s="197"/>
+      <c r="M29" s="197"/>
+      <c r="N29" s="193"/>
+      <c r="O29" s="197"/>
+      <c r="P29" s="197"/>
+      <c r="Q29" s="197"/>
+      <c r="R29" s="193"/>
+      <c r="S29" s="197"/>
+      <c r="T29" s="197"/>
+      <c r="U29" s="197"/>
+      <c r="V29" s="193"/>
+      <c r="W29" s="197"/>
+      <c r="X29" s="197"/>
     </row>
     <row r="30" spans="1:27" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="18"/>
-      <c r="C30" s="189"/>
-      <c r="D30" s="207"/>
-      <c r="E30" s="207"/>
-      <c r="F30" s="207"/>
-      <c r="G30" s="207"/>
-      <c r="H30" s="207"/>
-      <c r="I30" s="207"/>
-      <c r="J30" s="207"/>
-      <c r="K30" s="207"/>
-      <c r="L30" s="207"/>
-      <c r="M30" s="207"/>
-      <c r="N30" s="207"/>
-      <c r="O30" s="207"/>
-      <c r="P30" s="207"/>
-      <c r="Q30" s="207"/>
-      <c r="R30" s="207"/>
-      <c r="S30" s="207"/>
-      <c r="T30" s="207"/>
-      <c r="U30" s="207"/>
-      <c r="V30" s="207"/>
-      <c r="W30" s="207"/>
-      <c r="X30" s="207"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="201"/>
+      <c r="E30" s="201"/>
+      <c r="F30" s="201"/>
+      <c r="G30" s="201"/>
+      <c r="H30" s="201"/>
+      <c r="I30" s="201"/>
+      <c r="J30" s="201"/>
+      <c r="K30" s="201"/>
+      <c r="L30" s="201"/>
+      <c r="M30" s="201"/>
+      <c r="N30" s="201"/>
+      <c r="O30" s="201"/>
+      <c r="P30" s="201"/>
+      <c r="Q30" s="201"/>
+      <c r="R30" s="201"/>
+      <c r="S30" s="201"/>
+      <c r="T30" s="201"/>
+      <c r="U30" s="201"/>
+      <c r="V30" s="201"/>
+      <c r="W30" s="201"/>
+      <c r="X30" s="201"/>
     </row>
     <row r="31" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="57" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="178"/>
-      <c r="C31" s="190"/>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="203"/>
-      <c r="I31" s="196"/>
-      <c r="J31" s="210"/>
-      <c r="K31" s="210"/>
-      <c r="L31" s="210"/>
-      <c r="M31" s="203"/>
-      <c r="N31" s="196"/>
-      <c r="O31" s="196"/>
-      <c r="P31" s="196"/>
-      <c r="Q31" s="203"/>
-      <c r="R31" s="196"/>
-      <c r="S31" s="196"/>
-      <c r="T31" s="196"/>
-      <c r="U31" s="203"/>
-      <c r="V31" s="196"/>
-      <c r="W31" s="196"/>
-      <c r="X31" s="196"/>
+      <c r="C31" s="184"/>
+      <c r="D31" s="190"/>
+      <c r="E31" s="190"/>
+      <c r="F31" s="190"/>
+      <c r="G31" s="190"/>
+      <c r="H31" s="197"/>
+      <c r="I31" s="190"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="204"/>
+      <c r="L31" s="204"/>
+      <c r="M31" s="197"/>
+      <c r="N31" s="190"/>
+      <c r="O31" s="190"/>
+      <c r="P31" s="190"/>
+      <c r="Q31" s="197"/>
+      <c r="R31" s="190"/>
+      <c r="S31" s="190"/>
+      <c r="T31" s="190"/>
+      <c r="U31" s="197"/>
+      <c r="V31" s="190"/>
+      <c r="W31" s="190"/>
+      <c r="X31" s="190"/>
     </row>
     <row r="32" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="39"/>
       <c r="B32" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="186"/>
-      <c r="D32" s="196"/>
-      <c r="E32" s="196"/>
-      <c r="F32" s="196"/>
-      <c r="G32" s="214"/>
-      <c r="H32" s="214"/>
-      <c r="I32" s="202"/>
-      <c r="J32" s="196"/>
-      <c r="K32" s="196"/>
-      <c r="L32" s="196"/>
-      <c r="M32" s="196"/>
-      <c r="N32" s="199"/>
-      <c r="O32" s="196"/>
-      <c r="P32" s="196"/>
-      <c r="Q32" s="196"/>
-      <c r="R32" s="199"/>
-      <c r="S32" s="196"/>
-      <c r="T32" s="196"/>
-      <c r="U32" s="196"/>
-      <c r="V32" s="199"/>
-      <c r="W32" s="196"/>
-      <c r="X32" s="196"/>
+      <c r="C32" s="180"/>
+      <c r="D32" s="190"/>
+      <c r="E32" s="190"/>
+      <c r="F32" s="190"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="208"/>
+      <c r="I32" s="196"/>
+      <c r="J32" s="190"/>
+      <c r="K32" s="190"/>
+      <c r="L32" s="190"/>
+      <c r="M32" s="190"/>
+      <c r="N32" s="193"/>
+      <c r="O32" s="190"/>
+      <c r="P32" s="190"/>
+      <c r="Q32" s="190"/>
+      <c r="R32" s="193"/>
+      <c r="S32" s="190"/>
+      <c r="T32" s="190"/>
+      <c r="U32" s="190"/>
+      <c r="V32" s="193"/>
+      <c r="W32" s="190"/>
+      <c r="X32" s="190"/>
     </row>
     <row r="33" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="39"/>
       <c r="B33" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="186"/>
-      <c r="D33" s="196"/>
-      <c r="E33" s="196"/>
-      <c r="F33" s="196"/>
-      <c r="G33" s="214"/>
-      <c r="H33" s="214"/>
-      <c r="I33" s="196"/>
-      <c r="J33" s="202"/>
-      <c r="K33" s="196"/>
-      <c r="L33" s="196"/>
-      <c r="M33" s="196"/>
-      <c r="N33" s="199"/>
-      <c r="O33" s="196"/>
-      <c r="P33" s="196"/>
-      <c r="Q33" s="196"/>
-      <c r="R33" s="199"/>
-      <c r="S33" s="196"/>
-      <c r="T33" s="196"/>
-      <c r="U33" s="196"/>
-      <c r="V33" s="199"/>
-      <c r="W33" s="196"/>
-      <c r="X33" s="196"/>
+      <c r="C33" s="180"/>
+      <c r="D33" s="190"/>
+      <c r="E33" s="190"/>
+      <c r="F33" s="190"/>
+      <c r="G33" s="208"/>
+      <c r="H33" s="208"/>
+      <c r="I33" s="190"/>
+      <c r="J33" s="196"/>
+      <c r="K33" s="190"/>
+      <c r="L33" s="190"/>
+      <c r="M33" s="190"/>
+      <c r="N33" s="193"/>
+      <c r="O33" s="190"/>
+      <c r="P33" s="190"/>
+      <c r="Q33" s="190"/>
+      <c r="R33" s="193"/>
+      <c r="S33" s="190"/>
+      <c r="T33" s="190"/>
+      <c r="U33" s="190"/>
+      <c r="V33" s="193"/>
+      <c r="W33" s="190"/>
+      <c r="X33" s="190"/>
     </row>
     <row r="34" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="39"/>
       <c r="B34" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="186"/>
-      <c r="D34" s="196"/>
-      <c r="E34" s="196"/>
-      <c r="F34" s="196"/>
-      <c r="G34" s="196"/>
-      <c r="H34" s="214"/>
-      <c r="I34" s="196"/>
-      <c r="J34" s="214"/>
-      <c r="K34" s="211"/>
-      <c r="L34" s="202"/>
-      <c r="M34" s="196"/>
-      <c r="N34" s="199"/>
-      <c r="O34" s="196"/>
-      <c r="P34" s="196"/>
-      <c r="Q34" s="196"/>
-      <c r="R34" s="199"/>
-      <c r="S34" s="196"/>
-      <c r="T34" s="196"/>
-      <c r="U34" s="196"/>
-      <c r="V34" s="199"/>
-      <c r="W34" s="196"/>
-      <c r="X34" s="196"/>
+      <c r="C34" s="180"/>
+      <c r="D34" s="190"/>
+      <c r="E34" s="190"/>
+      <c r="F34" s="190"/>
+      <c r="G34" s="190"/>
+      <c r="H34" s="208"/>
+      <c r="I34" s="190"/>
+      <c r="J34" s="208"/>
+      <c r="K34" s="205"/>
+      <c r="L34" s="196"/>
+      <c r="M34" s="190"/>
+      <c r="N34" s="193"/>
+      <c r="O34" s="190"/>
+      <c r="P34" s="190"/>
+      <c r="Q34" s="190"/>
+      <c r="R34" s="193"/>
+      <c r="S34" s="190"/>
+      <c r="T34" s="190"/>
+      <c r="U34" s="190"/>
+      <c r="V34" s="193"/>
+      <c r="W34" s="190"/>
+      <c r="X34" s="190"/>
     </row>
     <row r="35" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="39"/>
       <c r="B35" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="186"/>
-      <c r="D35" s="196"/>
-      <c r="E35" s="196"/>
-      <c r="F35" s="196"/>
-      <c r="G35" s="196"/>
-      <c r="H35" s="196"/>
-      <c r="I35" s="199"/>
-      <c r="J35" s="196"/>
-      <c r="K35" s="214"/>
-      <c r="L35" s="214"/>
-      <c r="M35" s="202"/>
-      <c r="N35" s="202"/>
-      <c r="O35" s="196"/>
-      <c r="P35" s="196"/>
-      <c r="Q35" s="196"/>
-      <c r="R35" s="199"/>
-      <c r="S35" s="196"/>
-      <c r="T35" s="196"/>
-      <c r="U35" s="196"/>
-      <c r="V35" s="199"/>
-      <c r="W35" s="196"/>
-      <c r="X35" s="196"/>
+      <c r="C35" s="180"/>
+      <c r="D35" s="190"/>
+      <c r="E35" s="190"/>
+      <c r="F35" s="190"/>
+      <c r="G35" s="190"/>
+      <c r="H35" s="190"/>
+      <c r="I35" s="193"/>
+      <c r="J35" s="190"/>
+      <c r="K35" s="208"/>
+      <c r="L35" s="208"/>
+      <c r="M35" s="196"/>
+      <c r="N35" s="196"/>
+      <c r="O35" s="190"/>
+      <c r="P35" s="190"/>
+      <c r="Q35" s="190"/>
+      <c r="R35" s="193"/>
+      <c r="S35" s="190"/>
+      <c r="T35" s="190"/>
+      <c r="U35" s="190"/>
+      <c r="V35" s="193"/>
+      <c r="W35" s="190"/>
+      <c r="X35" s="190"/>
     </row>
     <row r="36" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="39"/>
       <c r="B36" s="46"/>
-      <c r="C36" s="186"/>
-      <c r="D36" s="196"/>
-      <c r="E36" s="196"/>
-      <c r="F36" s="196"/>
-      <c r="G36" s="196"/>
-      <c r="H36" s="196"/>
-      <c r="I36" s="199"/>
-      <c r="J36" s="196"/>
-      <c r="K36" s="196"/>
-      <c r="L36" s="196"/>
-      <c r="M36" s="196"/>
-      <c r="N36" s="199"/>
-      <c r="O36" s="196"/>
-      <c r="P36" s="196"/>
-      <c r="Q36" s="196"/>
-      <c r="R36" s="199"/>
-      <c r="S36" s="196"/>
-      <c r="T36" s="196"/>
-      <c r="U36" s="196"/>
-      <c r="V36" s="199"/>
-      <c r="W36" s="196"/>
-      <c r="X36" s="196"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="190"/>
+      <c r="E36" s="190"/>
+      <c r="F36" s="190"/>
+      <c r="G36" s="190"/>
+      <c r="H36" s="190"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="190"/>
+      <c r="K36" s="190"/>
+      <c r="L36" s="190"/>
+      <c r="M36" s="190"/>
+      <c r="N36" s="193"/>
+      <c r="O36" s="190"/>
+      <c r="P36" s="190"/>
+      <c r="Q36" s="190"/>
+      <c r="R36" s="193"/>
+      <c r="S36" s="190"/>
+      <c r="T36" s="190"/>
+      <c r="U36" s="190"/>
+      <c r="V36" s="193"/>
+      <c r="W36" s="190"/>
+      <c r="X36" s="190"/>
     </row>
     <row r="37" spans="1:24" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B37" s="18"/>
-      <c r="C37" s="189"/>
-      <c r="D37" s="207"/>
-      <c r="E37" s="207"/>
-      <c r="F37" s="207"/>
-      <c r="G37" s="207"/>
-      <c r="H37" s="207"/>
-      <c r="I37" s="207"/>
-      <c r="J37" s="207"/>
-      <c r="K37" s="207"/>
-      <c r="L37" s="207"/>
-      <c r="M37" s="207"/>
-      <c r="N37" s="207"/>
-      <c r="O37" s="207"/>
-      <c r="P37" s="207"/>
-      <c r="Q37" s="207"/>
-      <c r="R37" s="207"/>
-      <c r="S37" s="207"/>
-      <c r="T37" s="207"/>
-      <c r="U37" s="207"/>
-      <c r="V37" s="207"/>
-      <c r="W37" s="207"/>
-      <c r="X37" s="207"/>
+      <c r="C37" s="183"/>
+      <c r="D37" s="201"/>
+      <c r="E37" s="201"/>
+      <c r="F37" s="201"/>
+      <c r="G37" s="201"/>
+      <c r="H37" s="201"/>
+      <c r="I37" s="201"/>
+      <c r="J37" s="201"/>
+      <c r="K37" s="201"/>
+      <c r="L37" s="201"/>
+      <c r="M37" s="201"/>
+      <c r="N37" s="201"/>
+      <c r="O37" s="201"/>
+      <c r="P37" s="201"/>
+      <c r="Q37" s="201"/>
+      <c r="R37" s="201"/>
+      <c r="S37" s="201"/>
+      <c r="T37" s="201"/>
+      <c r="U37" s="201"/>
+      <c r="V37" s="201"/>
+      <c r="W37" s="201"/>
+      <c r="X37" s="201"/>
     </row>
     <row r="38" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="178"/>
-      <c r="C38" s="190"/>
-      <c r="D38" s="196"/>
-      <c r="E38" s="196"/>
-      <c r="F38" s="196"/>
-      <c r="G38" s="196"/>
-      <c r="H38" s="203"/>
-      <c r="I38" s="196"/>
-      <c r="J38" s="196"/>
-      <c r="K38" s="196"/>
-      <c r="L38" s="196"/>
-      <c r="M38" s="203"/>
-      <c r="N38" s="196"/>
-      <c r="O38" s="196"/>
-      <c r="P38" s="196"/>
-      <c r="Q38" s="203"/>
-      <c r="R38" s="196"/>
-      <c r="S38" s="196"/>
-      <c r="T38" s="196"/>
-      <c r="U38" s="203"/>
-      <c r="V38" s="196"/>
-      <c r="W38" s="196"/>
-      <c r="X38" s="196"/>
+      <c r="C38" s="184"/>
+      <c r="D38" s="190"/>
+      <c r="E38" s="190"/>
+      <c r="F38" s="190"/>
+      <c r="G38" s="190"/>
+      <c r="H38" s="197"/>
+      <c r="I38" s="190"/>
+      <c r="J38" s="190"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
+      <c r="M38" s="197"/>
+      <c r="N38" s="190"/>
+      <c r="O38" s="190"/>
+      <c r="P38" s="190"/>
+      <c r="Q38" s="197"/>
+      <c r="R38" s="190"/>
+      <c r="S38" s="190"/>
+      <c r="T38" s="190"/>
+      <c r="U38" s="197"/>
+      <c r="V38" s="190"/>
+      <c r="W38" s="190"/>
+      <c r="X38" s="190"/>
     </row>
     <row r="39" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="39"/>
       <c r="B39" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="186"/>
-      <c r="D39" s="202"/>
-      <c r="E39" s="202"/>
-      <c r="F39" s="202"/>
-      <c r="G39" s="202"/>
-      <c r="H39" s="202"/>
-      <c r="I39" s="199"/>
-      <c r="J39" s="196"/>
-      <c r="K39" s="196"/>
-      <c r="L39" s="196"/>
-      <c r="M39" s="196"/>
-      <c r="N39" s="199"/>
-      <c r="O39" s="196"/>
-      <c r="P39" s="196"/>
-      <c r="Q39" s="196"/>
-      <c r="R39" s="199"/>
-      <c r="S39" s="196"/>
-      <c r="T39" s="196"/>
-      <c r="U39" s="196"/>
-      <c r="V39" s="199"/>
-      <c r="W39" s="196"/>
-      <c r="X39" s="196"/>
+      <c r="C39" s="180"/>
+      <c r="D39" s="196"/>
+      <c r="E39" s="196"/>
+      <c r="F39" s="196"/>
+      <c r="G39" s="196"/>
+      <c r="H39" s="196"/>
+      <c r="I39" s="193"/>
+      <c r="J39" s="190"/>
+      <c r="K39" s="190"/>
+      <c r="L39" s="190"/>
+      <c r="M39" s="190"/>
+      <c r="N39" s="193"/>
+      <c r="O39" s="190"/>
+      <c r="P39" s="190"/>
+      <c r="Q39" s="190"/>
+      <c r="R39" s="193"/>
+      <c r="S39" s="190"/>
+      <c r="T39" s="190"/>
+      <c r="U39" s="190"/>
+      <c r="V39" s="193"/>
+      <c r="W39" s="190"/>
+      <c r="X39" s="190"/>
     </row>
     <row r="40" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="39"/>
       <c r="B40" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="186"/>
-      <c r="D40" s="196"/>
-      <c r="E40" s="196"/>
-      <c r="F40" s="196"/>
-      <c r="G40" s="196"/>
-      <c r="H40" s="196"/>
-      <c r="I40" s="211"/>
-      <c r="J40" s="202"/>
-      <c r="K40" s="202"/>
-      <c r="L40" s="202"/>
-      <c r="M40" s="196"/>
-      <c r="N40" s="199"/>
-      <c r="O40" s="196"/>
-      <c r="P40" s="196"/>
-      <c r="Q40" s="196"/>
-      <c r="R40" s="199"/>
-      <c r="S40" s="196"/>
-      <c r="T40" s="196"/>
-      <c r="U40" s="196"/>
-      <c r="V40" s="199"/>
-      <c r="W40" s="196"/>
-      <c r="X40" s="196"/>
+      <c r="C40" s="180"/>
+      <c r="D40" s="190"/>
+      <c r="E40" s="190"/>
+      <c r="F40" s="190"/>
+      <c r="G40" s="190"/>
+      <c r="H40" s="190"/>
+      <c r="I40" s="205"/>
+      <c r="J40" s="196"/>
+      <c r="K40" s="196"/>
+      <c r="L40" s="196"/>
+      <c r="M40" s="190"/>
+      <c r="N40" s="193"/>
+      <c r="O40" s="190"/>
+      <c r="P40" s="190"/>
+      <c r="Q40" s="190"/>
+      <c r="R40" s="193"/>
+      <c r="S40" s="190"/>
+      <c r="T40" s="190"/>
+      <c r="U40" s="190"/>
+      <c r="V40" s="193"/>
+      <c r="W40" s="190"/>
+      <c r="X40" s="190"/>
     </row>
     <row r="41" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="39"/>
       <c r="B41" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="186"/>
-      <c r="D41" s="196"/>
-      <c r="E41" s="196"/>
-      <c r="F41" s="196"/>
-      <c r="G41" s="196"/>
-      <c r="H41" s="196"/>
-      <c r="I41" s="199"/>
-      <c r="J41" s="196"/>
-      <c r="K41" s="211"/>
-      <c r="L41" s="211"/>
-      <c r="M41" s="202"/>
-      <c r="N41" s="196"/>
-      <c r="O41" s="196"/>
-      <c r="P41" s="196"/>
-      <c r="Q41" s="196"/>
-      <c r="R41" s="199"/>
-      <c r="S41" s="196"/>
-      <c r="T41" s="196"/>
-      <c r="U41" s="196"/>
-      <c r="V41" s="199"/>
-      <c r="W41" s="196"/>
-      <c r="X41" s="196"/>
+      <c r="C41" s="180"/>
+      <c r="D41" s="190"/>
+      <c r="E41" s="190"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="190"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="190"/>
+      <c r="K41" s="205"/>
+      <c r="L41" s="205"/>
+      <c r="M41" s="196"/>
+      <c r="N41" s="190"/>
+      <c r="O41" s="190"/>
+      <c r="P41" s="190"/>
+      <c r="Q41" s="190"/>
+      <c r="R41" s="193"/>
+      <c r="S41" s="190"/>
+      <c r="T41" s="190"/>
+      <c r="U41" s="190"/>
+      <c r="V41" s="193"/>
+      <c r="W41" s="190"/>
+      <c r="X41" s="190"/>
     </row>
     <row r="42" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="39"/>
       <c r="B42" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="186"/>
-      <c r="D42" s="196"/>
-      <c r="E42" s="196"/>
-      <c r="F42" s="196"/>
-      <c r="G42" s="196"/>
-      <c r="H42" s="196"/>
-      <c r="I42" s="199"/>
-      <c r="J42" s="196"/>
-      <c r="K42" s="199"/>
-      <c r="L42" s="199"/>
-      <c r="M42" s="202"/>
-      <c r="N42" s="202"/>
-      <c r="O42" s="196"/>
-      <c r="P42" s="196"/>
-      <c r="Q42" s="196"/>
-      <c r="R42" s="199"/>
-      <c r="S42" s="196"/>
-      <c r="T42" s="196"/>
-      <c r="U42" s="196"/>
-      <c r="V42" s="199"/>
-      <c r="W42" s="196"/>
-      <c r="X42" s="196"/>
+      <c r="C42" s="180"/>
+      <c r="D42" s="190"/>
+      <c r="E42" s="190"/>
+      <c r="F42" s="190"/>
+      <c r="G42" s="190"/>
+      <c r="H42" s="190"/>
+      <c r="I42" s="193"/>
+      <c r="J42" s="190"/>
+      <c r="K42" s="193"/>
+      <c r="L42" s="193"/>
+      <c r="M42" s="196"/>
+      <c r="N42" s="196"/>
+      <c r="O42" s="190"/>
+      <c r="P42" s="190"/>
+      <c r="Q42" s="190"/>
+      <c r="R42" s="193"/>
+      <c r="S42" s="190"/>
+      <c r="T42" s="190"/>
+      <c r="U42" s="190"/>
+      <c r="V42" s="193"/>
+      <c r="W42" s="190"/>
+      <c r="X42" s="190"/>
     </row>
     <row r="43" spans="1:24" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2"/>
       <c r="B43" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="188"/>
-      <c r="D43" s="203"/>
-      <c r="E43" s="203"/>
-      <c r="F43" s="203"/>
-      <c r="G43" s="203"/>
-      <c r="H43" s="203"/>
-      <c r="I43" s="199"/>
-      <c r="J43" s="199"/>
-      <c r="K43" s="199"/>
-      <c r="L43" s="199"/>
-      <c r="M43" s="199"/>
-      <c r="N43" s="211"/>
-      <c r="O43" s="202"/>
-      <c r="P43" s="196"/>
-      <c r="Q43" s="196"/>
-      <c r="R43" s="199"/>
-      <c r="S43" s="199"/>
-      <c r="T43" s="199"/>
-      <c r="U43" s="196"/>
-      <c r="V43" s="199"/>
-      <c r="W43" s="199"/>
-      <c r="X43" s="199"/>
+      <c r="C43" s="182"/>
+      <c r="D43" s="197"/>
+      <c r="E43" s="197"/>
+      <c r="F43" s="197"/>
+      <c r="G43" s="197"/>
+      <c r="H43" s="197"/>
+      <c r="I43" s="193"/>
+      <c r="J43" s="193"/>
+      <c r="K43" s="193"/>
+      <c r="L43" s="193"/>
+      <c r="M43" s="193"/>
+      <c r="N43" s="205"/>
+      <c r="O43" s="196"/>
+      <c r="P43" s="190"/>
+      <c r="Q43" s="190"/>
+      <c r="R43" s="193"/>
+      <c r="S43" s="193"/>
+      <c r="T43" s="193"/>
+      <c r="U43" s="190"/>
+      <c r="V43" s="193"/>
+      <c r="W43" s="193"/>
+      <c r="X43" s="193"/>
     </row>
     <row r="44" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="39"/>
       <c r="B44" s="42"/>
-      <c r="C44" s="190"/>
-      <c r="D44" s="196"/>
-      <c r="E44" s="196"/>
-      <c r="F44" s="196"/>
-      <c r="G44" s="196"/>
-      <c r="H44" s="196"/>
-      <c r="I44" s="196"/>
-      <c r="J44" s="196"/>
-      <c r="K44" s="196"/>
-      <c r="L44" s="196"/>
-      <c r="M44" s="196"/>
-      <c r="N44" s="196"/>
-      <c r="O44" s="196"/>
-      <c r="P44" s="196"/>
-      <c r="Q44" s="196"/>
-      <c r="R44" s="196"/>
-      <c r="S44" s="196"/>
-      <c r="T44" s="196"/>
-      <c r="U44" s="196"/>
-      <c r="V44" s="196"/>
-      <c r="W44" s="196"/>
-      <c r="X44" s="196"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="190"/>
+      <c r="E44" s="190"/>
+      <c r="F44" s="190"/>
+      <c r="G44" s="190"/>
+      <c r="H44" s="190"/>
+      <c r="I44" s="190"/>
+      <c r="J44" s="190"/>
+      <c r="K44" s="190"/>
+      <c r="L44" s="190"/>
+      <c r="M44" s="190"/>
+      <c r="N44" s="190"/>
+      <c r="O44" s="190"/>
+      <c r="P44" s="190"/>
+      <c r="Q44" s="190"/>
+      <c r="R44" s="190"/>
+      <c r="S44" s="190"/>
+      <c r="T44" s="190"/>
+      <c r="U44" s="190"/>
+      <c r="V44" s="190"/>
+      <c r="W44" s="190"/>
+      <c r="X44" s="190"/>
     </row>
     <row r="45" spans="1:24" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="18"/>
-      <c r="C45" s="189"/>
-      <c r="D45" s="207"/>
-      <c r="E45" s="207"/>
-      <c r="F45" s="207"/>
-      <c r="G45" s="207"/>
-      <c r="H45" s="207"/>
-      <c r="I45" s="207"/>
-      <c r="J45" s="207"/>
-      <c r="K45" s="207"/>
-      <c r="L45" s="207"/>
-      <c r="M45" s="207"/>
-      <c r="N45" s="207"/>
-      <c r="O45" s="207"/>
-      <c r="P45" s="207"/>
-      <c r="Q45" s="207"/>
-      <c r="R45" s="207"/>
-      <c r="S45" s="207"/>
-      <c r="T45" s="207"/>
-      <c r="U45" s="207"/>
-      <c r="V45" s="207"/>
-      <c r="W45" s="207"/>
-      <c r="X45" s="207"/>
+      <c r="C45" s="183"/>
+      <c r="D45" s="201"/>
+      <c r="E45" s="201"/>
+      <c r="F45" s="201"/>
+      <c r="G45" s="201"/>
+      <c r="H45" s="201"/>
+      <c r="I45" s="201"/>
+      <c r="J45" s="201"/>
+      <c r="K45" s="201"/>
+      <c r="L45" s="201"/>
+      <c r="M45" s="201"/>
+      <c r="N45" s="201"/>
+      <c r="O45" s="201"/>
+      <c r="P45" s="201"/>
+      <c r="Q45" s="201"/>
+      <c r="R45" s="201"/>
+      <c r="S45" s="201"/>
+      <c r="T45" s="201"/>
+      <c r="U45" s="201"/>
+      <c r="V45" s="201"/>
+      <c r="W45" s="201"/>
+      <c r="X45" s="201"/>
     </row>
     <row r="46" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="57" t="s">
         <v>23</v>
       </c>
       <c r="B46" s="178"/>
-      <c r="C46" s="190"/>
-      <c r="D46" s="196"/>
-      <c r="E46" s="196"/>
-      <c r="F46" s="196"/>
-      <c r="G46" s="196"/>
-      <c r="H46" s="203"/>
-      <c r="I46" s="196"/>
-      <c r="J46" s="196"/>
-      <c r="K46" s="196"/>
-      <c r="L46" s="196"/>
-      <c r="M46" s="203"/>
-      <c r="N46" s="196"/>
-      <c r="O46" s="196"/>
-      <c r="P46" s="202"/>
-      <c r="Q46" s="203"/>
-      <c r="R46" s="196"/>
-      <c r="S46" s="196"/>
-      <c r="T46" s="196"/>
-      <c r="U46" s="203"/>
-      <c r="V46" s="196"/>
-      <c r="W46" s="196"/>
-      <c r="X46" s="196"/>
+      <c r="C46" s="184"/>
+      <c r="D46" s="190"/>
+      <c r="E46" s="190"/>
+      <c r="F46" s="190"/>
+      <c r="G46" s="190"/>
+      <c r="H46" s="197"/>
+      <c r="I46" s="190"/>
+      <c r="J46" s="190"/>
+      <c r="K46" s="190"/>
+      <c r="L46" s="190"/>
+      <c r="M46" s="197"/>
+      <c r="N46" s="190"/>
+      <c r="O46" s="190"/>
+      <c r="P46" s="196"/>
+      <c r="Q46" s="197"/>
+      <c r="R46" s="190"/>
+      <c r="S46" s="190"/>
+      <c r="T46" s="190"/>
+      <c r="U46" s="197"/>
+      <c r="V46" s="190"/>
+      <c r="W46" s="190"/>
+      <c r="X46" s="190"/>
     </row>
     <row r="47" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="39"/>
       <c r="B47" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="186"/>
-      <c r="D47" s="196"/>
-      <c r="E47" s="196"/>
-      <c r="F47" s="196"/>
-      <c r="G47" s="196"/>
-      <c r="H47" s="196"/>
-      <c r="I47" s="199"/>
-      <c r="J47" s="196"/>
-      <c r="K47" s="196"/>
-      <c r="L47" s="196"/>
-      <c r="M47" s="196"/>
-      <c r="N47" s="199"/>
-      <c r="O47" s="196"/>
-      <c r="P47" s="202"/>
-      <c r="Q47" s="196"/>
-      <c r="R47" s="199"/>
-      <c r="S47" s="196"/>
-      <c r="T47" s="196"/>
-      <c r="U47" s="196"/>
-      <c r="V47" s="199"/>
-      <c r="W47" s="196"/>
-      <c r="X47" s="196"/>
+      <c r="C47" s="180"/>
+      <c r="D47" s="190"/>
+      <c r="E47" s="190"/>
+      <c r="F47" s="190"/>
+      <c r="G47" s="190"/>
+      <c r="H47" s="190"/>
+      <c r="I47" s="193"/>
+      <c r="J47" s="190"/>
+      <c r="K47" s="190"/>
+      <c r="L47" s="190"/>
+      <c r="M47" s="190"/>
+      <c r="N47" s="193"/>
+      <c r="O47" s="190"/>
+      <c r="P47" s="196"/>
+      <c r="Q47" s="190"/>
+      <c r="R47" s="193"/>
+      <c r="S47" s="190"/>
+      <c r="T47" s="190"/>
+      <c r="U47" s="190"/>
+      <c r="V47" s="193"/>
+      <c r="W47" s="190"/>
+      <c r="X47" s="190"/>
     </row>
     <row r="48" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="39"/>
       <c r="B48" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="186"/>
-      <c r="D48" s="196"/>
-      <c r="E48" s="196"/>
-      <c r="F48" s="196"/>
-      <c r="G48" s="196"/>
-      <c r="H48" s="196"/>
-      <c r="I48" s="199"/>
-      <c r="J48" s="196"/>
-      <c r="K48" s="196"/>
-      <c r="L48" s="196"/>
-      <c r="M48" s="196"/>
-      <c r="N48" s="199"/>
-      <c r="O48" s="196"/>
-      <c r="P48" s="202"/>
-      <c r="Q48" s="196"/>
-      <c r="R48" s="199"/>
-      <c r="S48" s="196"/>
-      <c r="T48" s="196"/>
-      <c r="U48" s="196"/>
-      <c r="V48" s="199"/>
-      <c r="W48" s="196"/>
-      <c r="X48" s="196"/>
+      <c r="C48" s="180"/>
+      <c r="D48" s="190"/>
+      <c r="E48" s="190"/>
+      <c r="F48" s="190"/>
+      <c r="G48" s="190"/>
+      <c r="H48" s="190"/>
+      <c r="I48" s="193"/>
+      <c r="J48" s="190"/>
+      <c r="K48" s="190"/>
+      <c r="L48" s="190"/>
+      <c r="M48" s="190"/>
+      <c r="N48" s="193"/>
+      <c r="O48" s="190"/>
+      <c r="P48" s="196"/>
+      <c r="Q48" s="190"/>
+      <c r="R48" s="193"/>
+      <c r="S48" s="190"/>
+      <c r="T48" s="190"/>
+      <c r="U48" s="190"/>
+      <c r="V48" s="193"/>
+      <c r="W48" s="190"/>
+      <c r="X48" s="190"/>
     </row>
     <row r="49" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="39"/>
       <c r="B49" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="186"/>
-      <c r="D49" s="196"/>
-      <c r="E49" s="196"/>
-      <c r="F49" s="196"/>
-      <c r="G49" s="196"/>
-      <c r="H49" s="196"/>
-      <c r="I49" s="199"/>
-      <c r="J49" s="196"/>
-      <c r="K49" s="196"/>
-      <c r="L49" s="196"/>
-      <c r="M49" s="196"/>
-      <c r="N49" s="199"/>
-      <c r="O49" s="196"/>
-      <c r="P49" s="202"/>
-      <c r="Q49" s="196"/>
-      <c r="R49" s="199"/>
-      <c r="S49" s="196"/>
-      <c r="T49" s="196"/>
-      <c r="U49" s="196"/>
-      <c r="V49" s="199"/>
-      <c r="W49" s="196"/>
-      <c r="X49" s="196"/>
+      <c r="C49" s="180"/>
+      <c r="D49" s="190"/>
+      <c r="E49" s="190"/>
+      <c r="F49" s="190"/>
+      <c r="G49" s="190"/>
+      <c r="H49" s="190"/>
+      <c r="I49" s="193"/>
+      <c r="J49" s="190"/>
+      <c r="K49" s="190"/>
+      <c r="L49" s="190"/>
+      <c r="M49" s="190"/>
+      <c r="N49" s="193"/>
+      <c r="O49" s="190"/>
+      <c r="P49" s="196"/>
+      <c r="Q49" s="190"/>
+      <c r="R49" s="193"/>
+      <c r="S49" s="190"/>
+      <c r="T49" s="190"/>
+      <c r="U49" s="190"/>
+      <c r="V49" s="193"/>
+      <c r="W49" s="190"/>
+      <c r="X49" s="190"/>
     </row>
     <row r="50" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="39"/>
       <c r="B50" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="186"/>
-      <c r="D50" s="196"/>
-      <c r="E50" s="196"/>
-      <c r="F50" s="196"/>
-      <c r="G50" s="196"/>
-      <c r="H50" s="196"/>
-      <c r="I50" s="199"/>
-      <c r="J50" s="196"/>
-      <c r="K50" s="196"/>
-      <c r="L50" s="196"/>
-      <c r="M50" s="196"/>
-      <c r="N50" s="199"/>
-      <c r="O50" s="196"/>
-      <c r="P50" s="196"/>
-      <c r="Q50" s="202"/>
-      <c r="R50" s="199"/>
-      <c r="S50" s="196"/>
-      <c r="T50" s="196"/>
-      <c r="U50" s="196"/>
-      <c r="V50" s="199"/>
-      <c r="W50" s="196"/>
-      <c r="X50" s="196"/>
+      <c r="C50" s="180"/>
+      <c r="D50" s="190"/>
+      <c r="E50" s="190"/>
+      <c r="F50" s="190"/>
+      <c r="G50" s="190"/>
+      <c r="H50" s="190"/>
+      <c r="I50" s="193"/>
+      <c r="J50" s="190"/>
+      <c r="K50" s="190"/>
+      <c r="L50" s="190"/>
+      <c r="M50" s="190"/>
+      <c r="N50" s="193"/>
+      <c r="O50" s="190"/>
+      <c r="P50" s="190"/>
+      <c r="Q50" s="196"/>
+      <c r="R50" s="193"/>
+      <c r="S50" s="190"/>
+      <c r="T50" s="190"/>
+      <c r="U50" s="190"/>
+      <c r="V50" s="193"/>
+      <c r="W50" s="190"/>
+      <c r="X50" s="190"/>
     </row>
     <row r="51" spans="1:24" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2"/>
       <c r="B51" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="188"/>
-      <c r="D51" s="203"/>
-      <c r="E51" s="203"/>
-      <c r="F51" s="203"/>
-      <c r="G51" s="203"/>
-      <c r="H51" s="203"/>
-      <c r="I51" s="199"/>
-      <c r="J51" s="199"/>
-      <c r="K51" s="199"/>
-      <c r="L51" s="199"/>
-      <c r="M51" s="203"/>
-      <c r="N51" s="199"/>
-      <c r="O51" s="199"/>
-      <c r="P51" s="199"/>
-      <c r="Q51" s="202"/>
-      <c r="R51" s="199"/>
-      <c r="S51" s="199"/>
-      <c r="T51" s="199"/>
-      <c r="U51" s="203"/>
-      <c r="V51" s="199"/>
-      <c r="W51" s="199"/>
-      <c r="X51" s="199"/>
+      <c r="C51" s="182"/>
+      <c r="D51" s="197"/>
+      <c r="E51" s="197"/>
+      <c r="F51" s="197"/>
+      <c r="G51" s="197"/>
+      <c r="H51" s="197"/>
+      <c r="I51" s="193"/>
+      <c r="J51" s="193"/>
+      <c r="K51" s="193"/>
+      <c r="L51" s="193"/>
+      <c r="M51" s="197"/>
+      <c r="N51" s="193"/>
+      <c r="O51" s="193"/>
+      <c r="P51" s="193"/>
+      <c r="Q51" s="196"/>
+      <c r="R51" s="193"/>
+      <c r="S51" s="193"/>
+      <c r="T51" s="193"/>
+      <c r="U51" s="197"/>
+      <c r="V51" s="193"/>
+      <c r="W51" s="193"/>
+      <c r="X51" s="193"/>
     </row>
     <row r="52" spans="1:24" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="5"/>
       <c r="B52" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="188"/>
-      <c r="D52" s="203"/>
-      <c r="E52" s="203"/>
-      <c r="F52" s="203"/>
-      <c r="G52" s="203"/>
-      <c r="H52" s="203"/>
-      <c r="I52" s="199"/>
-      <c r="J52" s="199"/>
-      <c r="K52" s="199"/>
-      <c r="L52" s="199"/>
-      <c r="M52" s="203"/>
-      <c r="N52" s="199"/>
-      <c r="O52" s="199"/>
-      <c r="P52" s="199"/>
-      <c r="Q52" s="202"/>
-      <c r="R52" s="199"/>
-      <c r="S52" s="199"/>
-      <c r="T52" s="199"/>
-      <c r="U52" s="203"/>
-      <c r="V52" s="199"/>
-      <c r="W52" s="199"/>
-      <c r="X52" s="199"/>
+      <c r="C52" s="182"/>
+      <c r="D52" s="197"/>
+      <c r="E52" s="197"/>
+      <c r="F52" s="197"/>
+      <c r="G52" s="197"/>
+      <c r="H52" s="197"/>
+      <c r="I52" s="193"/>
+      <c r="J52" s="193"/>
+      <c r="K52" s="193"/>
+      <c r="L52" s="193"/>
+      <c r="M52" s="197"/>
+      <c r="N52" s="193"/>
+      <c r="O52" s="193"/>
+      <c r="P52" s="193"/>
+      <c r="Q52" s="196"/>
+      <c r="R52" s="193"/>
+      <c r="S52" s="193"/>
+      <c r="T52" s="193"/>
+      <c r="U52" s="197"/>
+      <c r="V52" s="193"/>
+      <c r="W52" s="193"/>
+      <c r="X52" s="193"/>
     </row>
     <row r="53" spans="1:24" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="5"/>
       <c r="B53" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="188"/>
-      <c r="D53" s="203"/>
-      <c r="E53" s="203"/>
-      <c r="F53" s="203"/>
-      <c r="G53" s="203"/>
-      <c r="H53" s="203"/>
-      <c r="I53" s="199"/>
-      <c r="J53" s="199"/>
-      <c r="K53" s="199"/>
-      <c r="L53" s="199"/>
-      <c r="M53" s="203"/>
-      <c r="N53" s="199"/>
-      <c r="O53" s="199"/>
-      <c r="P53" s="199"/>
-      <c r="Q53" s="202"/>
-      <c r="R53" s="199"/>
-      <c r="S53" s="199"/>
-      <c r="T53" s="199"/>
-      <c r="U53" s="203"/>
-      <c r="V53" s="199"/>
-      <c r="W53" s="199"/>
-      <c r="X53" s="199"/>
+      <c r="C53" s="182"/>
+      <c r="D53" s="197"/>
+      <c r="E53" s="197"/>
+      <c r="F53" s="197"/>
+      <c r="G53" s="197"/>
+      <c r="H53" s="197"/>
+      <c r="I53" s="193"/>
+      <c r="J53" s="193"/>
+      <c r="K53" s="193"/>
+      <c r="L53" s="193"/>
+      <c r="M53" s="197"/>
+      <c r="N53" s="193"/>
+      <c r="O53" s="193"/>
+      <c r="P53" s="193"/>
+      <c r="Q53" s="196"/>
+      <c r="R53" s="193"/>
+      <c r="S53" s="193"/>
+      <c r="T53" s="193"/>
+      <c r="U53" s="197"/>
+      <c r="V53" s="193"/>
+      <c r="W53" s="193"/>
+      <c r="X53" s="193"/>
     </row>
     <row r="54" spans="1:24" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="5"/>
       <c r="B54" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="188"/>
-      <c r="D54" s="203"/>
-      <c r="E54" s="203"/>
-      <c r="F54" s="203"/>
-      <c r="G54" s="203"/>
-      <c r="H54" s="203"/>
-      <c r="I54" s="199"/>
-      <c r="J54" s="199"/>
-      <c r="K54" s="203"/>
-      <c r="L54" s="203"/>
-      <c r="M54" s="203"/>
-      <c r="N54" s="199"/>
-      <c r="O54" s="199"/>
-      <c r="P54" s="203"/>
-      <c r="Q54" s="202"/>
-      <c r="R54" s="199"/>
-      <c r="S54" s="199"/>
-      <c r="T54" s="203"/>
-      <c r="U54" s="203"/>
-      <c r="V54" s="199"/>
-      <c r="W54" s="199"/>
-      <c r="X54" s="203"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="197"/>
+      <c r="E54" s="197"/>
+      <c r="F54" s="197"/>
+      <c r="G54" s="197"/>
+      <c r="H54" s="197"/>
+      <c r="I54" s="193"/>
+      <c r="J54" s="193"/>
+      <c r="K54" s="197"/>
+      <c r="L54" s="197"/>
+      <c r="M54" s="197"/>
+      <c r="N54" s="193"/>
+      <c r="O54" s="193"/>
+      <c r="P54" s="197"/>
+      <c r="Q54" s="196"/>
+      <c r="R54" s="193"/>
+      <c r="S54" s="193"/>
+      <c r="T54" s="197"/>
+      <c r="U54" s="197"/>
+      <c r="V54" s="193"/>
+      <c r="W54" s="193"/>
+      <c r="X54" s="197"/>
     </row>
     <row r="55" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="36"/>
-      <c r="C55" s="188"/>
-      <c r="D55" s="203"/>
-      <c r="E55" s="203"/>
-      <c r="F55" s="203"/>
-      <c r="G55" s="203"/>
-      <c r="H55" s="203"/>
-      <c r="I55" s="199"/>
-      <c r="J55" s="203"/>
-      <c r="K55" s="203"/>
-      <c r="L55" s="203"/>
-      <c r="M55" s="203"/>
-      <c r="N55" s="199"/>
-      <c r="O55" s="203"/>
-      <c r="P55" s="203"/>
-      <c r="Q55" s="203"/>
-      <c r="R55" s="199"/>
-      <c r="S55" s="203"/>
-      <c r="T55" s="203"/>
-      <c r="U55" s="203"/>
-      <c r="V55" s="199"/>
-      <c r="W55" s="203"/>
-      <c r="X55" s="203"/>
+      <c r="C55" s="182"/>
+      <c r="D55" s="197"/>
+      <c r="E55" s="197"/>
+      <c r="F55" s="197"/>
+      <c r="G55" s="197"/>
+      <c r="H55" s="197"/>
+      <c r="I55" s="193"/>
+      <c r="J55" s="197"/>
+      <c r="K55" s="197"/>
+      <c r="L55" s="197"/>
+      <c r="M55" s="197"/>
+      <c r="N55" s="193"/>
+      <c r="O55" s="197"/>
+      <c r="P55" s="197"/>
+      <c r="Q55" s="197"/>
+      <c r="R55" s="193"/>
+      <c r="S55" s="197"/>
+      <c r="T55" s="197"/>
+      <c r="U55" s="197"/>
+      <c r="V55" s="193"/>
+      <c r="W55" s="197"/>
+      <c r="X55" s="197"/>
     </row>
     <row r="56" spans="1:24" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="5"/>
-      <c r="C56" s="192"/>
-      <c r="D56" s="203"/>
-      <c r="E56" s="203"/>
-      <c r="F56" s="203"/>
-      <c r="G56" s="203"/>
-      <c r="H56" s="203"/>
-      <c r="I56" s="203"/>
-      <c r="J56" s="203"/>
-      <c r="K56" s="203"/>
-      <c r="L56" s="203"/>
-      <c r="M56" s="203"/>
-      <c r="N56" s="203"/>
-      <c r="O56" s="203"/>
-      <c r="P56" s="203"/>
-      <c r="Q56" s="203"/>
-      <c r="R56" s="203"/>
-      <c r="S56" s="203"/>
-      <c r="T56" s="203"/>
-      <c r="U56" s="203"/>
-      <c r="V56" s="203"/>
-      <c r="W56" s="203"/>
-      <c r="X56" s="203"/>
+      <c r="C56" s="186"/>
+      <c r="D56" s="197"/>
+      <c r="E56" s="197"/>
+      <c r="F56" s="197"/>
+      <c r="G56" s="197"/>
+      <c r="H56" s="197"/>
+      <c r="I56" s="197"/>
+      <c r="J56" s="197"/>
+      <c r="K56" s="197"/>
+      <c r="L56" s="197"/>
+      <c r="M56" s="197"/>
+      <c r="N56" s="197"/>
+      <c r="O56" s="197"/>
+      <c r="P56" s="197"/>
+      <c r="Q56" s="197"/>
+      <c r="R56" s="197"/>
+      <c r="S56" s="197"/>
+      <c r="T56" s="197"/>
+      <c r="U56" s="197"/>
+      <c r="V56" s="197"/>
+      <c r="W56" s="197"/>
+      <c r="X56" s="197"/>
     </row>
     <row r="57" spans="1:24" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="14"/>
-      <c r="C57" s="193"/>
-      <c r="D57" s="212"/>
-      <c r="E57" s="212"/>
-      <c r="F57" s="212"/>
-      <c r="G57" s="212"/>
-      <c r="H57" s="212"/>
-      <c r="I57" s="212"/>
-      <c r="J57" s="212"/>
-      <c r="K57" s="212"/>
-      <c r="L57" s="212"/>
-      <c r="M57" s="212"/>
-      <c r="N57" s="212"/>
-      <c r="O57" s="212"/>
-      <c r="P57" s="212"/>
-      <c r="Q57" s="212"/>
-      <c r="R57" s="212"/>
-      <c r="S57" s="212"/>
-      <c r="T57" s="212"/>
-      <c r="U57" s="212"/>
-      <c r="V57" s="212"/>
-      <c r="W57" s="212"/>
-      <c r="X57" s="212"/>
+      <c r="C57" s="187"/>
+      <c r="D57" s="206"/>
+      <c r="E57" s="206"/>
+      <c r="F57" s="206"/>
+      <c r="G57" s="206"/>
+      <c r="H57" s="206"/>
+      <c r="I57" s="206"/>
+      <c r="J57" s="206"/>
+      <c r="K57" s="206"/>
+      <c r="L57" s="206"/>
+      <c r="M57" s="206"/>
+      <c r="N57" s="206"/>
+      <c r="O57" s="206"/>
+      <c r="P57" s="206"/>
+      <c r="Q57" s="206"/>
+      <c r="R57" s="206"/>
+      <c r="S57" s="206"/>
+      <c r="T57" s="206"/>
+      <c r="U57" s="206"/>
+      <c r="V57" s="206"/>
+      <c r="W57" s="206"/>
+      <c r="X57" s="206"/>
     </row>
     <row r="58" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39"/>
       <c r="B58" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="190"/>
-      <c r="D58" s="196"/>
-      <c r="E58" s="196"/>
-      <c r="F58" s="196"/>
-      <c r="G58" s="196"/>
-      <c r="H58" s="196"/>
-      <c r="I58" s="196"/>
-      <c r="J58" s="196"/>
-      <c r="K58" s="196"/>
-      <c r="L58" s="196"/>
-      <c r="M58" s="196"/>
-      <c r="N58" s="196"/>
-      <c r="O58" s="196"/>
-      <c r="P58" s="196"/>
-      <c r="Q58" s="210"/>
-      <c r="R58" s="202"/>
-      <c r="S58" s="202"/>
-      <c r="T58" s="202"/>
-      <c r="U58" s="210"/>
-      <c r="V58" s="210"/>
-      <c r="W58" s="210"/>
-      <c r="X58" s="210"/>
+      <c r="C58" s="184"/>
+      <c r="D58" s="190"/>
+      <c r="E58" s="190"/>
+      <c r="F58" s="190"/>
+      <c r="G58" s="190"/>
+      <c r="H58" s="190"/>
+      <c r="I58" s="190"/>
+      <c r="J58" s="190"/>
+      <c r="K58" s="190"/>
+      <c r="L58" s="190"/>
+      <c r="M58" s="190"/>
+      <c r="N58" s="190"/>
+      <c r="O58" s="190"/>
+      <c r="P58" s="190"/>
+      <c r="Q58" s="204"/>
+      <c r="R58" s="196"/>
+      <c r="S58" s="196"/>
+      <c r="T58" s="196"/>
+      <c r="U58" s="204"/>
+      <c r="V58" s="204"/>
+      <c r="W58" s="204"/>
+      <c r="X58" s="204"/>
     </row>
     <row r="59" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="39"/>
       <c r="B59" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="190"/>
-      <c r="D59" s="196"/>
-      <c r="E59" s="196"/>
-      <c r="F59" s="196"/>
-      <c r="G59" s="196"/>
-      <c r="H59" s="196"/>
-      <c r="I59" s="197"/>
-      <c r="J59" s="196"/>
-      <c r="K59" s="196"/>
-      <c r="L59" s="196"/>
-      <c r="M59" s="196"/>
-      <c r="N59" s="197"/>
-      <c r="O59" s="196"/>
-      <c r="P59" s="196"/>
-      <c r="Q59" s="196"/>
-      <c r="R59" s="197"/>
-      <c r="S59" s="196"/>
-      <c r="T59" s="196"/>
-      <c r="U59" s="196"/>
-      <c r="V59" s="202"/>
-      <c r="W59" s="214"/>
-      <c r="X59" s="196"/>
+      <c r="C59" s="184"/>
+      <c r="D59" s="190"/>
+      <c r="E59" s="190"/>
+      <c r="F59" s="190"/>
+      <c r="G59" s="190"/>
+      <c r="H59" s="190"/>
+      <c r="I59" s="191"/>
+      <c r="J59" s="190"/>
+      <c r="K59" s="190"/>
+      <c r="L59" s="190"/>
+      <c r="M59" s="190"/>
+      <c r="N59" s="191"/>
+      <c r="O59" s="190"/>
+      <c r="P59" s="190"/>
+      <c r="Q59" s="190"/>
+      <c r="R59" s="191"/>
+      <c r="S59" s="190"/>
+      <c r="T59" s="190"/>
+      <c r="U59" s="190"/>
+      <c r="V59" s="196"/>
+      <c r="W59" s="208"/>
+      <c r="X59" s="190"/>
     </row>
     <row r="60" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="4"/>
-      <c r="K60" s="194"/>
+      <c r="K60" s="188"/>
       <c r="L60" s="105"/>
-      <c r="P60" s="194"/>
-      <c r="T60" s="194"/>
+      <c r="P60" s="188"/>
+      <c r="T60" s="188"/>
       <c r="W60" s="111"/>
-      <c r="X60" s="194"/>
+      <c r="X60" s="188"/>
     </row>
     <row r="61" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="39"/>
@@ -5279,15 +5281,15 @@
     </row>
     <row r="100" spans="1:24" ht="13" x14ac:dyDescent="0.15">
       <c r="B100" s="29"/>
-      <c r="C100" s="183"/>
-      <c r="D100" s="184"/>
-      <c r="E100" s="184"/>
-      <c r="F100" s="184"/>
-      <c r="G100" s="184"/>
-      <c r="H100" s="184"/>
-      <c r="I100" s="184"/>
-      <c r="J100" s="184"/>
-      <c r="K100" s="185"/>
+      <c r="C100" s="227"/>
+      <c r="D100" s="228"/>
+      <c r="E100" s="228"/>
+      <c r="F100" s="228"/>
+      <c r="G100" s="228"/>
+      <c r="H100" s="228"/>
+      <c r="I100" s="228"/>
+      <c r="J100" s="228"/>
+      <c r="K100" s="229"/>
       <c r="L100" s="135"/>
       <c r="M100" s="136"/>
       <c r="N100" s="137"/>

</xml_diff>

<commit_message>
Updates to project status and TOC.
</commit_message>
<xml_diff>
--- a/project_management/E2E-Deliverables-Completion-Timeline.xlsx
+++ b/project_management/E2E-Deliverables-Completion-Timeline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39660" yWindow="460" windowWidth="35260" windowHeight="22260" tabRatio="500"/>
+    <workbookView xWindow="3140" yWindow="460" windowWidth="35260" windowHeight="22220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Current Plan 2015-16" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="90">
   <si>
     <t>MVA goes mobile and gets religion</t>
   </si>
@@ -1140,7 +1140,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1720,9 +1720,6 @@
     </xf>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2502,10 +2499,10 @@
   <dimension ref="A1:AB149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2597,37 +2594,37 @@
       <c r="C3" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="225" t="s">
+      <c r="D3" s="224" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="225"/>
-      <c r="F3" s="225"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="224" t="s">
+      <c r="E3" s="224"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="223" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="225"/>
-      <c r="J3" s="225"/>
-      <c r="K3" s="225"/>
-      <c r="L3" s="226"/>
-      <c r="M3" s="224" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="224"/>
+      <c r="K3" s="224"/>
+      <c r="L3" s="225"/>
+      <c r="M3" s="223" t="s">
         <v>39</v>
       </c>
-      <c r="N3" s="225"/>
-      <c r="O3" s="225"/>
-      <c r="P3" s="226"/>
-      <c r="Q3" s="224" t="s">
+      <c r="N3" s="224"/>
+      <c r="O3" s="224"/>
+      <c r="P3" s="225"/>
+      <c r="Q3" s="223" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="225"/>
-      <c r="S3" s="225"/>
-      <c r="T3" s="226"/>
-      <c r="U3" s="224" t="s">
+      <c r="R3" s="224"/>
+      <c r="S3" s="224"/>
+      <c r="T3" s="225"/>
+      <c r="U3" s="223" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="225"/>
-      <c r="W3" s="225"/>
-      <c r="X3" s="226"/>
+      <c r="V3" s="224"/>
+      <c r="W3" s="224"/>
+      <c r="X3" s="225"/>
       <c r="Y3" s="51"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51"/>
@@ -2779,27 +2776,27 @@
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="81"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="201"/>
-      <c r="F6" s="201"/>
-      <c r="G6" s="219"/>
-      <c r="H6" s="202"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="209"/>
-      <c r="K6" s="203"/>
-      <c r="L6" s="203"/>
-      <c r="M6" s="202"/>
-      <c r="N6" s="201"/>
-      <c r="O6" s="209"/>
-      <c r="P6" s="203"/>
-      <c r="Q6" s="202"/>
-      <c r="R6" s="201"/>
-      <c r="S6" s="209"/>
-      <c r="T6" s="203"/>
-      <c r="U6" s="202"/>
-      <c r="V6" s="201"/>
-      <c r="W6" s="209"/>
-      <c r="X6" s="203"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="218"/>
+      <c r="H6" s="201"/>
+      <c r="I6" s="200"/>
+      <c r="J6" s="208"/>
+      <c r="K6" s="202"/>
+      <c r="L6" s="202"/>
+      <c r="M6" s="201"/>
+      <c r="N6" s="200"/>
+      <c r="O6" s="208"/>
+      <c r="P6" s="202"/>
+      <c r="Q6" s="201"/>
+      <c r="R6" s="200"/>
+      <c r="S6" s="208"/>
+      <c r="T6" s="202"/>
+      <c r="U6" s="201"/>
+      <c r="V6" s="200"/>
+      <c r="W6" s="208"/>
+      <c r="X6" s="202"/>
     </row>
     <row r="7" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="57" t="s">
@@ -2807,55 +2804,55 @@
       </c>
       <c r="B7" s="40"/>
       <c r="C7" s="82"/>
-      <c r="D7" s="210"/>
-      <c r="E7" s="210"/>
-      <c r="F7" s="210"/>
-      <c r="G7" s="220"/>
-      <c r="H7" s="198"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
+      <c r="G7" s="219"/>
+      <c r="H7" s="197"/>
       <c r="I7" s="190"/>
       <c r="J7" s="190"/>
-      <c r="K7" s="211"/>
-      <c r="L7" s="211"/>
-      <c r="M7" s="198"/>
+      <c r="K7" s="210"/>
+      <c r="L7" s="210"/>
+      <c r="M7" s="197"/>
       <c r="N7" s="190"/>
       <c r="O7" s="190"/>
-      <c r="P7" s="211"/>
-      <c r="Q7" s="198"/>
+      <c r="P7" s="210"/>
+      <c r="Q7" s="197"/>
       <c r="R7" s="190"/>
       <c r="S7" s="190"/>
-      <c r="T7" s="211"/>
-      <c r="U7" s="198"/>
+      <c r="T7" s="210"/>
+      <c r="U7" s="197"/>
       <c r="V7" s="190"/>
       <c r="W7" s="190"/>
-      <c r="X7" s="211"/>
+      <c r="X7" s="210"/>
     </row>
     <row r="8" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="39"/>
       <c r="B8" s="46"/>
       <c r="C8" s="87"/>
-      <c r="D8" s="213"/>
-      <c r="E8" s="213"/>
-      <c r="F8" s="223">
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="222">
         <v>1</v>
       </c>
-      <c r="G8" s="221"/>
+      <c r="G8" s="220"/>
       <c r="H8" s="192"/>
-      <c r="I8" s="212"/>
-      <c r="J8" s="213"/>
-      <c r="K8" s="214"/>
-      <c r="L8" s="214"/>
+      <c r="I8" s="211"/>
+      <c r="J8" s="212"/>
+      <c r="K8" s="213"/>
+      <c r="L8" s="213"/>
       <c r="M8" s="192"/>
-      <c r="N8" s="212"/>
-      <c r="O8" s="213"/>
-      <c r="P8" s="214"/>
+      <c r="N8" s="211"/>
+      <c r="O8" s="212"/>
+      <c r="P8" s="213"/>
       <c r="Q8" s="192"/>
-      <c r="R8" s="212"/>
-      <c r="S8" s="213"/>
-      <c r="T8" s="214"/>
+      <c r="R8" s="211"/>
+      <c r="S8" s="212"/>
+      <c r="T8" s="213"/>
       <c r="U8" s="192"/>
-      <c r="V8" s="212"/>
-      <c r="W8" s="213"/>
-      <c r="X8" s="214"/>
+      <c r="V8" s="211"/>
+      <c r="W8" s="212"/>
+      <c r="X8" s="213"/>
     </row>
     <row r="9" spans="1:28" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
@@ -2863,27 +2860,27 @@
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="81"/>
-      <c r="D9" s="201"/>
-      <c r="E9" s="201"/>
-      <c r="F9" s="201"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="202"/>
-      <c r="I9" s="201"/>
-      <c r="J9" s="209"/>
-      <c r="K9" s="203"/>
-      <c r="L9" s="203"/>
-      <c r="M9" s="202"/>
-      <c r="N9" s="201"/>
-      <c r="O9" s="209"/>
-      <c r="P9" s="203"/>
-      <c r="Q9" s="202"/>
-      <c r="R9" s="201"/>
-      <c r="S9" s="209"/>
-      <c r="T9" s="203"/>
-      <c r="U9" s="202"/>
-      <c r="V9" s="201"/>
-      <c r="W9" s="209"/>
-      <c r="X9" s="203"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="218"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="208"/>
+      <c r="K9" s="202"/>
+      <c r="L9" s="202"/>
+      <c r="M9" s="201"/>
+      <c r="N9" s="200"/>
+      <c r="O9" s="208"/>
+      <c r="P9" s="202"/>
+      <c r="Q9" s="201"/>
+      <c r="R9" s="200"/>
+      <c r="S9" s="208"/>
+      <c r="T9" s="202"/>
+      <c r="U9" s="201"/>
+      <c r="V9" s="200"/>
+      <c r="W9" s="208"/>
+      <c r="X9" s="202"/>
     </row>
     <row r="10" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="57" t="s">
@@ -2891,27 +2888,27 @@
       </c>
       <c r="B10" s="178"/>
       <c r="C10" s="82"/>
-      <c r="D10" s="217"/>
-      <c r="E10" s="216"/>
-      <c r="F10" s="216"/>
-      <c r="G10" s="222"/>
-      <c r="H10" s="215"/>
-      <c r="I10" s="216"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="211"/>
-      <c r="L10" s="211"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="217"/>
-      <c r="O10" s="217"/>
-      <c r="P10" s="211"/>
-      <c r="Q10" s="218"/>
-      <c r="R10" s="217"/>
-      <c r="S10" s="217"/>
-      <c r="T10" s="211"/>
-      <c r="U10" s="218"/>
-      <c r="V10" s="217"/>
-      <c r="W10" s="217"/>
-      <c r="X10" s="211"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="215"/>
+      <c r="F10" s="215"/>
+      <c r="G10" s="221"/>
+      <c r="H10" s="214"/>
+      <c r="I10" s="215"/>
+      <c r="J10" s="216"/>
+      <c r="K10" s="210"/>
+      <c r="L10" s="210"/>
+      <c r="M10" s="217"/>
+      <c r="N10" s="216"/>
+      <c r="O10" s="216"/>
+      <c r="P10" s="210"/>
+      <c r="Q10" s="217"/>
+      <c r="R10" s="216"/>
+      <c r="S10" s="216"/>
+      <c r="T10" s="210"/>
+      <c r="U10" s="217"/>
+      <c r="V10" s="216"/>
+      <c r="W10" s="216"/>
+      <c r="X10" s="210"/>
     </row>
     <row r="11" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="39"/>
@@ -2927,23 +2924,25 @@
       <c r="G11" s="191">
         <v>0.3</v>
       </c>
-      <c r="H11" s="192"/>
+      <c r="H11" s="191">
+        <v>0.45</v>
+      </c>
       <c r="I11" s="193"/>
       <c r="J11" s="190"/>
-      <c r="K11" s="194"/>
-      <c r="L11" s="194"/>
-      <c r="M11" s="192"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
       <c r="N11" s="193"/>
       <c r="O11" s="190"/>
-      <c r="P11" s="194"/>
-      <c r="Q11" s="192"/>
+      <c r="P11" s="190"/>
+      <c r="Q11" s="190"/>
       <c r="R11" s="193"/>
       <c r="S11" s="190"/>
-      <c r="T11" s="194"/>
-      <c r="U11" s="192"/>
+      <c r="T11" s="190"/>
+      <c r="U11" s="190"/>
       <c r="V11" s="193"/>
       <c r="W11" s="190"/>
-      <c r="X11" s="194"/>
+      <c r="X11" s="190"/>
     </row>
     <row r="12" spans="1:28" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="39"/>
@@ -2959,7 +2958,9 @@
       <c r="G12" s="191">
         <v>0.25</v>
       </c>
-      <c r="H12" s="190"/>
+      <c r="H12" s="191">
+        <v>0.45</v>
+      </c>
       <c r="I12" s="193"/>
       <c r="J12" s="190"/>
       <c r="K12" s="190"/>
@@ -3043,27 +3044,27 @@
       </c>
       <c r="B15" s="170"/>
       <c r="C15" s="181"/>
-      <c r="D15" s="195"/>
-      <c r="E15" s="195"/>
-      <c r="F15" s="195"/>
-      <c r="G15" s="195"/>
-      <c r="H15" s="195"/>
-      <c r="I15" s="195"/>
-      <c r="J15" s="195"/>
-      <c r="K15" s="195"/>
-      <c r="L15" s="195"/>
-      <c r="M15" s="195"/>
-      <c r="N15" s="195"/>
-      <c r="O15" s="195"/>
-      <c r="P15" s="195"/>
-      <c r="Q15" s="195"/>
-      <c r="R15" s="195"/>
-      <c r="S15" s="195"/>
-      <c r="T15" s="195"/>
-      <c r="U15" s="195"/>
-      <c r="V15" s="195"/>
-      <c r="W15" s="195"/>
-      <c r="X15" s="195"/>
+      <c r="D15" s="194"/>
+      <c r="E15" s="194"/>
+      <c r="F15" s="194"/>
+      <c r="G15" s="194"/>
+      <c r="H15" s="194"/>
+      <c r="I15" s="194"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="194"/>
+      <c r="L15" s="194"/>
+      <c r="M15" s="194"/>
+      <c r="N15" s="194"/>
+      <c r="O15" s="194"/>
+      <c r="P15" s="194"/>
+      <c r="Q15" s="194"/>
+      <c r="R15" s="194"/>
+      <c r="S15" s="194"/>
+      <c r="T15" s="194"/>
+      <c r="U15" s="194"/>
+      <c r="V15" s="194"/>
+      <c r="W15" s="194"/>
+      <c r="X15" s="194"/>
       <c r="Y15" s="171"/>
       <c r="Z15" s="171"/>
       <c r="AA15" s="171"/>
@@ -3078,11 +3079,11 @@
       <c r="D16" s="190"/>
       <c r="E16" s="190"/>
       <c r="F16" s="190"/>
-      <c r="G16" s="196"/>
-      <c r="H16" s="196"/>
-      <c r="I16" s="196"/>
-      <c r="J16" s="196"/>
-      <c r="K16" s="196"/>
+      <c r="G16" s="195"/>
+      <c r="H16" s="195"/>
+      <c r="I16" s="195"/>
+      <c r="J16" s="195"/>
+      <c r="K16" s="195"/>
       <c r="L16" s="190"/>
       <c r="M16" s="190"/>
       <c r="N16" s="190"/>
@@ -3111,7 +3112,9 @@
       <c r="G17" s="191">
         <v>0.15</v>
       </c>
-      <c r="H17" s="190"/>
+      <c r="H17" s="191">
+        <v>0.15</v>
+      </c>
       <c r="I17" s="193"/>
       <c r="J17" s="190"/>
       <c r="K17" s="190"/>
@@ -3143,7 +3146,9 @@
       <c r="G18" s="191">
         <v>0.15</v>
       </c>
-      <c r="H18" s="190"/>
+      <c r="H18" s="191">
+        <v>0.15</v>
+      </c>
       <c r="I18" s="193"/>
       <c r="J18" s="190"/>
       <c r="K18" s="190"/>
@@ -3168,29 +3173,31 @@
       <c r="C19" s="182" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="197"/>
-      <c r="E19" s="197"/>
-      <c r="F19" s="197"/>
+      <c r="D19" s="196"/>
+      <c r="E19" s="196"/>
+      <c r="F19" s="196"/>
       <c r="G19" s="193">
         <v>0.15</v>
       </c>
-      <c r="H19" s="197"/>
+      <c r="H19" s="193">
+        <v>0.15</v>
+      </c>
       <c r="I19" s="193"/>
       <c r="J19" s="193"/>
-      <c r="K19" s="197"/>
-      <c r="L19" s="197"/>
-      <c r="M19" s="197"/>
+      <c r="K19" s="196"/>
+      <c r="L19" s="196"/>
+      <c r="M19" s="196"/>
       <c r="N19" s="193"/>
       <c r="O19" s="193"/>
-      <c r="P19" s="197"/>
-      <c r="Q19" s="197"/>
+      <c r="P19" s="196"/>
+      <c r="Q19" s="196"/>
       <c r="R19" s="193"/>
       <c r="S19" s="193"/>
-      <c r="T19" s="197"/>
-      <c r="U19" s="197"/>
+      <c r="T19" s="196"/>
+      <c r="U19" s="196"/>
       <c r="V19" s="193"/>
       <c r="W19" s="193"/>
-      <c r="X19" s="197"/>
+      <c r="X19" s="196"/>
     </row>
     <row r="20" spans="1:27" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
@@ -3200,55 +3207,57 @@
       <c r="C20" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="197"/>
-      <c r="E20" s="197"/>
-      <c r="F20" s="197"/>
-      <c r="G20" s="199">
+      <c r="D20" s="196"/>
+      <c r="E20" s="196"/>
+      <c r="F20" s="196"/>
+      <c r="G20" s="198">
         <v>0.2</v>
       </c>
-      <c r="H20" s="197"/>
+      <c r="H20" s="193">
+        <v>0.2</v>
+      </c>
       <c r="I20" s="193"/>
-      <c r="J20" s="197"/>
-      <c r="K20" s="197"/>
-      <c r="L20" s="197"/>
-      <c r="M20" s="197"/>
+      <c r="J20" s="196"/>
+      <c r="K20" s="196"/>
+      <c r="L20" s="196"/>
+      <c r="M20" s="196"/>
       <c r="N20" s="193"/>
-      <c r="O20" s="197"/>
-      <c r="P20" s="197"/>
-      <c r="Q20" s="197"/>
+      <c r="O20" s="196"/>
+      <c r="P20" s="196"/>
+      <c r="Q20" s="196"/>
       <c r="R20" s="193"/>
-      <c r="S20" s="197"/>
-      <c r="T20" s="197"/>
-      <c r="U20" s="197"/>
+      <c r="S20" s="196"/>
+      <c r="T20" s="196"/>
+      <c r="U20" s="196"/>
       <c r="V20" s="193"/>
-      <c r="W20" s="197"/>
-      <c r="X20" s="197"/>
+      <c r="W20" s="196"/>
+      <c r="X20" s="196"/>
     </row>
     <row r="21" spans="1:27" s="50" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="172"/>
       <c r="C21" s="182"/>
-      <c r="D21" s="197"/>
-      <c r="E21" s="197"/>
-      <c r="F21" s="197"/>
-      <c r="G21" s="200"/>
-      <c r="H21" s="197"/>
+      <c r="D21" s="196"/>
+      <c r="E21" s="196"/>
+      <c r="F21" s="196"/>
+      <c r="G21" s="199"/>
+      <c r="H21" s="196"/>
       <c r="I21" s="193"/>
-      <c r="J21" s="197"/>
-      <c r="K21" s="197"/>
-      <c r="L21" s="197"/>
-      <c r="M21" s="197"/>
+      <c r="J21" s="196"/>
+      <c r="K21" s="196"/>
+      <c r="L21" s="196"/>
+      <c r="M21" s="196"/>
       <c r="N21" s="193"/>
-      <c r="O21" s="197"/>
-      <c r="P21" s="197"/>
-      <c r="Q21" s="197"/>
+      <c r="O21" s="196"/>
+      <c r="P21" s="196"/>
+      <c r="Q21" s="196"/>
       <c r="R21" s="193"/>
-      <c r="S21" s="197"/>
-      <c r="T21" s="197"/>
-      <c r="U21" s="197"/>
+      <c r="S21" s="196"/>
+      <c r="T21" s="196"/>
+      <c r="U21" s="196"/>
       <c r="V21" s="193"/>
-      <c r="W21" s="197"/>
-      <c r="X21" s="197"/>
+      <c r="W21" s="196"/>
+      <c r="X21" s="196"/>
     </row>
     <row r="22" spans="1:27" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="16" t="s">
@@ -3256,27 +3265,27 @@
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="183"/>
-      <c r="D22" s="201"/>
-      <c r="E22" s="201"/>
-      <c r="F22" s="201"/>
-      <c r="G22" s="201"/>
-      <c r="H22" s="201"/>
-      <c r="I22" s="201"/>
-      <c r="J22" s="201"/>
-      <c r="K22" s="201"/>
-      <c r="L22" s="201"/>
-      <c r="M22" s="201"/>
-      <c r="N22" s="201"/>
-      <c r="O22" s="201"/>
-      <c r="P22" s="201"/>
-      <c r="Q22" s="201"/>
-      <c r="R22" s="201"/>
-      <c r="S22" s="201"/>
-      <c r="T22" s="201"/>
-      <c r="U22" s="201"/>
-      <c r="V22" s="201"/>
-      <c r="W22" s="201"/>
-      <c r="X22" s="201"/>
+      <c r="D22" s="200"/>
+      <c r="E22" s="200"/>
+      <c r="F22" s="200"/>
+      <c r="G22" s="200"/>
+      <c r="H22" s="200"/>
+      <c r="I22" s="200"/>
+      <c r="J22" s="200"/>
+      <c r="K22" s="200"/>
+      <c r="L22" s="200"/>
+      <c r="M22" s="200"/>
+      <c r="N22" s="200"/>
+      <c r="O22" s="200"/>
+      <c r="P22" s="200"/>
+      <c r="Q22" s="200"/>
+      <c r="R22" s="200"/>
+      <c r="S22" s="200"/>
+      <c r="T22" s="200"/>
+      <c r="U22" s="200"/>
+      <c r="V22" s="200"/>
+      <c r="W22" s="200"/>
+      <c r="X22" s="200"/>
     </row>
     <row r="23" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="57" t="s">
@@ -3288,20 +3297,20 @@
       <c r="E23" s="190"/>
       <c r="F23" s="190"/>
       <c r="G23" s="190"/>
-      <c r="H23" s="197"/>
+      <c r="H23" s="196"/>
       <c r="I23" s="190"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="196"/>
-      <c r="L23" s="196"/>
-      <c r="M23" s="196"/>
-      <c r="N23" s="196"/>
-      <c r="O23" s="204"/>
-      <c r="P23" s="204"/>
-      <c r="Q23" s="204"/>
+      <c r="J23" s="195"/>
+      <c r="K23" s="195"/>
+      <c r="L23" s="195"/>
+      <c r="M23" s="195"/>
+      <c r="N23" s="195"/>
+      <c r="O23" s="203"/>
+      <c r="P23" s="203"/>
+      <c r="Q23" s="203"/>
       <c r="R23" s="190"/>
       <c r="S23" s="190"/>
       <c r="T23" s="190"/>
-      <c r="U23" s="204"/>
+      <c r="U23" s="203"/>
       <c r="V23" s="190"/>
       <c r="W23" s="190"/>
       <c r="X23" s="190"/>
@@ -3320,20 +3329,22 @@
       <c r="G24" s="191">
         <v>0</v>
       </c>
-      <c r="H24" s="197"/>
+      <c r="H24" s="193">
+        <v>0</v>
+      </c>
       <c r="I24" s="190"/>
       <c r="J24" s="190"/>
       <c r="K24" s="190"/>
       <c r="L24" s="190"/>
       <c r="M24" s="190"/>
       <c r="N24" s="190"/>
-      <c r="O24" s="204"/>
-      <c r="P24" s="204"/>
-      <c r="Q24" s="204"/>
+      <c r="O24" s="203"/>
+      <c r="P24" s="203"/>
+      <c r="Q24" s="203"/>
       <c r="R24" s="190"/>
       <c r="S24" s="190"/>
       <c r="T24" s="190"/>
-      <c r="U24" s="204"/>
+      <c r="U24" s="203"/>
       <c r="V24" s="190"/>
       <c r="W24" s="190"/>
       <c r="X24" s="190"/>
@@ -3352,7 +3363,9 @@
       <c r="G25" s="191">
         <v>0.25</v>
       </c>
-      <c r="H25" s="190"/>
+      <c r="H25" s="191">
+        <v>0.25</v>
+      </c>
       <c r="I25" s="193"/>
       <c r="J25" s="190"/>
       <c r="K25" s="190"/>
@@ -3384,7 +3397,9 @@
       <c r="G26" s="191">
         <v>0.25</v>
       </c>
-      <c r="H26" s="190"/>
+      <c r="H26" s="191">
+        <v>0.25</v>
+      </c>
       <c r="I26" s="193"/>
       <c r="J26" s="190"/>
       <c r="K26" s="190"/>
@@ -3410,29 +3425,31 @@
       <c r="C27" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="197"/>
-      <c r="E27" s="197"/>
-      <c r="F27" s="197"/>
+      <c r="D27" s="196"/>
+      <c r="E27" s="196"/>
+      <c r="F27" s="196"/>
       <c r="G27" s="193">
         <v>0</v>
       </c>
-      <c r="H27" s="193"/>
-      <c r="I27" s="197"/>
-      <c r="J27" s="197"/>
-      <c r="K27" s="197"/>
-      <c r="L27" s="197"/>
+      <c r="H27" s="193">
+        <v>0</v>
+      </c>
+      <c r="I27" s="196"/>
+      <c r="J27" s="196"/>
+      <c r="K27" s="196"/>
+      <c r="L27" s="196"/>
       <c r="M27" s="193"/>
-      <c r="N27" s="197"/>
-      <c r="O27" s="197"/>
-      <c r="P27" s="197"/>
+      <c r="N27" s="196"/>
+      <c r="O27" s="196"/>
+      <c r="P27" s="196"/>
       <c r="Q27" s="193"/>
-      <c r="R27" s="197"/>
-      <c r="S27" s="197"/>
-      <c r="T27" s="197"/>
+      <c r="R27" s="196"/>
+      <c r="S27" s="196"/>
+      <c r="T27" s="196"/>
       <c r="U27" s="193"/>
-      <c r="V27" s="197"/>
-      <c r="W27" s="197"/>
-      <c r="X27" s="207"/>
+      <c r="V27" s="196"/>
+      <c r="W27" s="196"/>
+      <c r="X27" s="206"/>
       <c r="Y27" s="176"/>
       <c r="Z27" s="176"/>
       <c r="AA27" s="176"/>
@@ -3451,7 +3468,9 @@
       <c r="G28" s="190" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="190"/>
+      <c r="H28" s="190" t="s">
+        <v>85</v>
+      </c>
       <c r="I28" s="193"/>
       <c r="J28" s="190"/>
       <c r="K28" s="190"/>
@@ -3473,27 +3492,27 @@
       <c r="A29" s="2"/>
       <c r="B29" s="20"/>
       <c r="C29" s="182"/>
-      <c r="D29" s="197"/>
-      <c r="E29" s="197"/>
-      <c r="F29" s="197"/>
-      <c r="G29" s="200"/>
-      <c r="H29" s="197"/>
+      <c r="D29" s="196"/>
+      <c r="E29" s="196"/>
+      <c r="F29" s="196"/>
+      <c r="G29" s="199"/>
+      <c r="H29" s="196"/>
       <c r="I29" s="193"/>
-      <c r="J29" s="197"/>
-      <c r="K29" s="197"/>
-      <c r="L29" s="197"/>
-      <c r="M29" s="197"/>
+      <c r="J29" s="196"/>
+      <c r="K29" s="196"/>
+      <c r="L29" s="196"/>
+      <c r="M29" s="196"/>
       <c r="N29" s="193"/>
-      <c r="O29" s="197"/>
-      <c r="P29" s="197"/>
-      <c r="Q29" s="197"/>
+      <c r="O29" s="196"/>
+      <c r="P29" s="196"/>
+      <c r="Q29" s="196"/>
       <c r="R29" s="193"/>
-      <c r="S29" s="197"/>
-      <c r="T29" s="197"/>
-      <c r="U29" s="197"/>
+      <c r="S29" s="196"/>
+      <c r="T29" s="196"/>
+      <c r="U29" s="196"/>
       <c r="V29" s="193"/>
-      <c r="W29" s="197"/>
-      <c r="X29" s="197"/>
+      <c r="W29" s="196"/>
+      <c r="X29" s="196"/>
     </row>
     <row r="30" spans="1:27" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
@@ -3501,27 +3520,27 @@
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="183"/>
-      <c r="D30" s="201"/>
-      <c r="E30" s="201"/>
-      <c r="F30" s="201"/>
-      <c r="G30" s="201"/>
-      <c r="H30" s="201"/>
-      <c r="I30" s="201"/>
-      <c r="J30" s="201"/>
-      <c r="K30" s="201"/>
-      <c r="L30" s="201"/>
-      <c r="M30" s="201"/>
-      <c r="N30" s="201"/>
-      <c r="O30" s="201"/>
-      <c r="P30" s="201"/>
-      <c r="Q30" s="201"/>
-      <c r="R30" s="201"/>
-      <c r="S30" s="201"/>
-      <c r="T30" s="201"/>
-      <c r="U30" s="201"/>
-      <c r="V30" s="201"/>
-      <c r="W30" s="201"/>
-      <c r="X30" s="201"/>
+      <c r="D30" s="200"/>
+      <c r="E30" s="200"/>
+      <c r="F30" s="200"/>
+      <c r="G30" s="200"/>
+      <c r="H30" s="200"/>
+      <c r="I30" s="200"/>
+      <c r="J30" s="200"/>
+      <c r="K30" s="200"/>
+      <c r="L30" s="200"/>
+      <c r="M30" s="200"/>
+      <c r="N30" s="200"/>
+      <c r="O30" s="200"/>
+      <c r="P30" s="200"/>
+      <c r="Q30" s="200"/>
+      <c r="R30" s="200"/>
+      <c r="S30" s="200"/>
+      <c r="T30" s="200"/>
+      <c r="U30" s="200"/>
+      <c r="V30" s="200"/>
+      <c r="W30" s="200"/>
+      <c r="X30" s="200"/>
     </row>
     <row r="31" spans="1:27" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="57" t="s">
@@ -3533,20 +3552,20 @@
       <c r="E31" s="190"/>
       <c r="F31" s="190"/>
       <c r="G31" s="190"/>
-      <c r="H31" s="197"/>
+      <c r="H31" s="196"/>
       <c r="I31" s="190"/>
-      <c r="J31" s="204"/>
-      <c r="K31" s="204"/>
-      <c r="L31" s="204"/>
-      <c r="M31" s="197"/>
+      <c r="J31" s="203"/>
+      <c r="K31" s="203"/>
+      <c r="L31" s="203"/>
+      <c r="M31" s="196"/>
       <c r="N31" s="190"/>
       <c r="O31" s="190"/>
       <c r="P31" s="190"/>
-      <c r="Q31" s="197"/>
+      <c r="Q31" s="196"/>
       <c r="R31" s="190"/>
       <c r="S31" s="190"/>
       <c r="T31" s="190"/>
-      <c r="U31" s="197"/>
+      <c r="U31" s="196"/>
       <c r="V31" s="190"/>
       <c r="W31" s="190"/>
       <c r="X31" s="190"/>
@@ -3560,9 +3579,9 @@
       <c r="D32" s="190"/>
       <c r="E32" s="190"/>
       <c r="F32" s="190"/>
-      <c r="G32" s="208"/>
-      <c r="H32" s="208"/>
-      <c r="I32" s="196"/>
+      <c r="G32" s="207"/>
+      <c r="H32" s="207"/>
+      <c r="I32" s="195"/>
       <c r="J32" s="190"/>
       <c r="K32" s="190"/>
       <c r="L32" s="190"/>
@@ -3588,10 +3607,10 @@
       <c r="D33" s="190"/>
       <c r="E33" s="190"/>
       <c r="F33" s="190"/>
-      <c r="G33" s="208"/>
-      <c r="H33" s="208"/>
+      <c r="G33" s="207"/>
+      <c r="H33" s="207"/>
       <c r="I33" s="190"/>
-      <c r="J33" s="196"/>
+      <c r="J33" s="195"/>
       <c r="K33" s="190"/>
       <c r="L33" s="190"/>
       <c r="M33" s="190"/>
@@ -3617,11 +3636,11 @@
       <c r="E34" s="190"/>
       <c r="F34" s="190"/>
       <c r="G34" s="190"/>
-      <c r="H34" s="208"/>
+      <c r="H34" s="207"/>
       <c r="I34" s="190"/>
-      <c r="J34" s="208"/>
-      <c r="K34" s="205"/>
-      <c r="L34" s="196"/>
+      <c r="J34" s="207"/>
+      <c r="K34" s="204"/>
+      <c r="L34" s="195"/>
       <c r="M34" s="190"/>
       <c r="N34" s="193"/>
       <c r="O34" s="190"/>
@@ -3648,10 +3667,10 @@
       <c r="H35" s="190"/>
       <c r="I35" s="193"/>
       <c r="J35" s="190"/>
-      <c r="K35" s="208"/>
-      <c r="L35" s="208"/>
-      <c r="M35" s="196"/>
-      <c r="N35" s="196"/>
+      <c r="K35" s="207"/>
+      <c r="L35" s="207"/>
+      <c r="M35" s="195"/>
+      <c r="N35" s="195"/>
       <c r="O35" s="190"/>
       <c r="P35" s="190"/>
       <c r="Q35" s="190"/>
@@ -3695,27 +3714,27 @@
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="183"/>
-      <c r="D37" s="201"/>
-      <c r="E37" s="201"/>
-      <c r="F37" s="201"/>
-      <c r="G37" s="201"/>
-      <c r="H37" s="201"/>
-      <c r="I37" s="201"/>
-      <c r="J37" s="201"/>
-      <c r="K37" s="201"/>
-      <c r="L37" s="201"/>
-      <c r="M37" s="201"/>
-      <c r="N37" s="201"/>
-      <c r="O37" s="201"/>
-      <c r="P37" s="201"/>
-      <c r="Q37" s="201"/>
-      <c r="R37" s="201"/>
-      <c r="S37" s="201"/>
-      <c r="T37" s="201"/>
-      <c r="U37" s="201"/>
-      <c r="V37" s="201"/>
-      <c r="W37" s="201"/>
-      <c r="X37" s="201"/>
+      <c r="D37" s="200"/>
+      <c r="E37" s="200"/>
+      <c r="F37" s="200"/>
+      <c r="G37" s="200"/>
+      <c r="H37" s="200"/>
+      <c r="I37" s="200"/>
+      <c r="J37" s="200"/>
+      <c r="K37" s="200"/>
+      <c r="L37" s="200"/>
+      <c r="M37" s="200"/>
+      <c r="N37" s="200"/>
+      <c r="O37" s="200"/>
+      <c r="P37" s="200"/>
+      <c r="Q37" s="200"/>
+      <c r="R37" s="200"/>
+      <c r="S37" s="200"/>
+      <c r="T37" s="200"/>
+      <c r="U37" s="200"/>
+      <c r="V37" s="200"/>
+      <c r="W37" s="200"/>
+      <c r="X37" s="200"/>
     </row>
     <row r="38" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="57" t="s">
@@ -3727,20 +3746,20 @@
       <c r="E38" s="190"/>
       <c r="F38" s="190"/>
       <c r="G38" s="190"/>
-      <c r="H38" s="197"/>
+      <c r="H38" s="196"/>
       <c r="I38" s="190"/>
       <c r="J38" s="190"/>
       <c r="K38" s="190"/>
       <c r="L38" s="190"/>
-      <c r="M38" s="197"/>
+      <c r="M38" s="196"/>
       <c r="N38" s="190"/>
       <c r="O38" s="190"/>
       <c r="P38" s="190"/>
-      <c r="Q38" s="197"/>
+      <c r="Q38" s="196"/>
       <c r="R38" s="190"/>
       <c r="S38" s="190"/>
       <c r="T38" s="190"/>
-      <c r="U38" s="197"/>
+      <c r="U38" s="196"/>
       <c r="V38" s="190"/>
       <c r="W38" s="190"/>
       <c r="X38" s="190"/>
@@ -3751,11 +3770,11 @@
         <v>17</v>
       </c>
       <c r="C39" s="180"/>
-      <c r="D39" s="196"/>
-      <c r="E39" s="196"/>
-      <c r="F39" s="196"/>
-      <c r="G39" s="196"/>
-      <c r="H39" s="196"/>
+      <c r="D39" s="195"/>
+      <c r="E39" s="195"/>
+      <c r="F39" s="195"/>
+      <c r="G39" s="195"/>
+      <c r="H39" s="195"/>
       <c r="I39" s="193"/>
       <c r="J39" s="190"/>
       <c r="K39" s="190"/>
@@ -3784,10 +3803,10 @@
       <c r="F40" s="190"/>
       <c r="G40" s="190"/>
       <c r="H40" s="190"/>
-      <c r="I40" s="205"/>
-      <c r="J40" s="196"/>
-      <c r="K40" s="196"/>
-      <c r="L40" s="196"/>
+      <c r="I40" s="204"/>
+      <c r="J40" s="195"/>
+      <c r="K40" s="195"/>
+      <c r="L40" s="195"/>
       <c r="M40" s="190"/>
       <c r="N40" s="193"/>
       <c r="O40" s="190"/>
@@ -3814,9 +3833,9 @@
       <c r="H41" s="190"/>
       <c r="I41" s="193"/>
       <c r="J41" s="190"/>
-      <c r="K41" s="205"/>
-      <c r="L41" s="205"/>
-      <c r="M41" s="196"/>
+      <c r="K41" s="204"/>
+      <c r="L41" s="204"/>
+      <c r="M41" s="195"/>
       <c r="N41" s="190"/>
       <c r="O41" s="190"/>
       <c r="P41" s="190"/>
@@ -3844,8 +3863,8 @@
       <c r="J42" s="190"/>
       <c r="K42" s="193"/>
       <c r="L42" s="193"/>
-      <c r="M42" s="196"/>
-      <c r="N42" s="196"/>
+      <c r="M42" s="195"/>
+      <c r="N42" s="195"/>
       <c r="O42" s="190"/>
       <c r="P42" s="190"/>
       <c r="Q42" s="190"/>
@@ -3863,18 +3882,18 @@
         <v>21</v>
       </c>
       <c r="C43" s="182"/>
-      <c r="D43" s="197"/>
-      <c r="E43" s="197"/>
-      <c r="F43" s="197"/>
-      <c r="G43" s="197"/>
-      <c r="H43" s="197"/>
+      <c r="D43" s="196"/>
+      <c r="E43" s="196"/>
+      <c r="F43" s="196"/>
+      <c r="G43" s="196"/>
+      <c r="H43" s="196"/>
       <c r="I43" s="193"/>
       <c r="J43" s="193"/>
       <c r="K43" s="193"/>
       <c r="L43" s="193"/>
       <c r="M43" s="193"/>
-      <c r="N43" s="205"/>
-      <c r="O43" s="196"/>
+      <c r="N43" s="204"/>
+      <c r="O43" s="195"/>
       <c r="P43" s="190"/>
       <c r="Q43" s="190"/>
       <c r="R43" s="193"/>
@@ -3917,27 +3936,27 @@
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="183"/>
-      <c r="D45" s="201"/>
-      <c r="E45" s="201"/>
-      <c r="F45" s="201"/>
-      <c r="G45" s="201"/>
-      <c r="H45" s="201"/>
-      <c r="I45" s="201"/>
-      <c r="J45" s="201"/>
-      <c r="K45" s="201"/>
-      <c r="L45" s="201"/>
-      <c r="M45" s="201"/>
-      <c r="N45" s="201"/>
-      <c r="O45" s="201"/>
-      <c r="P45" s="201"/>
-      <c r="Q45" s="201"/>
-      <c r="R45" s="201"/>
-      <c r="S45" s="201"/>
-      <c r="T45" s="201"/>
-      <c r="U45" s="201"/>
-      <c r="V45" s="201"/>
-      <c r="W45" s="201"/>
-      <c r="X45" s="201"/>
+      <c r="D45" s="200"/>
+      <c r="E45" s="200"/>
+      <c r="F45" s="200"/>
+      <c r="G45" s="200"/>
+      <c r="H45" s="200"/>
+      <c r="I45" s="200"/>
+      <c r="J45" s="200"/>
+      <c r="K45" s="200"/>
+      <c r="L45" s="200"/>
+      <c r="M45" s="200"/>
+      <c r="N45" s="200"/>
+      <c r="O45" s="200"/>
+      <c r="P45" s="200"/>
+      <c r="Q45" s="200"/>
+      <c r="R45" s="200"/>
+      <c r="S45" s="200"/>
+      <c r="T45" s="200"/>
+      <c r="U45" s="200"/>
+      <c r="V45" s="200"/>
+      <c r="W45" s="200"/>
+      <c r="X45" s="200"/>
     </row>
     <row r="46" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="57" t="s">
@@ -3949,20 +3968,20 @@
       <c r="E46" s="190"/>
       <c r="F46" s="190"/>
       <c r="G46" s="190"/>
-      <c r="H46" s="197"/>
+      <c r="H46" s="196"/>
       <c r="I46" s="190"/>
       <c r="J46" s="190"/>
       <c r="K46" s="190"/>
       <c r="L46" s="190"/>
-      <c r="M46" s="197"/>
+      <c r="M46" s="196"/>
       <c r="N46" s="190"/>
       <c r="O46" s="190"/>
-      <c r="P46" s="196"/>
-      <c r="Q46" s="197"/>
+      <c r="P46" s="195"/>
+      <c r="Q46" s="196"/>
       <c r="R46" s="190"/>
       <c r="S46" s="190"/>
       <c r="T46" s="190"/>
-      <c r="U46" s="197"/>
+      <c r="U46" s="196"/>
       <c r="V46" s="190"/>
       <c r="W46" s="190"/>
       <c r="X46" s="190"/>
@@ -3985,7 +4004,7 @@
       <c r="M47" s="190"/>
       <c r="N47" s="193"/>
       <c r="O47" s="190"/>
-      <c r="P47" s="196"/>
+      <c r="P47" s="195"/>
       <c r="Q47" s="190"/>
       <c r="R47" s="193"/>
       <c r="S47" s="190"/>
@@ -4013,7 +4032,7 @@
       <c r="M48" s="190"/>
       <c r="N48" s="193"/>
       <c r="O48" s="190"/>
-      <c r="P48" s="196"/>
+      <c r="P48" s="195"/>
       <c r="Q48" s="190"/>
       <c r="R48" s="193"/>
       <c r="S48" s="190"/>
@@ -4041,7 +4060,7 @@
       <c r="M49" s="190"/>
       <c r="N49" s="193"/>
       <c r="O49" s="190"/>
-      <c r="P49" s="196"/>
+      <c r="P49" s="195"/>
       <c r="Q49" s="190"/>
       <c r="R49" s="193"/>
       <c r="S49" s="190"/>
@@ -4070,7 +4089,7 @@
       <c r="N50" s="193"/>
       <c r="O50" s="190"/>
       <c r="P50" s="190"/>
-      <c r="Q50" s="196"/>
+      <c r="Q50" s="195"/>
       <c r="R50" s="193"/>
       <c r="S50" s="190"/>
       <c r="T50" s="190"/>
@@ -4085,24 +4104,24 @@
         <v>30</v>
       </c>
       <c r="C51" s="182"/>
-      <c r="D51" s="197"/>
-      <c r="E51" s="197"/>
-      <c r="F51" s="197"/>
-      <c r="G51" s="197"/>
-      <c r="H51" s="197"/>
+      <c r="D51" s="196"/>
+      <c r="E51" s="196"/>
+      <c r="F51" s="196"/>
+      <c r="G51" s="196"/>
+      <c r="H51" s="196"/>
       <c r="I51" s="193"/>
       <c r="J51" s="193"/>
       <c r="K51" s="193"/>
       <c r="L51" s="193"/>
-      <c r="M51" s="197"/>
+      <c r="M51" s="196"/>
       <c r="N51" s="193"/>
       <c r="O51" s="193"/>
       <c r="P51" s="193"/>
-      <c r="Q51" s="196"/>
+      <c r="Q51" s="195"/>
       <c r="R51" s="193"/>
       <c r="S51" s="193"/>
       <c r="T51" s="193"/>
-      <c r="U51" s="197"/>
+      <c r="U51" s="196"/>
       <c r="V51" s="193"/>
       <c r="W51" s="193"/>
       <c r="X51" s="193"/>
@@ -4113,24 +4132,24 @@
         <v>28</v>
       </c>
       <c r="C52" s="182"/>
-      <c r="D52" s="197"/>
-      <c r="E52" s="197"/>
-      <c r="F52" s="197"/>
-      <c r="G52" s="197"/>
-      <c r="H52" s="197"/>
+      <c r="D52" s="196"/>
+      <c r="E52" s="196"/>
+      <c r="F52" s="196"/>
+      <c r="G52" s="196"/>
+      <c r="H52" s="196"/>
       <c r="I52" s="193"/>
       <c r="J52" s="193"/>
       <c r="K52" s="193"/>
       <c r="L52" s="193"/>
-      <c r="M52" s="197"/>
+      <c r="M52" s="196"/>
       <c r="N52" s="193"/>
       <c r="O52" s="193"/>
       <c r="P52" s="193"/>
-      <c r="Q52" s="196"/>
+      <c r="Q52" s="195"/>
       <c r="R52" s="193"/>
       <c r="S52" s="193"/>
       <c r="T52" s="193"/>
-      <c r="U52" s="197"/>
+      <c r="U52" s="196"/>
       <c r="V52" s="193"/>
       <c r="W52" s="193"/>
       <c r="X52" s="193"/>
@@ -4141,24 +4160,24 @@
         <v>29</v>
       </c>
       <c r="C53" s="182"/>
-      <c r="D53" s="197"/>
-      <c r="E53" s="197"/>
-      <c r="F53" s="197"/>
-      <c r="G53" s="197"/>
-      <c r="H53" s="197"/>
+      <c r="D53" s="196"/>
+      <c r="E53" s="196"/>
+      <c r="F53" s="196"/>
+      <c r="G53" s="196"/>
+      <c r="H53" s="196"/>
       <c r="I53" s="193"/>
       <c r="J53" s="193"/>
       <c r="K53" s="193"/>
       <c r="L53" s="193"/>
-      <c r="M53" s="197"/>
+      <c r="M53" s="196"/>
       <c r="N53" s="193"/>
       <c r="O53" s="193"/>
       <c r="P53" s="193"/>
-      <c r="Q53" s="196"/>
+      <c r="Q53" s="195"/>
       <c r="R53" s="193"/>
       <c r="S53" s="193"/>
       <c r="T53" s="193"/>
-      <c r="U53" s="197"/>
+      <c r="U53" s="196"/>
       <c r="V53" s="193"/>
       <c r="W53" s="193"/>
       <c r="X53" s="193"/>
@@ -4169,77 +4188,77 @@
         <v>31</v>
       </c>
       <c r="C54" s="182"/>
-      <c r="D54" s="197"/>
-      <c r="E54" s="197"/>
-      <c r="F54" s="197"/>
-      <c r="G54" s="197"/>
-      <c r="H54" s="197"/>
+      <c r="D54" s="196"/>
+      <c r="E54" s="196"/>
+      <c r="F54" s="196"/>
+      <c r="G54" s="196"/>
+      <c r="H54" s="196"/>
       <c r="I54" s="193"/>
       <c r="J54" s="193"/>
-      <c r="K54" s="197"/>
-      <c r="L54" s="197"/>
-      <c r="M54" s="197"/>
+      <c r="K54" s="196"/>
+      <c r="L54" s="196"/>
+      <c r="M54" s="196"/>
       <c r="N54" s="193"/>
       <c r="O54" s="193"/>
-      <c r="P54" s="197"/>
-      <c r="Q54" s="196"/>
+      <c r="P54" s="196"/>
+      <c r="Q54" s="195"/>
       <c r="R54" s="193"/>
       <c r="S54" s="193"/>
-      <c r="T54" s="197"/>
-      <c r="U54" s="197"/>
+      <c r="T54" s="196"/>
+      <c r="U54" s="196"/>
       <c r="V54" s="193"/>
       <c r="W54" s="193"/>
-      <c r="X54" s="197"/>
+      <c r="X54" s="196"/>
     </row>
     <row r="55" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="36"/>
       <c r="C55" s="182"/>
-      <c r="D55" s="197"/>
-      <c r="E55" s="197"/>
-      <c r="F55" s="197"/>
-      <c r="G55" s="197"/>
-      <c r="H55" s="197"/>
+      <c r="D55" s="196"/>
+      <c r="E55" s="196"/>
+      <c r="F55" s="196"/>
+      <c r="G55" s="196"/>
+      <c r="H55" s="196"/>
       <c r="I55" s="193"/>
-      <c r="J55" s="197"/>
-      <c r="K55" s="197"/>
-      <c r="L55" s="197"/>
-      <c r="M55" s="197"/>
+      <c r="J55" s="196"/>
+      <c r="K55" s="196"/>
+      <c r="L55" s="196"/>
+      <c r="M55" s="196"/>
       <c r="N55" s="193"/>
-      <c r="O55" s="197"/>
-      <c r="P55" s="197"/>
-      <c r="Q55" s="197"/>
+      <c r="O55" s="196"/>
+      <c r="P55" s="196"/>
+      <c r="Q55" s="196"/>
       <c r="R55" s="193"/>
-      <c r="S55" s="197"/>
-      <c r="T55" s="197"/>
-      <c r="U55" s="197"/>
+      <c r="S55" s="196"/>
+      <c r="T55" s="196"/>
+      <c r="U55" s="196"/>
       <c r="V55" s="193"/>
-      <c r="W55" s="197"/>
-      <c r="X55" s="197"/>
+      <c r="W55" s="196"/>
+      <c r="X55" s="196"/>
     </row>
     <row r="56" spans="1:24" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="5"/>
       <c r="C56" s="186"/>
-      <c r="D56" s="197"/>
-      <c r="E56" s="197"/>
-      <c r="F56" s="197"/>
-      <c r="G56" s="197"/>
-      <c r="H56" s="197"/>
-      <c r="I56" s="197"/>
-      <c r="J56" s="197"/>
-      <c r="K56" s="197"/>
-      <c r="L56" s="197"/>
-      <c r="M56" s="197"/>
-      <c r="N56" s="197"/>
-      <c r="O56" s="197"/>
-      <c r="P56" s="197"/>
-      <c r="Q56" s="197"/>
-      <c r="R56" s="197"/>
-      <c r="S56" s="197"/>
-      <c r="T56" s="197"/>
-      <c r="U56" s="197"/>
-      <c r="V56" s="197"/>
-      <c r="W56" s="197"/>
-      <c r="X56" s="197"/>
+      <c r="D56" s="196"/>
+      <c r="E56" s="196"/>
+      <c r="F56" s="196"/>
+      <c r="G56" s="196"/>
+      <c r="H56" s="196"/>
+      <c r="I56" s="196"/>
+      <c r="J56" s="196"/>
+      <c r="K56" s="196"/>
+      <c r="L56" s="196"/>
+      <c r="M56" s="196"/>
+      <c r="N56" s="196"/>
+      <c r="O56" s="196"/>
+      <c r="P56" s="196"/>
+      <c r="Q56" s="196"/>
+      <c r="R56" s="196"/>
+      <c r="S56" s="196"/>
+      <c r="T56" s="196"/>
+      <c r="U56" s="196"/>
+      <c r="V56" s="196"/>
+      <c r="W56" s="196"/>
+      <c r="X56" s="196"/>
     </row>
     <row r="57" spans="1:24" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
@@ -4247,27 +4266,27 @@
       </c>
       <c r="B57" s="14"/>
       <c r="C57" s="187"/>
-      <c r="D57" s="206"/>
-      <c r="E57" s="206"/>
-      <c r="F57" s="206"/>
-      <c r="G57" s="206"/>
-      <c r="H57" s="206"/>
-      <c r="I57" s="206"/>
-      <c r="J57" s="206"/>
-      <c r="K57" s="206"/>
-      <c r="L57" s="206"/>
-      <c r="M57" s="206"/>
-      <c r="N57" s="206"/>
-      <c r="O57" s="206"/>
-      <c r="P57" s="206"/>
-      <c r="Q57" s="206"/>
-      <c r="R57" s="206"/>
-      <c r="S57" s="206"/>
-      <c r="T57" s="206"/>
-      <c r="U57" s="206"/>
-      <c r="V57" s="206"/>
-      <c r="W57" s="206"/>
-      <c r="X57" s="206"/>
+      <c r="D57" s="205"/>
+      <c r="E57" s="205"/>
+      <c r="F57" s="205"/>
+      <c r="G57" s="205"/>
+      <c r="H57" s="205"/>
+      <c r="I57" s="205"/>
+      <c r="J57" s="205"/>
+      <c r="K57" s="205"/>
+      <c r="L57" s="205"/>
+      <c r="M57" s="205"/>
+      <c r="N57" s="205"/>
+      <c r="O57" s="205"/>
+      <c r="P57" s="205"/>
+      <c r="Q57" s="205"/>
+      <c r="R57" s="205"/>
+      <c r="S57" s="205"/>
+      <c r="T57" s="205"/>
+      <c r="U57" s="205"/>
+      <c r="V57" s="205"/>
+      <c r="W57" s="205"/>
+      <c r="X57" s="205"/>
     </row>
     <row r="58" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="39"/>
@@ -4288,14 +4307,14 @@
       <c r="N58" s="190"/>
       <c r="O58" s="190"/>
       <c r="P58" s="190"/>
-      <c r="Q58" s="204"/>
-      <c r="R58" s="196"/>
-      <c r="S58" s="196"/>
-      <c r="T58" s="196"/>
-      <c r="U58" s="204"/>
-      <c r="V58" s="204"/>
-      <c r="W58" s="204"/>
-      <c r="X58" s="204"/>
+      <c r="Q58" s="203"/>
+      <c r="R58" s="195"/>
+      <c r="S58" s="195"/>
+      <c r="T58" s="195"/>
+      <c r="U58" s="203"/>
+      <c r="V58" s="203"/>
+      <c r="W58" s="203"/>
+      <c r="X58" s="203"/>
     </row>
     <row r="59" spans="1:24" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="39"/>
@@ -4321,8 +4340,8 @@
       <c r="S59" s="190"/>
       <c r="T59" s="190"/>
       <c r="U59" s="190"/>
-      <c r="V59" s="196"/>
-      <c r="W59" s="208"/>
+      <c r="V59" s="195"/>
+      <c r="W59" s="207"/>
       <c r="X59" s="190"/>
     </row>
     <row r="60" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -5281,15 +5300,15 @@
     </row>
     <row r="100" spans="1:24" ht="13" x14ac:dyDescent="0.15">
       <c r="B100" s="29"/>
-      <c r="C100" s="227"/>
-      <c r="D100" s="228"/>
-      <c r="E100" s="228"/>
-      <c r="F100" s="228"/>
-      <c r="G100" s="228"/>
-      <c r="H100" s="228"/>
-      <c r="I100" s="228"/>
-      <c r="J100" s="228"/>
-      <c r="K100" s="229"/>
+      <c r="C100" s="226"/>
+      <c r="D100" s="227"/>
+      <c r="E100" s="227"/>
+      <c r="F100" s="227"/>
+      <c r="G100" s="227"/>
+      <c r="H100" s="227"/>
+      <c r="I100" s="227"/>
+      <c r="J100" s="227"/>
+      <c r="K100" s="228"/>
       <c r="L100" s="135"/>
       <c r="M100" s="136"/>
       <c r="N100" s="137"/>

</xml_diff>

<commit_message>
Update for this week.
</commit_message>
<xml_diff>
--- a/project_management/E2E-Deliverables-Completion-Timeline.xlsx
+++ b/project_management/E2E-Deliverables-Completion-Timeline.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25725"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmz/galois-repos/e2eviv/project_management/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27760" windowHeight="19920"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Current Plan 2015-16" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -304,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -385,6 +380,18 @@
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -978,8 +985,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
@@ -1339,6 +1352,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,47 +1412,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2725,11 +2740,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B20" zoomScale="125" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.125" style="1" customWidth="1"/>
@@ -2738,7 +2753,7 @@
     <col min="25" max="256" width="8" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="40" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2770,7 +2785,7 @@
       <c r="AA1" s="10"/>
       <c r="AB1" s="10"/>
     </row>
-    <row r="2" spans="1:28" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:28" ht="40" customHeight="1">
       <c r="A2" s="11"/>
       <c r="B2" s="12" t="s">
         <v>1</v>
@@ -2802,7 +2817,7 @@
       <c r="AA2" s="10"/>
       <c r="AB2" s="10"/>
     </row>
-    <row r="3" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:28" ht="25" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -2810,43 +2825,43 @@
       <c r="C3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="127" t="s">
+      <c r="D3" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="121" t="s">
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="121" t="s">
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="135"/>
+      <c r="L3" s="136"/>
+      <c r="M3" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="121" t="s">
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
+      <c r="P3" s="136"/>
+      <c r="Q3" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="122"/>
-      <c r="S3" s="122"/>
-      <c r="T3" s="123"/>
-      <c r="U3" s="121" t="s">
+      <c r="R3" s="135"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="134" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="122"/>
-      <c r="W3" s="122"/>
-      <c r="X3" s="123"/>
+      <c r="V3" s="135"/>
+      <c r="W3" s="135"/>
+      <c r="X3" s="136"/>
       <c r="Y3" s="20"/>
       <c r="Z3" s="21"/>
       <c r="AA3" s="21"/>
       <c r="AB3" s="21"/>
     </row>
-    <row r="4" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" ht="18" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="23"/>
@@ -2918,7 +2933,7 @@
       <c r="AA4" s="26"/>
       <c r="AB4" s="26"/>
     </row>
-    <row r="5" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" ht="18" customHeight="1">
       <c r="A5" s="27"/>
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
@@ -2990,7 +3005,7 @@
       <c r="AA5" s="30"/>
       <c r="AB5" s="30"/>
     </row>
-    <row r="6" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="18" customHeight="1">
       <c r="A6" s="31" t="s">
         <v>35</v>
       </c>
@@ -3022,7 +3037,7 @@
       <c r="AA6" s="38"/>
       <c r="AB6" s="38"/>
     </row>
-    <row r="7" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="18" customHeight="1">
       <c r="A7" s="39" t="s">
         <v>36</v>
       </c>
@@ -3054,7 +3069,7 @@
       <c r="AA7" s="22"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="18" customHeight="1">
       <c r="A8" s="47"/>
       <c r="B8" s="48"/>
       <c r="C8" s="41"/>
@@ -3064,20 +3079,20 @@
         <v>1</v>
       </c>
       <c r="G8" s="49"/>
-      <c r="H8" s="128"/>
+      <c r="H8" s="121"/>
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
       <c r="K8" s="96"/>
       <c r="L8" s="96"/>
-      <c r="M8" s="128"/>
+      <c r="M8" s="121"/>
       <c r="N8" s="49"/>
       <c r="O8" s="49"/>
       <c r="P8" s="96"/>
-      <c r="Q8" s="128"/>
+      <c r="Q8" s="121"/>
       <c r="R8" s="49"/>
       <c r="S8" s="49"/>
       <c r="T8" s="96"/>
-      <c r="U8" s="128"/>
+      <c r="U8" s="121"/>
       <c r="V8" s="49"/>
       <c r="W8" s="49"/>
       <c r="X8" s="96"/>
@@ -3086,39 +3101,39 @@
       <c r="AA8" s="51"/>
       <c r="AB8" s="51"/>
     </row>
-    <row r="9" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" ht="18" customHeight="1">
       <c r="A9" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="129"/>
-      <c r="J9" s="129"/>
-      <c r="K9" s="131"/>
-      <c r="L9" s="131"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="129"/>
-      <c r="O9" s="129"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="130"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="129"/>
-      <c r="T9" s="131"/>
-      <c r="U9" s="130"/>
-      <c r="V9" s="129"/>
-      <c r="W9" s="129"/>
-      <c r="X9" s="131"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="124"/>
+      <c r="Q9" s="123"/>
+      <c r="R9" s="122"/>
+      <c r="S9" s="122"/>
+      <c r="T9" s="124"/>
+      <c r="U9" s="123"/>
+      <c r="V9" s="122"/>
+      <c r="W9" s="122"/>
+      <c r="X9" s="124"/>
       <c r="Y9" s="37"/>
       <c r="Z9" s="38"/>
       <c r="AA9" s="38"/>
       <c r="AB9" s="38"/>
     </row>
-    <row r="10" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="18" customHeight="1">
       <c r="A10" s="52" t="s">
         <v>38</v>
       </c>
@@ -3128,20 +3143,20 @@
       <c r="E10" s="75"/>
       <c r="F10" s="75"/>
       <c r="G10" s="75"/>
-      <c r="H10" s="132"/>
+      <c r="H10" s="125"/>
       <c r="I10" s="75"/>
       <c r="J10" s="49"/>
       <c r="K10" s="96"/>
       <c r="L10" s="96"/>
-      <c r="M10" s="128"/>
+      <c r="M10" s="121"/>
       <c r="N10" s="49"/>
       <c r="O10" s="49"/>
       <c r="P10" s="96"/>
-      <c r="Q10" s="128"/>
+      <c r="Q10" s="121"/>
       <c r="R10" s="49"/>
       <c r="S10" s="49"/>
       <c r="T10" s="96"/>
-      <c r="U10" s="128"/>
+      <c r="U10" s="121"/>
       <c r="V10" s="49"/>
       <c r="W10" s="49"/>
       <c r="X10" s="96"/>
@@ -3150,7 +3165,7 @@
       <c r="AA10" s="22"/>
       <c r="AB10" s="22"/>
     </row>
-    <row r="11" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" ht="18" customHeight="1">
       <c r="A11" s="54"/>
       <c r="B11" s="55" t="s">
         <v>39</v>
@@ -3170,10 +3185,12 @@
       <c r="I11" s="49">
         <v>0.7</v>
       </c>
-      <c r="J11" s="136">
+      <c r="J11" s="129">
         <v>0.95</v>
       </c>
-      <c r="K11" s="49"/>
+      <c r="K11" s="129">
+        <v>1</v>
+      </c>
       <c r="L11" s="49"/>
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
@@ -3192,7 +3209,7 @@
       <c r="AA11" s="57"/>
       <c r="AB11" s="57"/>
     </row>
-    <row r="12" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="18" customHeight="1">
       <c r="A12" s="58"/>
       <c r="B12" s="55" t="s">
         <v>41</v>
@@ -3212,10 +3229,12 @@
       <c r="I12" s="49">
         <v>0.75</v>
       </c>
-      <c r="J12" s="136">
+      <c r="J12" s="129">
         <v>0.95</v>
       </c>
-      <c r="K12" s="49"/>
+      <c r="K12" s="129">
+        <v>1</v>
+      </c>
       <c r="L12" s="49"/>
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
@@ -3234,7 +3253,7 @@
       <c r="AA12" s="57"/>
       <c r="AB12" s="57"/>
     </row>
-    <row r="13" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" ht="18" customHeight="1">
       <c r="A13" s="58"/>
       <c r="B13" s="55" t="s">
         <v>43</v>
@@ -3254,10 +3273,12 @@
       <c r="I13" s="49">
         <v>1</v>
       </c>
-      <c r="J13" s="136">
+      <c r="J13" s="129">
         <v>1</v>
       </c>
-      <c r="K13" s="49"/>
+      <c r="K13" s="129">
+        <v>1</v>
+      </c>
       <c r="L13" s="49"/>
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
@@ -3276,7 +3297,7 @@
       <c r="AA13" s="57"/>
       <c r="AB13" s="57"/>
     </row>
-    <row r="14" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="18" customHeight="1">
       <c r="A14" s="59"/>
       <c r="B14" s="60"/>
       <c r="C14" s="41"/>
@@ -3286,7 +3307,7 @@
       <c r="G14" s="49"/>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
-      <c r="J14" s="136"/>
+      <c r="J14" s="129"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
       <c r="M14" s="49"/>
@@ -3306,39 +3327,39 @@
       <c r="AA14" s="27"/>
       <c r="AB14" s="27"/>
     </row>
-    <row r="15" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="18" customHeight="1">
       <c r="A15" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="129"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="129"/>
-      <c r="L15" s="129"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
-      <c r="S15" s="129"/>
-      <c r="T15" s="129"/>
-      <c r="U15" s="129"/>
-      <c r="V15" s="129"/>
-      <c r="W15" s="129"/>
-      <c r="X15" s="129"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="122"/>
+      <c r="F15" s="122"/>
+      <c r="G15" s="122"/>
+      <c r="H15" s="122"/>
+      <c r="I15" s="122"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="122"/>
+      <c r="O15" s="122"/>
+      <c r="P15" s="122"/>
+      <c r="Q15" s="122"/>
+      <c r="R15" s="122"/>
+      <c r="S15" s="122"/>
+      <c r="T15" s="122"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="122"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="122"/>
       <c r="Y15" s="62"/>
       <c r="Z15" s="63"/>
       <c r="AA15" s="63"/>
       <c r="AB15" s="63"/>
     </row>
-    <row r="16" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="18" customHeight="1">
       <c r="A16" s="52" t="s">
         <v>46</v>
       </c>
@@ -3350,7 +3371,7 @@
       <c r="G16" s="75"/>
       <c r="H16" s="75"/>
       <c r="I16" s="75"/>
-      <c r="J16" s="138"/>
+      <c r="J16" s="131"/>
       <c r="K16" s="75"/>
       <c r="L16" s="49"/>
       <c r="M16" s="49"/>
@@ -3370,7 +3391,7 @@
       <c r="AA16" s="65"/>
       <c r="AB16" s="65"/>
     </row>
-    <row r="17" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" ht="18" customHeight="1">
       <c r="A17" s="54"/>
       <c r="B17" s="55" t="s">
         <v>47</v>
@@ -3390,8 +3411,12 @@
       <c r="I17" s="49">
         <v>0.15</v>
       </c>
-      <c r="J17" s="136"/>
-      <c r="K17" s="49"/>
+      <c r="J17" s="129">
+        <v>0.15</v>
+      </c>
+      <c r="K17" s="49">
+        <v>0.15</v>
+      </c>
       <c r="L17" s="49"/>
       <c r="M17" s="49"/>
       <c r="N17" s="49"/>
@@ -3410,7 +3435,7 @@
       <c r="AA17" s="57"/>
       <c r="AB17" s="57"/>
     </row>
-    <row r="18" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" ht="18" customHeight="1">
       <c r="A18" s="58"/>
       <c r="B18" s="55" t="s">
         <v>49</v>
@@ -3430,8 +3455,12 @@
       <c r="I18" s="49">
         <v>0.25</v>
       </c>
-      <c r="J18" s="136"/>
-      <c r="K18" s="49"/>
+      <c r="J18" s="129">
+        <v>0.3</v>
+      </c>
+      <c r="K18" s="49">
+        <v>0.4</v>
+      </c>
       <c r="L18" s="49"/>
       <c r="M18" s="49"/>
       <c r="N18" s="49"/>
@@ -3450,7 +3479,7 @@
       <c r="AA18" s="57"/>
       <c r="AB18" s="57"/>
     </row>
-    <row r="19" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" ht="18" customHeight="1">
       <c r="A19" s="57"/>
       <c r="B19" s="55" t="s">
         <v>50</v>
@@ -3470,8 +3499,12 @@
       <c r="I19" s="49">
         <v>0.25</v>
       </c>
-      <c r="J19" s="136"/>
-      <c r="K19" s="49"/>
+      <c r="J19" s="129">
+        <v>0.25</v>
+      </c>
+      <c r="K19" s="49">
+        <v>0.25</v>
+      </c>
       <c r="L19" s="49"/>
       <c r="M19" s="49"/>
       <c r="N19" s="49"/>
@@ -3490,7 +3523,7 @@
       <c r="AA19" s="57"/>
       <c r="AB19" s="57"/>
     </row>
-    <row r="20" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" ht="18" customHeight="1">
       <c r="A20" s="66"/>
       <c r="B20" s="55" t="s">
         <v>51</v>
@@ -3510,8 +3543,12 @@
       <c r="I20" s="49">
         <v>0.25</v>
       </c>
-      <c r="J20" s="136"/>
-      <c r="K20" s="49"/>
+      <c r="J20" s="129">
+        <v>0.25</v>
+      </c>
+      <c r="K20" s="49">
+        <v>0.4</v>
+      </c>
       <c r="L20" s="49"/>
       <c r="M20" s="49"/>
       <c r="N20" s="49"/>
@@ -3530,7 +3567,7 @@
       <c r="AA20" s="57"/>
       <c r="AB20" s="57"/>
     </row>
-    <row r="21" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" ht="18" customHeight="1">
       <c r="A21" s="68"/>
       <c r="B21" s="60"/>
       <c r="C21" s="41"/>
@@ -3540,7 +3577,7 @@
       <c r="G21" s="67"/>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
-      <c r="J21" s="136"/>
+      <c r="J21" s="129"/>
       <c r="K21" s="49"/>
       <c r="L21" s="49"/>
       <c r="M21" s="49"/>
@@ -3560,39 +3597,39 @@
       <c r="AA21" s="51"/>
       <c r="AB21" s="51"/>
     </row>
-    <row r="22" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" ht="18" customHeight="1">
       <c r="A22" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B22" s="32"/>
       <c r="C22" s="33"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
-      <c r="G22" s="129"/>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="137"/>
-      <c r="K22" s="129"/>
-      <c r="L22" s="129"/>
-      <c r="M22" s="129"/>
-      <c r="N22" s="129"/>
-      <c r="O22" s="129"/>
-      <c r="P22" s="129"/>
-      <c r="Q22" s="129"/>
-      <c r="R22" s="129"/>
-      <c r="S22" s="129"/>
-      <c r="T22" s="129"/>
-      <c r="U22" s="129"/>
-      <c r="V22" s="129"/>
-      <c r="W22" s="129"/>
-      <c r="X22" s="129"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="122"/>
+      <c r="H22" s="122"/>
+      <c r="I22" s="122"/>
+      <c r="J22" s="130"/>
+      <c r="K22" s="122"/>
+      <c r="L22" s="122"/>
+      <c r="M22" s="122"/>
+      <c r="N22" s="122"/>
+      <c r="O22" s="122"/>
+      <c r="P22" s="122"/>
+      <c r="Q22" s="122"/>
+      <c r="R22" s="122"/>
+      <c r="S22" s="122"/>
+      <c r="T22" s="122"/>
+      <c r="U22" s="122"/>
+      <c r="V22" s="122"/>
+      <c r="W22" s="122"/>
+      <c r="X22" s="122"/>
       <c r="Y22" s="37"/>
       <c r="Z22" s="38"/>
       <c r="AA22" s="38"/>
       <c r="AB22" s="38"/>
     </row>
-    <row r="23" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" ht="18" customHeight="1">
       <c r="A23" s="39" t="s">
         <v>54</v>
       </c>
@@ -3604,18 +3641,18 @@
       <c r="G23" s="49"/>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
-      <c r="J23" s="138"/>
+      <c r="J23" s="131"/>
       <c r="K23" s="75"/>
       <c r="L23" s="75"/>
       <c r="M23" s="75"/>
       <c r="N23" s="75"/>
-      <c r="O23" s="133"/>
-      <c r="P23" s="133"/>
-      <c r="Q23" s="133"/>
+      <c r="O23" s="126"/>
+      <c r="P23" s="126"/>
+      <c r="Q23" s="126"/>
       <c r="R23" s="49"/>
       <c r="S23" s="49"/>
       <c r="T23" s="49"/>
-      <c r="U23" s="133"/>
+      <c r="U23" s="126"/>
       <c r="V23" s="49"/>
       <c r="W23" s="49"/>
       <c r="X23" s="49"/>
@@ -3624,7 +3661,7 @@
       <c r="AA23" s="22"/>
       <c r="AB23" s="22"/>
     </row>
-    <row r="24" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" ht="18" customHeight="1">
       <c r="A24" s="69"/>
       <c r="B24" s="70" t="s">
         <v>55</v>
@@ -3644,20 +3681,22 @@
       <c r="I24" s="49">
         <v>0</v>
       </c>
-      <c r="J24" s="136">
+      <c r="J24" s="129">
         <v>0</v>
       </c>
-      <c r="K24" s="49"/>
+      <c r="K24" s="49">
+        <v>0</v>
+      </c>
       <c r="L24" s="49"/>
       <c r="M24" s="49"/>
       <c r="N24" s="49"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
-      <c r="Q24" s="133"/>
+      <c r="O24" s="126"/>
+      <c r="P24" s="126"/>
+      <c r="Q24" s="126"/>
       <c r="R24" s="49"/>
       <c r="S24" s="49"/>
       <c r="T24" s="49"/>
-      <c r="U24" s="133"/>
+      <c r="U24" s="126"/>
       <c r="V24" s="49"/>
       <c r="W24" s="49"/>
       <c r="X24" s="49"/>
@@ -3666,7 +3705,7 @@
       <c r="AA24" s="57"/>
       <c r="AB24" s="57"/>
     </row>
-    <row r="25" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28" ht="18" customHeight="1">
       <c r="A25" s="58"/>
       <c r="B25" s="55" t="s">
         <v>57</v>
@@ -3686,10 +3725,12 @@
       <c r="I25" s="49">
         <v>0.7</v>
       </c>
-      <c r="J25" s="136">
+      <c r="J25" s="129">
         <v>0.85</v>
       </c>
-      <c r="K25" s="49"/>
+      <c r="K25" s="49">
+        <v>0.9</v>
+      </c>
       <c r="L25" s="49"/>
       <c r="M25" s="49"/>
       <c r="N25" s="49"/>
@@ -3708,7 +3749,7 @@
       <c r="AA25" s="57"/>
       <c r="AB25" s="57"/>
     </row>
-    <row r="26" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28" ht="18" customHeight="1">
       <c r="A26" s="58"/>
       <c r="B26" s="55" t="s">
         <v>58</v>
@@ -3728,10 +3769,12 @@
       <c r="I26" s="49">
         <v>0.25</v>
       </c>
-      <c r="J26" s="136">
+      <c r="J26" s="129">
         <v>0.25</v>
       </c>
-      <c r="K26" s="49"/>
+      <c r="K26" s="49">
+        <v>0.25</v>
+      </c>
       <c r="L26" s="49"/>
       <c r="M26" s="49"/>
       <c r="N26" s="49"/>
@@ -3750,7 +3793,7 @@
       <c r="AA26" s="57"/>
       <c r="AB26" s="57"/>
     </row>
-    <row r="27" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28" ht="18" customHeight="1">
       <c r="A27" s="58"/>
       <c r="B27" s="71" t="s">
         <v>60</v>
@@ -3770,10 +3813,12 @@
       <c r="I27" s="49">
         <v>0</v>
       </c>
-      <c r="J27" s="136">
+      <c r="J27" s="129">
         <v>0</v>
       </c>
-      <c r="K27" s="49"/>
+      <c r="K27" s="49">
+        <v>0</v>
+      </c>
       <c r="L27" s="49"/>
       <c r="M27" s="49"/>
       <c r="N27" s="49"/>
@@ -3786,13 +3831,13 @@
       <c r="U27" s="49"/>
       <c r="V27" s="49"/>
       <c r="W27" s="49"/>
-      <c r="X27" s="134"/>
+      <c r="X27" s="127"/>
       <c r="Y27" s="73"/>
       <c r="Z27" s="74"/>
       <c r="AA27" s="74"/>
       <c r="AB27" s="57"/>
     </row>
-    <row r="28" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28" ht="18" customHeight="1">
       <c r="A28" s="58"/>
       <c r="B28" s="55" t="s">
         <v>61</v>
@@ -3812,10 +3857,12 @@
       <c r="I28" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="J28" s="136" t="s">
+      <c r="J28" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="49"/>
+      <c r="K28" s="49">
+        <v>0.25</v>
+      </c>
       <c r="L28" s="49"/>
       <c r="M28" s="49"/>
       <c r="N28" s="49"/>
@@ -3834,7 +3881,7 @@
       <c r="AA28" s="57"/>
       <c r="AB28" s="57"/>
     </row>
-    <row r="29" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28" ht="18" customHeight="1">
       <c r="A29" s="68"/>
       <c r="B29" s="60"/>
       <c r="C29" s="41"/>
@@ -3844,7 +3891,7 @@
       <c r="G29" s="67"/>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
-      <c r="J29" s="136"/>
+      <c r="J29" s="129"/>
       <c r="K29" s="49"/>
       <c r="L29" s="49"/>
       <c r="M29" s="49"/>
@@ -3864,39 +3911,39 @@
       <c r="AA29" s="51"/>
       <c r="AB29" s="51"/>
     </row>
-    <row r="30" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" ht="18" customHeight="1">
       <c r="A30" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="129"/>
-      <c r="E30" s="129"/>
-      <c r="F30" s="129"/>
-      <c r="G30" s="129"/>
-      <c r="H30" s="129"/>
-      <c r="I30" s="129"/>
-      <c r="J30" s="137"/>
-      <c r="K30" s="129"/>
-      <c r="L30" s="129"/>
-      <c r="M30" s="129"/>
-      <c r="N30" s="129"/>
-      <c r="O30" s="129"/>
-      <c r="P30" s="129"/>
-      <c r="Q30" s="129"/>
-      <c r="R30" s="129"/>
-      <c r="S30" s="129"/>
-      <c r="T30" s="129"/>
-      <c r="U30" s="129"/>
-      <c r="V30" s="129"/>
-      <c r="W30" s="129"/>
-      <c r="X30" s="129"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="122"/>
+      <c r="G30" s="122"/>
+      <c r="H30" s="122"/>
+      <c r="I30" s="122"/>
+      <c r="J30" s="130"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="122"/>
+      <c r="M30" s="122"/>
+      <c r="N30" s="122"/>
+      <c r="O30" s="122"/>
+      <c r="P30" s="122"/>
+      <c r="Q30" s="122"/>
+      <c r="R30" s="122"/>
+      <c r="S30" s="122"/>
+      <c r="T30" s="122"/>
+      <c r="U30" s="122"/>
+      <c r="V30" s="122"/>
+      <c r="W30" s="122"/>
+      <c r="X30" s="122"/>
       <c r="Y30" s="37"/>
       <c r="Z30" s="38"/>
       <c r="AA30" s="38"/>
       <c r="AB30" s="38"/>
     </row>
-    <row r="31" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" ht="18" customHeight="1">
       <c r="A31" s="52" t="s">
         <v>64</v>
       </c>
@@ -3908,9 +3955,9 @@
       <c r="G31" s="49"/>
       <c r="H31" s="49"/>
       <c r="I31" s="49"/>
-      <c r="J31" s="139"/>
-      <c r="K31" s="133"/>
-      <c r="L31" s="133"/>
+      <c r="J31" s="132"/>
+      <c r="K31" s="126"/>
+      <c r="L31" s="126"/>
       <c r="M31" s="49"/>
       <c r="N31" s="49"/>
       <c r="O31" s="49"/>
@@ -3928,7 +3975,7 @@
       <c r="AA31" s="22"/>
       <c r="AB31" s="22"/>
     </row>
-    <row r="32" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" ht="18" customHeight="1">
       <c r="A32" s="54"/>
       <c r="B32" s="55" t="s">
         <v>65</v>
@@ -3937,10 +3984,10 @@
       <c r="D32" s="49"/>
       <c r="E32" s="49"/>
       <c r="F32" s="49"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="134"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="127"/>
       <c r="I32" s="75"/>
-      <c r="J32" s="136"/>
+      <c r="J32" s="129"/>
       <c r="K32" s="49"/>
       <c r="L32" s="49"/>
       <c r="M32" s="49"/>
@@ -3960,7 +4007,7 @@
       <c r="AA32" s="57"/>
       <c r="AB32" s="57"/>
     </row>
-    <row r="33" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28" ht="18" customHeight="1">
       <c r="A33" s="58"/>
       <c r="B33" s="55" t="s">
         <v>66</v>
@@ -3969,10 +4016,10 @@
       <c r="D33" s="49"/>
       <c r="E33" s="49"/>
       <c r="F33" s="49"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="134"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="127"/>
       <c r="I33" s="49"/>
-      <c r="J33" s="138"/>
+      <c r="J33" s="131"/>
       <c r="K33" s="49"/>
       <c r="L33" s="49"/>
       <c r="M33" s="49"/>
@@ -3992,7 +4039,7 @@
       <c r="AA33" s="57"/>
       <c r="AB33" s="57"/>
     </row>
-    <row r="34" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" ht="18" customHeight="1">
       <c r="A34" s="58"/>
       <c r="B34" s="55" t="s">
         <v>67</v>
@@ -4002,9 +4049,9 @@
       <c r="E34" s="49"/>
       <c r="F34" s="49"/>
       <c r="G34" s="49"/>
-      <c r="H34" s="134"/>
+      <c r="H34" s="127"/>
       <c r="I34" s="49"/>
-      <c r="J34" s="140"/>
+      <c r="J34" s="133"/>
       <c r="K34" s="75"/>
       <c r="L34" s="75"/>
       <c r="M34" s="49"/>
@@ -4024,7 +4071,7 @@
       <c r="AA34" s="57"/>
       <c r="AB34" s="57"/>
     </row>
-    <row r="35" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28" ht="18" customHeight="1">
       <c r="A35" s="58"/>
       <c r="B35" s="55" t="s">
         <v>68</v>
@@ -4036,9 +4083,9 @@
       <c r="G35" s="49"/>
       <c r="H35" s="49"/>
       <c r="I35" s="49"/>
-      <c r="J35" s="136"/>
-      <c r="K35" s="134"/>
-      <c r="L35" s="134"/>
+      <c r="J35" s="129"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="127"/>
       <c r="M35" s="75"/>
       <c r="N35" s="75"/>
       <c r="O35" s="49"/>
@@ -4056,7 +4103,7 @@
       <c r="AA35" s="57"/>
       <c r="AB35" s="57"/>
     </row>
-    <row r="36" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28" ht="18" customHeight="1">
       <c r="A36" s="59"/>
       <c r="B36" s="60"/>
       <c r="C36" s="41"/>
@@ -4066,7 +4113,7 @@
       <c r="G36" s="49"/>
       <c r="H36" s="49"/>
       <c r="I36" s="49"/>
-      <c r="J36" s="136"/>
+      <c r="J36" s="129"/>
       <c r="K36" s="49"/>
       <c r="L36" s="49"/>
       <c r="M36" s="49"/>
@@ -4086,39 +4133,39 @@
       <c r="AA36" s="51"/>
       <c r="AB36" s="51"/>
     </row>
-    <row r="37" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28" ht="18" customHeight="1">
       <c r="A37" s="31" t="s">
         <v>69</v>
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="33"/>
-      <c r="D37" s="129"/>
-      <c r="E37" s="129"/>
-      <c r="F37" s="129"/>
-      <c r="G37" s="129"/>
-      <c r="H37" s="129"/>
-      <c r="I37" s="129"/>
-      <c r="J37" s="137"/>
-      <c r="K37" s="129"/>
-      <c r="L37" s="129"/>
-      <c r="M37" s="129"/>
-      <c r="N37" s="129"/>
-      <c r="O37" s="129"/>
-      <c r="P37" s="129"/>
-      <c r="Q37" s="129"/>
-      <c r="R37" s="129"/>
-      <c r="S37" s="129"/>
-      <c r="T37" s="129"/>
-      <c r="U37" s="129"/>
-      <c r="V37" s="129"/>
-      <c r="W37" s="129"/>
-      <c r="X37" s="129"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="130"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="122"/>
+      <c r="P37" s="122"/>
+      <c r="Q37" s="122"/>
+      <c r="R37" s="122"/>
+      <c r="S37" s="122"/>
+      <c r="T37" s="122"/>
+      <c r="U37" s="122"/>
+      <c r="V37" s="122"/>
+      <c r="W37" s="122"/>
+      <c r="X37" s="122"/>
       <c r="Y37" s="37"/>
       <c r="Z37" s="38"/>
       <c r="AA37" s="38"/>
       <c r="AB37" s="38"/>
     </row>
-    <row r="38" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28" ht="18" customHeight="1">
       <c r="A38" s="52" t="s">
         <v>70</v>
       </c>
@@ -4130,7 +4177,7 @@
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
       <c r="I38" s="49"/>
-      <c r="J38" s="136"/>
+      <c r="J38" s="129"/>
       <c r="K38" s="49"/>
       <c r="L38" s="49"/>
       <c r="M38" s="49"/>
@@ -4150,7 +4197,7 @@
       <c r="AA38" s="22"/>
       <c r="AB38" s="22"/>
     </row>
-    <row r="39" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28" ht="18" customHeight="1">
       <c r="A39" s="54"/>
       <c r="B39" s="55" t="s">
         <v>71</v>
@@ -4162,10 +4209,12 @@
       <c r="G39" s="75"/>
       <c r="H39" s="75"/>
       <c r="I39" s="49"/>
-      <c r="J39" s="136">
+      <c r="J39" s="129">
         <v>0.85</v>
       </c>
-      <c r="K39" s="49"/>
+      <c r="K39" s="49">
+        <v>0.9</v>
+      </c>
       <c r="L39" s="49"/>
       <c r="M39" s="49"/>
       <c r="N39" s="49"/>
@@ -4184,7 +4233,7 @@
       <c r="AA39" s="57"/>
       <c r="AB39" s="57"/>
     </row>
-    <row r="40" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28" ht="18" customHeight="1">
       <c r="A40" s="58"/>
       <c r="B40" s="55" t="s">
         <v>72</v>
@@ -4196,7 +4245,7 @@
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
       <c r="I40" s="75"/>
-      <c r="J40" s="138">
+      <c r="J40" s="131">
         <v>0.05</v>
       </c>
       <c r="K40" s="75"/>
@@ -4218,7 +4267,7 @@
       <c r="AA40" s="57"/>
       <c r="AB40" s="57"/>
     </row>
-    <row r="41" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28" ht="18" customHeight="1">
       <c r="A41" s="58"/>
       <c r="B41" s="55" t="s">
         <v>73</v>
@@ -4230,7 +4279,7 @@
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
       <c r="I41" s="49"/>
-      <c r="J41" s="136">
+      <c r="J41" s="129">
         <v>0</v>
       </c>
       <c r="K41" s="75"/>
@@ -4252,7 +4301,7 @@
       <c r="AA41" s="57"/>
       <c r="AB41" s="57"/>
     </row>
-    <row r="42" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28" ht="18" customHeight="1">
       <c r="A42" s="58"/>
       <c r="B42" s="55" t="s">
         <v>74</v>
@@ -4264,7 +4313,7 @@
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
       <c r="I42" s="49"/>
-      <c r="J42" s="136">
+      <c r="J42" s="129">
         <v>0</v>
       </c>
       <c r="K42" s="49"/>
@@ -4286,7 +4335,7 @@
       <c r="AA42" s="57"/>
       <c r="AB42" s="57"/>
     </row>
-    <row r="43" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28" ht="18" customHeight="1">
       <c r="A43" s="66"/>
       <c r="B43" s="55" t="s">
         <v>75</v>
@@ -4298,7 +4347,7 @@
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
       <c r="I43" s="49"/>
-      <c r="J43" s="136">
+      <c r="J43" s="129">
         <v>0</v>
       </c>
       <c r="K43" s="49"/>
@@ -4320,7 +4369,7 @@
       <c r="AA43" s="57"/>
       <c r="AB43" s="57"/>
     </row>
-    <row r="44" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28" ht="18" customHeight="1">
       <c r="A44" s="59"/>
       <c r="B44" s="76"/>
       <c r="C44" s="41"/>
@@ -4350,39 +4399,39 @@
       <c r="AA44" s="51"/>
       <c r="AB44" s="51"/>
     </row>
-    <row r="45" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" ht="18" customHeight="1">
       <c r="A45" s="31" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="32"/>
       <c r="C45" s="33"/>
-      <c r="D45" s="129"/>
-      <c r="E45" s="129"/>
-      <c r="F45" s="129"/>
-      <c r="G45" s="129"/>
-      <c r="H45" s="129"/>
-      <c r="I45" s="129"/>
-      <c r="J45" s="129"/>
-      <c r="K45" s="129"/>
-      <c r="L45" s="129"/>
-      <c r="M45" s="129"/>
-      <c r="N45" s="129"/>
-      <c r="O45" s="129"/>
-      <c r="P45" s="129"/>
-      <c r="Q45" s="129"/>
-      <c r="R45" s="129"/>
-      <c r="S45" s="129"/>
-      <c r="T45" s="129"/>
-      <c r="U45" s="129"/>
-      <c r="V45" s="129"/>
-      <c r="W45" s="129"/>
-      <c r="X45" s="129"/>
+      <c r="D45" s="122"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="122"/>
+      <c r="G45" s="122"/>
+      <c r="H45" s="122"/>
+      <c r="I45" s="122"/>
+      <c r="J45" s="122"/>
+      <c r="K45" s="122"/>
+      <c r="L45" s="122"/>
+      <c r="M45" s="122"/>
+      <c r="N45" s="122"/>
+      <c r="O45" s="122"/>
+      <c r="P45" s="122"/>
+      <c r="Q45" s="122"/>
+      <c r="R45" s="122"/>
+      <c r="S45" s="122"/>
+      <c r="T45" s="122"/>
+      <c r="U45" s="122"/>
+      <c r="V45" s="122"/>
+      <c r="W45" s="122"/>
+      <c r="X45" s="122"/>
       <c r="Y45" s="37"/>
       <c r="Z45" s="38"/>
       <c r="AA45" s="38"/>
       <c r="AB45" s="38"/>
     </row>
-    <row r="46" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:28" ht="18" customHeight="1">
       <c r="A46" s="52" t="s">
         <v>77</v>
       </c>
@@ -4414,7 +4463,7 @@
       <c r="AA46" s="22"/>
       <c r="AB46" s="22"/>
     </row>
-    <row r="47" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:28" ht="18" customHeight="1">
       <c r="A47" s="54"/>
       <c r="B47" s="55" t="s">
         <v>78</v>
@@ -4446,7 +4495,7 @@
       <c r="AA47" s="57"/>
       <c r="AB47" s="57"/>
     </row>
-    <row r="48" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:28" ht="18" customHeight="1">
       <c r="A48" s="58"/>
       <c r="B48" s="55" t="s">
         <v>79</v>
@@ -4478,7 +4527,7 @@
       <c r="AA48" s="57"/>
       <c r="AB48" s="57"/>
     </row>
-    <row r="49" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:28" ht="18" customHeight="1">
       <c r="A49" s="58"/>
       <c r="B49" s="55" t="s">
         <v>80</v>
@@ -4510,7 +4559,7 @@
       <c r="AA49" s="57"/>
       <c r="AB49" s="57"/>
     </row>
-    <row r="50" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:28" ht="18" customHeight="1">
       <c r="A50" s="58"/>
       <c r="B50" s="55" t="s">
         <v>81</v>
@@ -4542,7 +4591,7 @@
       <c r="AA50" s="57"/>
       <c r="AB50" s="57"/>
     </row>
-    <row r="51" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:28" ht="18" customHeight="1">
       <c r="A51" s="66"/>
       <c r="B51" s="55" t="s">
         <v>82</v>
@@ -4574,7 +4623,7 @@
       <c r="AA51" s="57"/>
       <c r="AB51" s="57"/>
     </row>
-    <row r="52" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:28" ht="18" customHeight="1">
       <c r="A52" s="77"/>
       <c r="B52" s="55" t="s">
         <v>83</v>
@@ -4606,7 +4655,7 @@
       <c r="AA52" s="57"/>
       <c r="AB52" s="57"/>
     </row>
-    <row r="53" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:28" ht="18" customHeight="1">
       <c r="A53" s="77"/>
       <c r="B53" s="55" t="s">
         <v>84</v>
@@ -4638,7 +4687,7 @@
       <c r="AA53" s="57"/>
       <c r="AB53" s="57"/>
     </row>
-    <row r="54" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:28" ht="18" customHeight="1">
       <c r="A54" s="77"/>
       <c r="B54" s="78" t="s">
         <v>85</v>
@@ -4670,7 +4719,7 @@
       <c r="AA54" s="57"/>
       <c r="AB54" s="57"/>
     </row>
-    <row r="55" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:28" ht="18" customHeight="1">
       <c r="A55" s="57"/>
       <c r="B55" s="60"/>
       <c r="C55" s="41"/>
@@ -4700,7 +4749,7 @@
       <c r="AA55" s="57"/>
       <c r="AB55" s="57"/>
     </row>
-    <row r="56" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:28" ht="18" customHeight="1">
       <c r="A56" s="79"/>
       <c r="B56" s="80"/>
       <c r="C56" s="41"/>
@@ -4730,39 +4779,39 @@
       <c r="AA56" s="57"/>
       <c r="AB56" s="57"/>
     </row>
-    <row r="57" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:28" ht="18" customHeight="1">
       <c r="A57" s="81" t="s">
         <v>86</v>
       </c>
       <c r="B57" s="82"/>
       <c r="C57" s="83"/>
-      <c r="D57" s="135"/>
-      <c r="E57" s="135"/>
-      <c r="F57" s="135"/>
-      <c r="G57" s="135"/>
-      <c r="H57" s="135"/>
-      <c r="I57" s="135"/>
-      <c r="J57" s="135"/>
-      <c r="K57" s="135"/>
-      <c r="L57" s="135"/>
-      <c r="M57" s="135"/>
-      <c r="N57" s="135"/>
-      <c r="O57" s="135"/>
-      <c r="P57" s="135"/>
-      <c r="Q57" s="135"/>
-      <c r="R57" s="135"/>
-      <c r="S57" s="135"/>
-      <c r="T57" s="135"/>
-      <c r="U57" s="135"/>
-      <c r="V57" s="135"/>
-      <c r="W57" s="135"/>
-      <c r="X57" s="135"/>
+      <c r="D57" s="128"/>
+      <c r="E57" s="128"/>
+      <c r="F57" s="128"/>
+      <c r="G57" s="128"/>
+      <c r="H57" s="128"/>
+      <c r="I57" s="128"/>
+      <c r="J57" s="128"/>
+      <c r="K57" s="128"/>
+      <c r="L57" s="128"/>
+      <c r="M57" s="128"/>
+      <c r="N57" s="128"/>
+      <c r="O57" s="128"/>
+      <c r="P57" s="128"/>
+      <c r="Q57" s="128"/>
+      <c r="R57" s="128"/>
+      <c r="S57" s="128"/>
+      <c r="T57" s="128"/>
+      <c r="U57" s="128"/>
+      <c r="V57" s="128"/>
+      <c r="W57" s="128"/>
+      <c r="X57" s="128"/>
       <c r="Y57" s="56"/>
       <c r="Z57" s="57"/>
       <c r="AA57" s="57"/>
       <c r="AB57" s="57"/>
     </row>
-    <row r="58" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:28" ht="18" customHeight="1">
       <c r="A58" s="54"/>
       <c r="B58" s="84" t="s">
         <v>87</v>
@@ -4781,20 +4830,20 @@
       <c r="N58" s="49"/>
       <c r="O58" s="49"/>
       <c r="P58" s="49"/>
-      <c r="Q58" s="133"/>
+      <c r="Q58" s="126"/>
       <c r="R58" s="75"/>
       <c r="S58" s="75"/>
       <c r="T58" s="75"/>
-      <c r="U58" s="133"/>
-      <c r="V58" s="133"/>
-      <c r="W58" s="133"/>
-      <c r="X58" s="133"/>
+      <c r="U58" s="126"/>
+      <c r="V58" s="126"/>
+      <c r="W58" s="126"/>
+      <c r="X58" s="126"/>
       <c r="Y58" s="56"/>
       <c r="Z58" s="57"/>
       <c r="AA58" s="57"/>
       <c r="AB58" s="57"/>
     </row>
-    <row r="59" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:28" ht="18" customHeight="1">
       <c r="A59" s="58"/>
       <c r="B59" s="78" t="s">
         <v>88</v>
@@ -4819,14 +4868,14 @@
       <c r="T59" s="49"/>
       <c r="U59" s="49"/>
       <c r="V59" s="75"/>
-      <c r="W59" s="134"/>
+      <c r="W59" s="127"/>
       <c r="X59" s="49"/>
       <c r="Y59" s="56"/>
       <c r="Z59" s="57"/>
       <c r="AA59" s="57"/>
       <c r="AB59" s="57"/>
     </row>
-    <row r="60" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:28" ht="18" customHeight="1">
       <c r="A60" s="57"/>
       <c r="B60" s="85"/>
       <c r="C60" s="86"/>
@@ -4856,7 +4905,7 @@
       <c r="AA60" s="57"/>
       <c r="AB60" s="57"/>
     </row>
-    <row r="61" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:28" ht="18" customHeight="1">
       <c r="A61" s="58"/>
       <c r="B61" s="60"/>
       <c r="C61" s="90"/>
@@ -4886,7 +4935,7 @@
       <c r="AA61" s="57"/>
       <c r="AB61" s="57"/>
     </row>
-    <row r="62" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:28" ht="18" customHeight="1">
       <c r="A62" s="58"/>
       <c r="B62" s="60"/>
       <c r="C62" s="90"/>
@@ -4916,7 +4965,7 @@
       <c r="AA62" s="57"/>
       <c r="AB62" s="57"/>
     </row>
-    <row r="63" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:28" ht="18" customHeight="1">
       <c r="A63" s="57"/>
       <c r="B63" s="60"/>
       <c r="C63" s="41"/>
@@ -4946,7 +4995,7 @@
       <c r="AA63" s="57"/>
       <c r="AB63" s="57"/>
     </row>
-    <row r="64" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:28" ht="18" customHeight="1">
       <c r="A64" s="66"/>
       <c r="B64" s="60"/>
       <c r="C64" s="41"/>
@@ -4976,7 +5025,7 @@
       <c r="AA64" s="57"/>
       <c r="AB64" s="57"/>
     </row>
-    <row r="65" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:28" ht="18" customHeight="1">
       <c r="A65" s="66"/>
       <c r="B65" s="60"/>
       <c r="C65" s="41"/>
@@ -5006,7 +5055,7 @@
       <c r="AA65" s="57"/>
       <c r="AB65" s="57"/>
     </row>
-    <row r="66" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:28" ht="18" customHeight="1">
       <c r="A66" s="66"/>
       <c r="B66" s="60"/>
       <c r="C66" s="41"/>
@@ -5036,7 +5085,7 @@
       <c r="AA66" s="57"/>
       <c r="AB66" s="57"/>
     </row>
-    <row r="67" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:28" ht="18" customHeight="1">
       <c r="A67" s="58"/>
       <c r="B67" s="60"/>
       <c r="C67" s="90"/>
@@ -5066,7 +5115,7 @@
       <c r="AA67" s="57"/>
       <c r="AB67" s="57"/>
     </row>
-    <row r="68" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:28" ht="18" customHeight="1">
       <c r="A68" s="58"/>
       <c r="B68" s="60"/>
       <c r="C68" s="90"/>
@@ -5096,7 +5145,7 @@
       <c r="AA68" s="57"/>
       <c r="AB68" s="57"/>
     </row>
-    <row r="69" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:28" ht="18" customHeight="1">
       <c r="A69" s="66"/>
       <c r="B69" s="60"/>
       <c r="C69" s="41"/>
@@ -5126,7 +5175,7 @@
       <c r="AA69" s="57"/>
       <c r="AB69" s="57"/>
     </row>
-    <row r="70" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:28" ht="18" customHeight="1">
       <c r="A70" s="66"/>
       <c r="B70" s="60"/>
       <c r="C70" s="41"/>
@@ -5156,7 +5205,7 @@
       <c r="AA70" s="57"/>
       <c r="AB70" s="57"/>
     </row>
-    <row r="71" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:28" ht="18" customHeight="1">
       <c r="A71" s="66"/>
       <c r="B71" s="60"/>
       <c r="C71" s="41"/>
@@ -5186,7 +5235,7 @@
       <c r="AA71" s="57"/>
       <c r="AB71" s="57"/>
     </row>
-    <row r="72" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:28" ht="18" customHeight="1">
       <c r="A72" s="57"/>
       <c r="B72" s="60"/>
       <c r="C72" s="41"/>
@@ -5216,7 +5265,7 @@
       <c r="AA72" s="57"/>
       <c r="AB72" s="57"/>
     </row>
-    <row r="73" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:28" ht="18" customHeight="1">
       <c r="A73" s="57"/>
       <c r="B73" s="85"/>
       <c r="C73" s="86"/>
@@ -5246,7 +5295,7 @@
       <c r="AA73" s="57"/>
       <c r="AB73" s="57"/>
     </row>
-    <row r="74" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:28" ht="18" customHeight="1">
       <c r="A74" s="58"/>
       <c r="B74" s="60"/>
       <c r="C74" s="90"/>
@@ -5276,7 +5325,7 @@
       <c r="AA74" s="57"/>
       <c r="AB74" s="57"/>
     </row>
-    <row r="75" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:28" ht="18" customHeight="1">
       <c r="A75" s="58"/>
       <c r="B75" s="93"/>
       <c r="C75" s="41"/>
@@ -5306,7 +5355,7 @@
       <c r="AA75" s="57"/>
       <c r="AB75" s="57"/>
     </row>
-    <row r="76" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:28" ht="18" customHeight="1">
       <c r="A76" s="58"/>
       <c r="B76" s="60"/>
       <c r="C76" s="90"/>
@@ -5336,7 +5385,7 @@
       <c r="AA76" s="57"/>
       <c r="AB76" s="57"/>
     </row>
-    <row r="77" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:28" ht="18" customHeight="1">
       <c r="A77" s="58"/>
       <c r="B77" s="60"/>
       <c r="C77" s="90"/>
@@ -5366,7 +5415,7 @@
       <c r="AA77" s="57"/>
       <c r="AB77" s="57"/>
     </row>
-    <row r="78" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:28" ht="18" customHeight="1">
       <c r="A78" s="57"/>
       <c r="B78" s="94"/>
       <c r="C78" s="95"/>
@@ -5396,7 +5445,7 @@
       <c r="AA78" s="57"/>
       <c r="AB78" s="57"/>
     </row>
-    <row r="79" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:28" ht="18" customHeight="1">
       <c r="A79" s="66"/>
       <c r="B79" s="93"/>
       <c r="C79" s="95"/>
@@ -5426,7 +5475,7 @@
       <c r="AA79" s="57"/>
       <c r="AB79" s="57"/>
     </row>
-    <row r="80" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:28" ht="18" customHeight="1">
       <c r="A80" s="57"/>
       <c r="B80" s="60"/>
       <c r="C80" s="90"/>
@@ -5456,7 +5505,7 @@
       <c r="AA80" s="57"/>
       <c r="AB80" s="57"/>
     </row>
-    <row r="81" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:28" ht="18" customHeight="1">
       <c r="A81" s="57"/>
       <c r="B81" s="60"/>
       <c r="C81" s="90"/>
@@ -5486,7 +5535,7 @@
       <c r="AA81" s="57"/>
       <c r="AB81" s="57"/>
     </row>
-    <row r="82" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:28" ht="18" customHeight="1">
       <c r="A82" s="57"/>
       <c r="B82" s="60"/>
       <c r="C82" s="90"/>
@@ -5516,7 +5565,7 @@
       <c r="AA82" s="57"/>
       <c r="AB82" s="57"/>
     </row>
-    <row r="83" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:28" ht="18" customHeight="1">
       <c r="A83" s="57"/>
       <c r="B83" s="60"/>
       <c r="C83" s="90"/>
@@ -5546,7 +5595,7 @@
       <c r="AA83" s="57"/>
       <c r="AB83" s="57"/>
     </row>
-    <row r="84" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:28" ht="18" customHeight="1">
       <c r="A84" s="57"/>
       <c r="B84" s="60"/>
       <c r="C84" s="90"/>
@@ -5576,7 +5625,7 @@
       <c r="AA84" s="57"/>
       <c r="AB84" s="57"/>
     </row>
-    <row r="85" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:28" ht="18" customHeight="1">
       <c r="A85" s="57"/>
       <c r="B85" s="60"/>
       <c r="C85" s="90"/>
@@ -5606,7 +5655,7 @@
       <c r="AA85" s="57"/>
       <c r="AB85" s="57"/>
     </row>
-    <row r="86" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:28" ht="18" customHeight="1">
       <c r="A86" s="57"/>
       <c r="B86" s="60"/>
       <c r="C86" s="90"/>
@@ -5636,7 +5685,7 @@
       <c r="AA86" s="57"/>
       <c r="AB86" s="57"/>
     </row>
-    <row r="87" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:28" ht="18" customHeight="1">
       <c r="A87" s="57"/>
       <c r="B87" s="60"/>
       <c r="C87" s="90"/>
@@ -5666,7 +5715,7 @@
       <c r="AA87" s="57"/>
       <c r="AB87" s="57"/>
     </row>
-    <row r="88" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:28" ht="18" customHeight="1">
       <c r="A88" s="57"/>
       <c r="B88" s="60"/>
       <c r="C88" s="90"/>
@@ -5696,7 +5745,7 @@
       <c r="AA88" s="57"/>
       <c r="AB88" s="57"/>
     </row>
-    <row r="89" spans="1:28" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:28" ht="17" customHeight="1">
       <c r="A89" s="57"/>
       <c r="B89" s="86"/>
       <c r="C89" s="86"/>
@@ -5726,7 +5775,7 @@
       <c r="AA89" s="57"/>
       <c r="AB89" s="57"/>
     </row>
-    <row r="90" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:28" ht="18" customHeight="1">
       <c r="A90" s="57"/>
       <c r="B90" s="97"/>
       <c r="C90" s="41"/>
@@ -5756,7 +5805,7 @@
       <c r="AA90" s="57"/>
       <c r="AB90" s="57"/>
     </row>
-    <row r="91" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:28" ht="18" customHeight="1">
       <c r="A91" s="66"/>
       <c r="B91" s="76"/>
       <c r="C91" s="41"/>
@@ -5786,7 +5835,7 @@
       <c r="AA91" s="57"/>
       <c r="AB91" s="57"/>
     </row>
-    <row r="92" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:28" ht="18" customHeight="1">
       <c r="A92" s="66"/>
       <c r="B92" s="60"/>
       <c r="C92" s="41"/>
@@ -5816,7 +5865,7 @@
       <c r="AA92" s="57"/>
       <c r="AB92" s="57"/>
     </row>
-    <row r="93" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:28" ht="18" customHeight="1">
       <c r="A93" s="66"/>
       <c r="B93" s="60"/>
       <c r="C93" s="41"/>
@@ -5846,7 +5895,7 @@
       <c r="AA93" s="57"/>
       <c r="AB93" s="57"/>
     </row>
-    <row r="94" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:28" ht="18" customHeight="1">
       <c r="A94" s="66"/>
       <c r="B94" s="76"/>
       <c r="C94" s="41"/>
@@ -5876,7 +5925,7 @@
       <c r="AA94" s="57"/>
       <c r="AB94" s="57"/>
     </row>
-    <row r="95" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:28" ht="18" customHeight="1">
       <c r="A95" s="66"/>
       <c r="B95" s="60"/>
       <c r="C95" s="41"/>
@@ -5906,7 +5955,7 @@
       <c r="AA95" s="57"/>
       <c r="AB95" s="57"/>
     </row>
-    <row r="96" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:28" ht="18" customHeight="1">
       <c r="A96" s="66"/>
       <c r="B96" s="60"/>
       <c r="C96" s="41"/>
@@ -5936,7 +5985,7 @@
       <c r="AA96" s="57"/>
       <c r="AB96" s="57"/>
     </row>
-    <row r="97" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:28" ht="18" customHeight="1">
       <c r="A97" s="27"/>
       <c r="B97" s="100"/>
       <c r="C97" s="86"/>
@@ -5966,7 +6015,7 @@
       <c r="AA97" s="51"/>
       <c r="AB97" s="51"/>
     </row>
-    <row r="98" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:28" ht="18" customHeight="1">
       <c r="A98" s="101"/>
       <c r="B98" s="102"/>
       <c r="C98" s="103"/>
@@ -5996,7 +6045,7 @@
       <c r="AA98" s="109"/>
       <c r="AB98" s="109"/>
     </row>
-    <row r="99" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:28" ht="18" customHeight="1">
       <c r="A99" s="65"/>
       <c r="B99" s="110"/>
       <c r="C99" s="41"/>
@@ -6026,18 +6075,18 @@
       <c r="AA99" s="22"/>
       <c r="AB99" s="22"/>
     </row>
-    <row r="100" spans="1:28" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:28" ht="13" customHeight="1">
       <c r="A100" s="57"/>
       <c r="B100" s="76"/>
-      <c r="C100" s="124"/>
-      <c r="D100" s="125"/>
-      <c r="E100" s="125"/>
-      <c r="F100" s="125"/>
-      <c r="G100" s="125"/>
-      <c r="H100" s="125"/>
-      <c r="I100" s="125"/>
-      <c r="J100" s="125"/>
-      <c r="K100" s="126"/>
+      <c r="C100" s="137"/>
+      <c r="D100" s="138"/>
+      <c r="E100" s="138"/>
+      <c r="F100" s="138"/>
+      <c r="G100" s="138"/>
+      <c r="H100" s="138"/>
+      <c r="I100" s="138"/>
+      <c r="J100" s="138"/>
+      <c r="K100" s="139"/>
       <c r="L100" s="113"/>
       <c r="M100" s="114"/>
       <c r="N100" s="115"/>
@@ -6070,6 +6119,11 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6079,33 +6133,33 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.125" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="256" width="8.125" style="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="17" customHeight="1">
       <c r="A1" s="119"/>
       <c r="B1" s="119"/>
       <c r="C1" s="119"/>
       <c r="D1" s="119"/>
       <c r="E1" s="119"/>
     </row>
-    <row r="2" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="17" customHeight="1">
       <c r="A2" s="119"/>
       <c r="B2" s="119"/>
       <c r="C2" s="119"/>
       <c r="D2" s="119"/>
       <c r="E2" s="119"/>
     </row>
-    <row r="3" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="17" customHeight="1">
       <c r="A3" s="119"/>
       <c r="B3" s="119"/>
       <c r="C3" s="119"/>
       <c r="D3" s="119"/>
       <c r="E3" s="119"/>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="17" customHeight="1">
       <c r="A4" s="120" t="s">
         <v>89</v>
       </c>
@@ -6114,42 +6168,42 @@
       <c r="D4" s="119"/>
       <c r="E4" s="119"/>
     </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="17" customHeight="1">
       <c r="A5" s="119"/>
       <c r="B5" s="119"/>
       <c r="C5" s="119"/>
       <c r="D5" s="119"/>
       <c r="E5" s="119"/>
     </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="17" customHeight="1">
       <c r="A6" s="119"/>
       <c r="B6" s="119"/>
       <c r="C6" s="119"/>
       <c r="D6" s="119"/>
       <c r="E6" s="119"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="17" customHeight="1">
       <c r="A7" s="119"/>
       <c r="B7" s="119"/>
       <c r="C7" s="119"/>
       <c r="D7" s="119"/>
       <c r="E7" s="119"/>
     </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="17" customHeight="1">
       <c r="A8" s="119"/>
       <c r="B8" s="119"/>
       <c r="C8" s="119"/>
       <c r="D8" s="119"/>
       <c r="E8" s="119"/>
     </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="17" customHeight="1">
       <c r="A9" s="119"/>
       <c r="B9" s="119"/>
       <c r="C9" s="119"/>
       <c r="D9" s="119"/>
       <c r="E9" s="119"/>
     </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="17" customHeight="1">
       <c r="A10" s="119"/>
       <c r="B10" s="119"/>
       <c r="C10" s="119"/>
@@ -6162,5 +6216,10 @@
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>